<commit_message>
Making changes to sleep
</commit_message>
<xml_diff>
--- a/datasets/TotalSleep.xlsx
+++ b/datasets/TotalSleep.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="TotalSleep" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -911,14 +911,14 @@
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="C1" sqref="C1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="3" max="4" width="13.7265625" customWidth="1"/>
     <col min="5" max="5" width="20.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
@@ -5257,5 +5257,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding updated datasheets for December 2017
</commit_message>
<xml_diff>
--- a/datasets/TotalSleep.xlsx
+++ b/datasets/TotalSleep.xlsx
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +207,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="33">
@@ -506,7 +510,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -549,6 +553,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -556,7 +561,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -594,6 +599,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -910,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4661,31 +4667,31 @@
         <v>86</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ref="J66:J76" si="14">IF(C66&gt;=420,"Yes","No")</f>
+        <f t="shared" ref="J66:J99" si="14">IF(C66&gt;=420,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="K66" s="2">
-        <f t="shared" ref="K66:K76" si="15">ROUND((C66/F66)*100, 2)</f>
+        <f t="shared" ref="K66:K99" si="15">ROUND((C66/F66)*100, 2)</f>
         <v>88.02</v>
       </c>
       <c r="L66" s="2">
-        <f t="shared" ref="L66:L76" si="16">ROUND((D66/F66)*100,2)</f>
+        <f t="shared" ref="L66:L99" si="16">ROUND((D66/F66)*100,2)</f>
         <v>11.98</v>
       </c>
       <c r="M66" s="2">
-        <f t="shared" ref="M66:M76" si="17">ROUND((H66/F66)*100,2)</f>
+        <f t="shared" ref="M66:M99" si="17">ROUND((H66/F66)*100,2)</f>
         <v>50</v>
       </c>
       <c r="N66" s="2">
-        <f t="shared" ref="N66:N76" si="18">ROUND((G66/F66)*100,2)</f>
+        <f t="shared" ref="N66:N99" si="18">ROUND((G66/F66)*100,2)</f>
         <v>18.2</v>
       </c>
       <c r="O66" s="2">
-        <f t="shared" ref="O66:O76" si="19">ROUND((I66/F66)*100,2)</f>
+        <f t="shared" ref="O66:O99" si="19">ROUND((I66/F66)*100,2)</f>
         <v>19.82</v>
       </c>
       <c r="P66" s="2">
-        <f t="shared" ref="P66:P97" si="20">100-(O66+N66+M66)</f>
+        <f t="shared" ref="P66:P99" si="20">100-(O66+N66+M66)</f>
         <v>11.980000000000004</v>
       </c>
     </row>
@@ -5257,6 +5263,1317 @@
       <c r="P76" s="2">
         <f t="shared" si="20"/>
         <v>13.439999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>43070.916666666664</v>
+      </c>
+      <c r="B77" s="1">
+        <v>43071.262499999997</v>
+      </c>
+      <c r="C77" s="3">
+        <v>447</v>
+      </c>
+      <c r="D77" s="3">
+        <v>51</v>
+      </c>
+      <c r="E77" s="3">
+        <v>39</v>
+      </c>
+      <c r="F77" s="3">
+        <v>498</v>
+      </c>
+      <c r="G77" s="3">
+        <v>85</v>
+      </c>
+      <c r="H77" s="3">
+        <v>287</v>
+      </c>
+      <c r="I77" s="3">
+        <v>75</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K77" s="2">
+        <f t="shared" si="15"/>
+        <v>89.76</v>
+      </c>
+      <c r="L77" s="2">
+        <f t="shared" si="16"/>
+        <v>10.24</v>
+      </c>
+      <c r="M77" s="2">
+        <f t="shared" si="17"/>
+        <v>57.63</v>
+      </c>
+      <c r="N77" s="2">
+        <f t="shared" si="18"/>
+        <v>17.07</v>
+      </c>
+      <c r="O77" s="2">
+        <f t="shared" si="19"/>
+        <v>15.06</v>
+      </c>
+      <c r="P77" s="2">
+        <f t="shared" si="20"/>
+        <v>10.239999999999995</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>43072.926388888889</v>
+      </c>
+      <c r="B78" s="1">
+        <v>43073.143055555556</v>
+      </c>
+      <c r="C78" s="3">
+        <v>277</v>
+      </c>
+      <c r="D78" s="3">
+        <v>34</v>
+      </c>
+      <c r="E78" s="3">
+        <v>21</v>
+      </c>
+      <c r="F78" s="3">
+        <v>311</v>
+      </c>
+      <c r="G78" s="3">
+        <v>43</v>
+      </c>
+      <c r="H78" s="3">
+        <v>175</v>
+      </c>
+      <c r="I78" s="3">
+        <v>59</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K78" s="2">
+        <f t="shared" si="15"/>
+        <v>89.07</v>
+      </c>
+      <c r="L78" s="2">
+        <f t="shared" si="16"/>
+        <v>10.93</v>
+      </c>
+      <c r="M78" s="2">
+        <f t="shared" si="17"/>
+        <v>56.27</v>
+      </c>
+      <c r="N78" s="2">
+        <f t="shared" si="18"/>
+        <v>13.83</v>
+      </c>
+      <c r="O78" s="2">
+        <f t="shared" si="19"/>
+        <v>18.97</v>
+      </c>
+      <c r="P78" s="2">
+        <f t="shared" si="20"/>
+        <v>10.930000000000007</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>43073.948611111111</v>
+      </c>
+      <c r="B79" s="1">
+        <v>43074.214583333334</v>
+      </c>
+      <c r="C79" s="3">
+        <v>335</v>
+      </c>
+      <c r="D79" s="3">
+        <v>48</v>
+      </c>
+      <c r="E79" s="3">
+        <v>30</v>
+      </c>
+      <c r="F79" s="3">
+        <v>383</v>
+      </c>
+      <c r="G79" s="3">
+        <v>61</v>
+      </c>
+      <c r="H79" s="3">
+        <v>233</v>
+      </c>
+      <c r="I79" s="3">
+        <v>41</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K79" s="2">
+        <f t="shared" si="15"/>
+        <v>87.47</v>
+      </c>
+      <c r="L79" s="2">
+        <f t="shared" si="16"/>
+        <v>12.53</v>
+      </c>
+      <c r="M79" s="2">
+        <f t="shared" si="17"/>
+        <v>60.84</v>
+      </c>
+      <c r="N79" s="2">
+        <f t="shared" si="18"/>
+        <v>15.93</v>
+      </c>
+      <c r="O79" s="2">
+        <f t="shared" si="19"/>
+        <v>10.7</v>
+      </c>
+      <c r="P79" s="2">
+        <f t="shared" si="20"/>
+        <v>12.530000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>43074.929861111108</v>
+      </c>
+      <c r="B80" s="1">
+        <v>43075.206250000003</v>
+      </c>
+      <c r="C80" s="3">
+        <v>371</v>
+      </c>
+      <c r="D80" s="3">
+        <v>27</v>
+      </c>
+      <c r="E80" s="3">
+        <v>23</v>
+      </c>
+      <c r="F80" s="3">
+        <v>398</v>
+      </c>
+      <c r="G80" s="3">
+        <v>73</v>
+      </c>
+      <c r="H80" s="3">
+        <v>191</v>
+      </c>
+      <c r="I80" s="3">
+        <v>107</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K80" s="2">
+        <f t="shared" si="15"/>
+        <v>93.22</v>
+      </c>
+      <c r="L80" s="2">
+        <f t="shared" si="16"/>
+        <v>6.78</v>
+      </c>
+      <c r="M80" s="2">
+        <f t="shared" si="17"/>
+        <v>47.99</v>
+      </c>
+      <c r="N80" s="2">
+        <f t="shared" si="18"/>
+        <v>18.34</v>
+      </c>
+      <c r="O80" s="2">
+        <f t="shared" si="19"/>
+        <v>26.88</v>
+      </c>
+      <c r="P80" s="2">
+        <f t="shared" si="20"/>
+        <v>6.789999999999992</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>43075.898611111108</v>
+      </c>
+      <c r="B81" s="1">
+        <v>43076.206944444442</v>
+      </c>
+      <c r="C81" s="3">
+        <v>393</v>
+      </c>
+      <c r="D81" s="3">
+        <v>51</v>
+      </c>
+      <c r="E81" s="3">
+        <v>27</v>
+      </c>
+      <c r="F81" s="3">
+        <v>444</v>
+      </c>
+      <c r="G81" s="3">
+        <v>52</v>
+      </c>
+      <c r="H81" s="3">
+        <v>240</v>
+      </c>
+      <c r="I81" s="3">
+        <v>101</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K81" s="2">
+        <f t="shared" si="15"/>
+        <v>88.51</v>
+      </c>
+      <c r="L81" s="2">
+        <f t="shared" si="16"/>
+        <v>11.49</v>
+      </c>
+      <c r="M81" s="2">
+        <f t="shared" si="17"/>
+        <v>54.05</v>
+      </c>
+      <c r="N81" s="2">
+        <f t="shared" si="18"/>
+        <v>11.71</v>
+      </c>
+      <c r="O81" s="2">
+        <f t="shared" si="19"/>
+        <v>22.75</v>
+      </c>
+      <c r="P81" s="2">
+        <f t="shared" si="20"/>
+        <v>11.490000000000009</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>43076.911805555559</v>
+      </c>
+      <c r="B82" s="1">
+        <v>43077.206944444442</v>
+      </c>
+      <c r="C82" s="3">
+        <v>381</v>
+      </c>
+      <c r="D82" s="3">
+        <v>43</v>
+      </c>
+      <c r="E82" s="3">
+        <v>32</v>
+      </c>
+      <c r="F82" s="3">
+        <v>424</v>
+      </c>
+      <c r="G82" s="3">
+        <v>60</v>
+      </c>
+      <c r="H82" s="3">
+        <v>232</v>
+      </c>
+      <c r="I82" s="3">
+        <v>89</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K82" s="2">
+        <f t="shared" si="15"/>
+        <v>89.86</v>
+      </c>
+      <c r="L82" s="2">
+        <f t="shared" si="16"/>
+        <v>10.14</v>
+      </c>
+      <c r="M82" s="2">
+        <f t="shared" si="17"/>
+        <v>54.72</v>
+      </c>
+      <c r="N82" s="2">
+        <f t="shared" si="18"/>
+        <v>14.15</v>
+      </c>
+      <c r="O82" s="2">
+        <f t="shared" si="19"/>
+        <v>20.99</v>
+      </c>
+      <c r="P82" s="2">
+        <f t="shared" si="20"/>
+        <v>10.14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>43077.941666666666</v>
+      </c>
+      <c r="B83" s="1">
+        <v>43078.211805555555</v>
+      </c>
+      <c r="C83" s="3">
+        <v>354</v>
+      </c>
+      <c r="D83" s="3">
+        <v>35</v>
+      </c>
+      <c r="E83" s="3">
+        <v>29</v>
+      </c>
+      <c r="F83" s="3">
+        <v>389</v>
+      </c>
+      <c r="G83" s="3">
+        <v>105</v>
+      </c>
+      <c r="H83" s="3">
+        <v>158</v>
+      </c>
+      <c r="I83" s="3">
+        <v>91</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K83" s="2">
+        <f t="shared" si="15"/>
+        <v>91</v>
+      </c>
+      <c r="L83" s="2">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="M83" s="2">
+        <f t="shared" si="17"/>
+        <v>40.619999999999997</v>
+      </c>
+      <c r="N83" s="2">
+        <f t="shared" si="18"/>
+        <v>26.99</v>
+      </c>
+      <c r="O83" s="2">
+        <f t="shared" si="19"/>
+        <v>23.39</v>
+      </c>
+      <c r="P83" s="2">
+        <f t="shared" si="20"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>43079.943749999999</v>
+      </c>
+      <c r="B84" s="1">
+        <v>43080.10833333333</v>
+      </c>
+      <c r="C84" s="3">
+        <v>220</v>
+      </c>
+      <c r="D84" s="3">
+        <v>17</v>
+      </c>
+      <c r="E84" s="3">
+        <v>13</v>
+      </c>
+      <c r="F84" s="3">
+        <v>237</v>
+      </c>
+      <c r="G84" s="3">
+        <v>31</v>
+      </c>
+      <c r="H84" s="3">
+        <v>156</v>
+      </c>
+      <c r="I84" s="3">
+        <v>33</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K84" s="2">
+        <f t="shared" si="15"/>
+        <v>92.83</v>
+      </c>
+      <c r="L84" s="2">
+        <f t="shared" si="16"/>
+        <v>7.17</v>
+      </c>
+      <c r="M84" s="2">
+        <f t="shared" si="17"/>
+        <v>65.819999999999993</v>
+      </c>
+      <c r="N84" s="2">
+        <f t="shared" si="18"/>
+        <v>13.08</v>
+      </c>
+      <c r="O84" s="2">
+        <f t="shared" si="19"/>
+        <v>13.92</v>
+      </c>
+      <c r="P84" s="2">
+        <f t="shared" si="20"/>
+        <v>7.1800000000000068</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>43080.9375</v>
+      </c>
+      <c r="B85" s="1">
+        <v>43081.207638888889</v>
+      </c>
+      <c r="C85" s="3">
+        <v>344</v>
+      </c>
+      <c r="D85" s="3">
+        <v>44</v>
+      </c>
+      <c r="E85" s="3">
+        <v>31</v>
+      </c>
+      <c r="F85" s="3">
+        <v>388</v>
+      </c>
+      <c r="G85" s="3">
+        <v>48</v>
+      </c>
+      <c r="H85" s="3">
+        <v>205</v>
+      </c>
+      <c r="I85" s="3">
+        <v>91</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K85" s="2">
+        <f t="shared" si="15"/>
+        <v>88.66</v>
+      </c>
+      <c r="L85" s="2">
+        <f t="shared" si="16"/>
+        <v>11.34</v>
+      </c>
+      <c r="M85" s="2">
+        <f t="shared" si="17"/>
+        <v>52.84</v>
+      </c>
+      <c r="N85" s="2">
+        <f t="shared" si="18"/>
+        <v>12.37</v>
+      </c>
+      <c r="O85" s="2">
+        <f t="shared" si="19"/>
+        <v>23.45</v>
+      </c>
+      <c r="P85" s="2">
+        <f t="shared" si="20"/>
+        <v>11.340000000000003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>43087.9375</v>
+      </c>
+      <c r="B86" s="1">
+        <v>43088.209722222222</v>
+      </c>
+      <c r="C86" s="3">
+        <v>348</v>
+      </c>
+      <c r="D86" s="3">
+        <v>43</v>
+      </c>
+      <c r="E86" s="3">
+        <v>31</v>
+      </c>
+      <c r="F86" s="3">
+        <v>391</v>
+      </c>
+      <c r="G86" s="3">
+        <v>66</v>
+      </c>
+      <c r="H86" s="3">
+        <v>189</v>
+      </c>
+      <c r="I86" s="3">
+        <v>93</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K86" s="2">
+        <f t="shared" si="15"/>
+        <v>89</v>
+      </c>
+      <c r="L86" s="2">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="M86" s="2">
+        <f t="shared" si="17"/>
+        <v>48.34</v>
+      </c>
+      <c r="N86" s="2">
+        <f t="shared" si="18"/>
+        <v>16.88</v>
+      </c>
+      <c r="O86" s="2">
+        <f t="shared" si="19"/>
+        <v>23.79</v>
+      </c>
+      <c r="P86" s="2">
+        <f t="shared" si="20"/>
+        <v>10.989999999999995</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>43088.890972222223</v>
+      </c>
+      <c r="B87" s="1">
+        <v>43089.184027777781</v>
+      </c>
+      <c r="C87" s="3">
+        <v>379</v>
+      </c>
+      <c r="D87" s="3">
+        <v>43</v>
+      </c>
+      <c r="E87" s="3">
+        <v>32</v>
+      </c>
+      <c r="F87" s="3">
+        <v>422</v>
+      </c>
+      <c r="G87" s="3">
+        <v>72</v>
+      </c>
+      <c r="H87" s="3">
+        <v>208</v>
+      </c>
+      <c r="I87" s="3">
+        <v>99</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K87" s="2">
+        <f t="shared" si="15"/>
+        <v>89.81</v>
+      </c>
+      <c r="L87" s="2">
+        <f t="shared" si="16"/>
+        <v>10.19</v>
+      </c>
+      <c r="M87" s="2">
+        <f t="shared" si="17"/>
+        <v>49.29</v>
+      </c>
+      <c r="N87" s="2">
+        <f t="shared" si="18"/>
+        <v>17.059999999999999</v>
+      </c>
+      <c r="O87" s="2">
+        <f t="shared" si="19"/>
+        <v>23.46</v>
+      </c>
+      <c r="P87" s="2">
+        <f t="shared" si="20"/>
+        <v>10.189999999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>43089.907638888886</v>
+      </c>
+      <c r="B88" s="1">
+        <v>43090.209027777775</v>
+      </c>
+      <c r="C88" s="3">
+        <v>372</v>
+      </c>
+      <c r="D88" s="3">
+        <v>62</v>
+      </c>
+      <c r="E88" s="3">
+        <v>30</v>
+      </c>
+      <c r="F88" s="3">
+        <v>434</v>
+      </c>
+      <c r="G88" s="3">
+        <v>65</v>
+      </c>
+      <c r="H88" s="3">
+        <v>196</v>
+      </c>
+      <c r="I88" s="3">
+        <v>111</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K88" s="2">
+        <f t="shared" si="15"/>
+        <v>85.71</v>
+      </c>
+      <c r="L88" s="2">
+        <f t="shared" si="16"/>
+        <v>14.29</v>
+      </c>
+      <c r="M88" s="2">
+        <f t="shared" si="17"/>
+        <v>45.16</v>
+      </c>
+      <c r="N88" s="2">
+        <f t="shared" si="18"/>
+        <v>14.98</v>
+      </c>
+      <c r="O88" s="2">
+        <f t="shared" si="19"/>
+        <v>25.58</v>
+      </c>
+      <c r="P88" s="2">
+        <f t="shared" si="20"/>
+        <v>14.280000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>43090.913888888892</v>
+      </c>
+      <c r="B89" s="1">
+        <v>43091.214583333334</v>
+      </c>
+      <c r="C89" s="3">
+        <v>382</v>
+      </c>
+      <c r="D89" s="3">
+        <v>51</v>
+      </c>
+      <c r="E89" s="3">
+        <v>28</v>
+      </c>
+      <c r="F89" s="3">
+        <v>433</v>
+      </c>
+      <c r="G89" s="3">
+        <v>58</v>
+      </c>
+      <c r="H89" s="3">
+        <v>209</v>
+      </c>
+      <c r="I89" s="3">
+        <v>115</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K89" s="2">
+        <f t="shared" si="15"/>
+        <v>88.22</v>
+      </c>
+      <c r="L89" s="2">
+        <f t="shared" si="16"/>
+        <v>11.78</v>
+      </c>
+      <c r="M89" s="2">
+        <f t="shared" si="17"/>
+        <v>48.27</v>
+      </c>
+      <c r="N89" s="2">
+        <f t="shared" si="18"/>
+        <v>13.39</v>
+      </c>
+      <c r="O89" s="2">
+        <f t="shared" si="19"/>
+        <v>26.56</v>
+      </c>
+      <c r="P89" s="2">
+        <f t="shared" si="20"/>
+        <v>11.780000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>43091.904861111114</v>
+      </c>
+      <c r="B90" s="1">
+        <v>43092.178472222222</v>
+      </c>
+      <c r="C90" s="3">
+        <v>348</v>
+      </c>
+      <c r="D90" s="3">
+        <v>46</v>
+      </c>
+      <c r="E90" s="3">
+        <v>25</v>
+      </c>
+      <c r="F90" s="3">
+        <v>394</v>
+      </c>
+      <c r="G90" s="3">
+        <v>55</v>
+      </c>
+      <c r="H90" s="3">
+        <v>188</v>
+      </c>
+      <c r="I90" s="3">
+        <v>105</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K90" s="2">
+        <f t="shared" si="15"/>
+        <v>88.32</v>
+      </c>
+      <c r="L90" s="2">
+        <f t="shared" si="16"/>
+        <v>11.68</v>
+      </c>
+      <c r="M90" s="2">
+        <f t="shared" si="17"/>
+        <v>47.72</v>
+      </c>
+      <c r="N90" s="2">
+        <f t="shared" si="18"/>
+        <v>13.96</v>
+      </c>
+      <c r="O90" s="2">
+        <f t="shared" si="19"/>
+        <v>26.65</v>
+      </c>
+      <c r="P90" s="2">
+        <f t="shared" si="20"/>
+        <v>11.670000000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>43092.886805555558</v>
+      </c>
+      <c r="B91" s="1">
+        <v>43093.189583333333</v>
+      </c>
+      <c r="C91" s="3">
+        <v>394</v>
+      </c>
+      <c r="D91" s="3">
+        <v>42</v>
+      </c>
+      <c r="E91" s="3">
+        <v>29</v>
+      </c>
+      <c r="F91" s="3">
+        <v>436</v>
+      </c>
+      <c r="G91" s="3">
+        <v>78</v>
+      </c>
+      <c r="H91" s="3">
+        <v>219</v>
+      </c>
+      <c r="I91" s="3">
+        <v>97</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K91" s="2">
+        <f t="shared" si="15"/>
+        <v>90.37</v>
+      </c>
+      <c r="L91" s="2">
+        <f t="shared" si="16"/>
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="M91" s="2">
+        <f t="shared" si="17"/>
+        <v>50.23</v>
+      </c>
+      <c r="N91" s="2">
+        <f t="shared" si="18"/>
+        <v>17.89</v>
+      </c>
+      <c r="O91" s="2">
+        <f t="shared" si="19"/>
+        <v>22.25</v>
+      </c>
+      <c r="P91" s="2">
+        <f t="shared" si="20"/>
+        <v>9.6299999999999955</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>43093.930555555555</v>
+      </c>
+      <c r="B92" s="1">
+        <v>43094.197916666664</v>
+      </c>
+      <c r="C92" s="3">
+        <v>351</v>
+      </c>
+      <c r="D92" s="3">
+        <v>34</v>
+      </c>
+      <c r="E92" s="3">
+        <v>29</v>
+      </c>
+      <c r="F92" s="3">
+        <v>385</v>
+      </c>
+      <c r="G92" s="3">
+        <v>67</v>
+      </c>
+      <c r="H92" s="3">
+        <v>191</v>
+      </c>
+      <c r="I92" s="3">
+        <v>93</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K92" s="2">
+        <f t="shared" si="15"/>
+        <v>91.17</v>
+      </c>
+      <c r="L92" s="2">
+        <f t="shared" si="16"/>
+        <v>8.83</v>
+      </c>
+      <c r="M92" s="2">
+        <f t="shared" si="17"/>
+        <v>49.61</v>
+      </c>
+      <c r="N92" s="2">
+        <f t="shared" si="18"/>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="O92" s="2">
+        <f t="shared" si="19"/>
+        <v>24.16</v>
+      </c>
+      <c r="P92" s="2">
+        <f t="shared" si="20"/>
+        <v>8.8299999999999983</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A93" s="1">
+        <v>43094.943055555559</v>
+      </c>
+      <c r="B93" s="1">
+        <v>43095.203472222223</v>
+      </c>
+      <c r="C93" s="3">
+        <v>333</v>
+      </c>
+      <c r="D93" s="3">
+        <v>42</v>
+      </c>
+      <c r="E93" s="3">
+        <v>28</v>
+      </c>
+      <c r="F93" s="3">
+        <v>375</v>
+      </c>
+      <c r="G93" s="3">
+        <v>75</v>
+      </c>
+      <c r="H93" s="3">
+        <v>187</v>
+      </c>
+      <c r="I93" s="3">
+        <v>71</v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K93" s="2">
+        <f t="shared" si="15"/>
+        <v>88.8</v>
+      </c>
+      <c r="L93" s="2">
+        <f t="shared" si="16"/>
+        <v>11.2</v>
+      </c>
+      <c r="M93" s="2">
+        <f t="shared" si="17"/>
+        <v>49.87</v>
+      </c>
+      <c r="N93" s="2">
+        <f t="shared" si="18"/>
+        <v>20</v>
+      </c>
+      <c r="O93" s="2">
+        <f t="shared" si="19"/>
+        <v>18.93</v>
+      </c>
+      <c r="P93" s="2">
+        <f t="shared" si="20"/>
+        <v>11.200000000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A94" s="1">
+        <v>43095.911805555559</v>
+      </c>
+      <c r="B94" s="1">
+        <v>43096.2</v>
+      </c>
+      <c r="C94" s="3">
+        <v>370</v>
+      </c>
+      <c r="D94" s="3">
+        <v>45</v>
+      </c>
+      <c r="E94" s="3">
+        <v>35</v>
+      </c>
+      <c r="F94" s="3">
+        <v>415</v>
+      </c>
+      <c r="G94" s="3">
+        <v>76</v>
+      </c>
+      <c r="H94" s="3">
+        <v>191</v>
+      </c>
+      <c r="I94" s="3">
+        <v>103</v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K94" s="2">
+        <f t="shared" si="15"/>
+        <v>89.16</v>
+      </c>
+      <c r="L94" s="2">
+        <f t="shared" si="16"/>
+        <v>10.84</v>
+      </c>
+      <c r="M94" s="2">
+        <f t="shared" si="17"/>
+        <v>46.02</v>
+      </c>
+      <c r="N94" s="2">
+        <f t="shared" si="18"/>
+        <v>18.309999999999999</v>
+      </c>
+      <c r="O94" s="2">
+        <f t="shared" si="19"/>
+        <v>24.82</v>
+      </c>
+      <c r="P94" s="2">
+        <f t="shared" si="20"/>
+        <v>10.849999999999994</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A95" s="1">
+        <v>43096.897222222222</v>
+      </c>
+      <c r="B95" s="1">
+        <v>43097.206944444442</v>
+      </c>
+      <c r="C95" s="3">
+        <v>392</v>
+      </c>
+      <c r="D95" s="3">
+        <v>54</v>
+      </c>
+      <c r="E95" s="3">
+        <v>34</v>
+      </c>
+      <c r="F95" s="3">
+        <v>446</v>
+      </c>
+      <c r="G95" s="3">
+        <v>66</v>
+      </c>
+      <c r="H95" s="3">
+        <v>259</v>
+      </c>
+      <c r="I95" s="3">
+        <v>67</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K95" s="2">
+        <f t="shared" si="15"/>
+        <v>87.89</v>
+      </c>
+      <c r="L95" s="2">
+        <f t="shared" si="16"/>
+        <v>12.11</v>
+      </c>
+      <c r="M95" s="2">
+        <f t="shared" si="17"/>
+        <v>58.07</v>
+      </c>
+      <c r="N95" s="2">
+        <f t="shared" si="18"/>
+        <v>14.8</v>
+      </c>
+      <c r="O95" s="2">
+        <f t="shared" si="19"/>
+        <v>15.02</v>
+      </c>
+      <c r="P95" s="2">
+        <f t="shared" si="20"/>
+        <v>12.11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A96" s="1">
+        <v>43097.911805555559</v>
+      </c>
+      <c r="B96" s="1">
+        <v>43098.211805555555</v>
+      </c>
+      <c r="C96" s="3">
+        <v>388</v>
+      </c>
+      <c r="D96" s="3">
+        <v>44</v>
+      </c>
+      <c r="E96" s="3">
+        <v>31</v>
+      </c>
+      <c r="F96" s="3">
+        <v>432</v>
+      </c>
+      <c r="G96" s="3">
+        <v>78</v>
+      </c>
+      <c r="H96" s="3">
+        <v>225</v>
+      </c>
+      <c r="I96" s="3">
+        <v>85</v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K96" s="2">
+        <f t="shared" si="15"/>
+        <v>89.81</v>
+      </c>
+      <c r="L96" s="2">
+        <f t="shared" si="16"/>
+        <v>10.19</v>
+      </c>
+      <c r="M96" s="2">
+        <f t="shared" si="17"/>
+        <v>52.08</v>
+      </c>
+      <c r="N96" s="2">
+        <f t="shared" si="18"/>
+        <v>18.059999999999999</v>
+      </c>
+      <c r="O96" s="2">
+        <f t="shared" si="19"/>
+        <v>19.68</v>
+      </c>
+      <c r="P96" s="2">
+        <f t="shared" si="20"/>
+        <v>10.180000000000007</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A97" s="1">
+        <v>43098.905555555553</v>
+      </c>
+      <c r="B97" s="1">
+        <v>43099.195138888892</v>
+      </c>
+      <c r="C97" s="3">
+        <v>377</v>
+      </c>
+      <c r="D97" s="3">
+        <v>40</v>
+      </c>
+      <c r="E97" s="3">
+        <v>33</v>
+      </c>
+      <c r="F97" s="3">
+        <v>417</v>
+      </c>
+      <c r="G97" s="3">
+        <v>58</v>
+      </c>
+      <c r="H97" s="3">
+        <v>243</v>
+      </c>
+      <c r="I97" s="3">
+        <v>76</v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K97" s="2">
+        <f t="shared" si="15"/>
+        <v>90.41</v>
+      </c>
+      <c r="L97" s="2">
+        <f t="shared" si="16"/>
+        <v>9.59</v>
+      </c>
+      <c r="M97" s="2">
+        <f t="shared" si="17"/>
+        <v>58.27</v>
+      </c>
+      <c r="N97" s="2">
+        <f t="shared" si="18"/>
+        <v>13.91</v>
+      </c>
+      <c r="O97" s="2">
+        <f t="shared" si="19"/>
+        <v>18.23</v>
+      </c>
+      <c r="P97" s="2">
+        <f t="shared" si="20"/>
+        <v>9.5900000000000034</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A98" s="1">
+        <v>43069.927777777775</v>
+      </c>
+      <c r="B98" s="1">
+        <v>43070.243750000001</v>
+      </c>
+      <c r="C98" s="3">
+        <v>385</v>
+      </c>
+      <c r="D98" s="3">
+        <v>70</v>
+      </c>
+      <c r="E98" s="3">
+        <v>33</v>
+      </c>
+      <c r="F98" s="3">
+        <v>455</v>
+      </c>
+      <c r="G98" s="3">
+        <v>61</v>
+      </c>
+      <c r="H98" s="3">
+        <v>240</v>
+      </c>
+      <c r="I98" s="3">
+        <v>84</v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K98" s="2">
+        <f t="shared" si="15"/>
+        <v>84.62</v>
+      </c>
+      <c r="L98" s="2">
+        <f t="shared" si="16"/>
+        <v>15.38</v>
+      </c>
+      <c r="M98" s="2">
+        <f t="shared" si="17"/>
+        <v>52.75</v>
+      </c>
+      <c r="N98" s="2">
+        <f t="shared" si="18"/>
+        <v>13.41</v>
+      </c>
+      <c r="O98" s="2">
+        <f t="shared" si="19"/>
+        <v>18.46</v>
+      </c>
+      <c r="P98" s="2">
+        <f t="shared" si="20"/>
+        <v>15.379999999999995</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A99" s="1">
+        <v>43099.890972222223</v>
+      </c>
+      <c r="B99" s="1">
+        <v>43100.228472222225</v>
+      </c>
+      <c r="C99" s="3">
+        <v>425</v>
+      </c>
+      <c r="D99" s="3">
+        <v>61</v>
+      </c>
+      <c r="E99" s="3">
+        <v>41</v>
+      </c>
+      <c r="F99" s="3">
+        <v>486</v>
+      </c>
+      <c r="G99" s="3">
+        <v>72</v>
+      </c>
+      <c r="H99" s="3">
+        <v>290</v>
+      </c>
+      <c r="I99" s="3">
+        <v>63</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K99" s="2">
+        <f t="shared" si="15"/>
+        <v>87.45</v>
+      </c>
+      <c r="L99" s="2">
+        <f t="shared" si="16"/>
+        <v>12.55</v>
+      </c>
+      <c r="M99" s="2">
+        <f t="shared" si="17"/>
+        <v>59.67</v>
+      </c>
+      <c r="N99" s="2">
+        <f t="shared" si="18"/>
+        <v>14.81</v>
+      </c>
+      <c r="O99" s="2">
+        <f t="shared" si="19"/>
+        <v>12.96</v>
+      </c>
+      <c r="P99" s="2">
+        <f t="shared" si="20"/>
+        <v>12.560000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Jan 2018 TotalSleep Numbers
</commit_message>
<xml_diff>
--- a/datasets/TotalSleep.xlsx
+++ b/datasets/TotalSleep.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Start Time</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>% Unclassified</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -916,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P99"/>
+  <dimension ref="A1:P129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P99" sqref="P99:P129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4667,31 +4670,31 @@
         <v>86</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ref="J66:J99" si="14">IF(C66&gt;=420,"Yes","No")</f>
+        <f t="shared" ref="J66:J129" si="14">IF(C66&gt;=420,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="K66" s="2">
-        <f t="shared" ref="K66:K99" si="15">ROUND((C66/F66)*100, 2)</f>
+        <f t="shared" ref="K66:K129" si="15">ROUND((C66/F66)*100, 2)</f>
         <v>88.02</v>
       </c>
       <c r="L66" s="2">
-        <f t="shared" ref="L66:L99" si="16">ROUND((D66/F66)*100,2)</f>
+        <f t="shared" ref="L66:L129" si="16">ROUND((D66/F66)*100,2)</f>
         <v>11.98</v>
       </c>
       <c r="M66" s="2">
-        <f t="shared" ref="M66:M99" si="17">ROUND((H66/F66)*100,2)</f>
+        <f t="shared" ref="M66:M129" si="17">ROUND((H66/F66)*100,2)</f>
         <v>50</v>
       </c>
       <c r="N66" s="2">
-        <f t="shared" ref="N66:N99" si="18">ROUND((G66/F66)*100,2)</f>
+        <f t="shared" ref="N66:N129" si="18">ROUND((G66/F66)*100,2)</f>
         <v>18.2</v>
       </c>
       <c r="O66" s="2">
-        <f t="shared" ref="O66:O99" si="19">ROUND((I66/F66)*100,2)</f>
+        <f t="shared" ref="O66:O129" si="19">ROUND((I66/F66)*100,2)</f>
         <v>19.82</v>
       </c>
       <c r="P66" s="2">
-        <f t="shared" ref="P66:P99" si="20">100-(O66+N66+M66)</f>
+        <f t="shared" ref="P66:P129" si="20">100-(O66+N66+M66)</f>
         <v>11.980000000000004</v>
       </c>
     </row>
@@ -6576,10 +6579,1717 @@
         <v>12.560000000000002</v>
       </c>
     </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A100" s="1">
+        <v>43100.888888888891</v>
+      </c>
+      <c r="B100" s="1">
+        <v>43101.198611111111</v>
+      </c>
+      <c r="C100" s="3">
+        <v>395</v>
+      </c>
+      <c r="D100" s="3">
+        <v>51</v>
+      </c>
+      <c r="E100" s="3">
+        <v>40</v>
+      </c>
+      <c r="F100" s="3">
+        <v>446</v>
+      </c>
+      <c r="G100" s="3">
+        <v>61</v>
+      </c>
+      <c r="H100" s="3">
+        <v>244</v>
+      </c>
+      <c r="I100" s="3">
+        <v>90</v>
+      </c>
+      <c r="J100" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K100" s="2">
+        <f t="shared" si="15"/>
+        <v>88.57</v>
+      </c>
+      <c r="L100" s="2">
+        <f t="shared" si="16"/>
+        <v>11.43</v>
+      </c>
+      <c r="M100" s="2">
+        <f t="shared" si="17"/>
+        <v>54.71</v>
+      </c>
+      <c r="N100" s="2">
+        <f t="shared" si="18"/>
+        <v>13.68</v>
+      </c>
+      <c r="O100" s="2">
+        <f t="shared" si="19"/>
+        <v>20.18</v>
+      </c>
+      <c r="P100" s="2">
+        <f t="shared" si="20"/>
+        <v>11.430000000000007</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A101" s="1">
+        <v>43101.849305555559</v>
+      </c>
+      <c r="B101" s="1">
+        <v>43102.069444444445</v>
+      </c>
+      <c r="C101" s="3">
+        <v>266</v>
+      </c>
+      <c r="D101" s="3">
+        <v>50</v>
+      </c>
+      <c r="E101" s="3">
+        <v>22</v>
+      </c>
+      <c r="F101" s="3">
+        <v>316</v>
+      </c>
+      <c r="G101" s="3">
+        <v>26</v>
+      </c>
+      <c r="H101" s="3">
+        <v>187</v>
+      </c>
+      <c r="I101" s="3">
+        <v>53</v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K101" s="2">
+        <f t="shared" si="15"/>
+        <v>84.18</v>
+      </c>
+      <c r="L101" s="2">
+        <f t="shared" si="16"/>
+        <v>15.82</v>
+      </c>
+      <c r="M101" s="2">
+        <f t="shared" si="17"/>
+        <v>59.18</v>
+      </c>
+      <c r="N101" s="2">
+        <f t="shared" si="18"/>
+        <v>8.23</v>
+      </c>
+      <c r="O101" s="2">
+        <f t="shared" si="19"/>
+        <v>16.77</v>
+      </c>
+      <c r="P101" s="2">
+        <f t="shared" si="20"/>
+        <v>15.819999999999993</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A102" s="1">
+        <v>43102.88958333333</v>
+      </c>
+      <c r="B102" s="1">
+        <v>43103.246527777781</v>
+      </c>
+      <c r="C102" s="3">
+        <v>425</v>
+      </c>
+      <c r="D102" s="3">
+        <v>89</v>
+      </c>
+      <c r="E102" s="3">
+        <v>36</v>
+      </c>
+      <c r="F102" s="3">
+        <v>514</v>
+      </c>
+      <c r="G102" s="3">
+        <v>64</v>
+      </c>
+      <c r="H102" s="3">
+        <v>318</v>
+      </c>
+      <c r="I102" s="3">
+        <v>43</v>
+      </c>
+      <c r="J102" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K102" s="2">
+        <f t="shared" si="15"/>
+        <v>82.68</v>
+      </c>
+      <c r="L102" s="2">
+        <f t="shared" si="16"/>
+        <v>17.32</v>
+      </c>
+      <c r="M102" s="2">
+        <f t="shared" si="17"/>
+        <v>61.87</v>
+      </c>
+      <c r="N102" s="2">
+        <f t="shared" si="18"/>
+        <v>12.45</v>
+      </c>
+      <c r="O102" s="2">
+        <f t="shared" si="19"/>
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="P102" s="2">
+        <f t="shared" si="20"/>
+        <v>17.310000000000002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A103" s="1">
+        <v>43103.861805555556</v>
+      </c>
+      <c r="B103" s="1">
+        <v>43104.232638888891</v>
+      </c>
+      <c r="C103" s="3">
+        <v>471</v>
+      </c>
+      <c r="D103" s="3">
+        <v>63</v>
+      </c>
+      <c r="E103" s="3">
+        <v>40</v>
+      </c>
+      <c r="F103" s="3">
+        <v>534</v>
+      </c>
+      <c r="G103" s="3">
+        <v>93</v>
+      </c>
+      <c r="H103" s="3">
+        <v>270</v>
+      </c>
+      <c r="I103" s="3">
+        <v>108</v>
+      </c>
+      <c r="J103" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K103" s="2">
+        <f t="shared" si="15"/>
+        <v>88.2</v>
+      </c>
+      <c r="L103" s="2">
+        <f t="shared" si="16"/>
+        <v>11.8</v>
+      </c>
+      <c r="M103" s="2">
+        <f t="shared" si="17"/>
+        <v>50.56</v>
+      </c>
+      <c r="N103" s="2">
+        <f t="shared" si="18"/>
+        <v>17.420000000000002</v>
+      </c>
+      <c r="O103" s="2">
+        <f t="shared" si="19"/>
+        <v>20.22</v>
+      </c>
+      <c r="P103" s="2">
+        <f t="shared" si="20"/>
+        <v>11.799999999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A104" s="1">
+        <v>43104.89166666667</v>
+      </c>
+      <c r="B104" s="1">
+        <v>43105.102777777778</v>
+      </c>
+      <c r="C104" s="3">
+        <v>273</v>
+      </c>
+      <c r="D104" s="3">
+        <v>31</v>
+      </c>
+      <c r="E104" s="3">
+        <v>19</v>
+      </c>
+      <c r="F104" s="3">
+        <v>304</v>
+      </c>
+      <c r="G104" s="3">
+        <v>64</v>
+      </c>
+      <c r="H104" s="3">
+        <v>166</v>
+      </c>
+      <c r="I104" s="3">
+        <v>43</v>
+      </c>
+      <c r="J104" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K104" s="2">
+        <f t="shared" si="15"/>
+        <v>89.8</v>
+      </c>
+      <c r="L104" s="2">
+        <f t="shared" si="16"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M104" s="2">
+        <f t="shared" si="17"/>
+        <v>54.61</v>
+      </c>
+      <c r="N104" s="2">
+        <f t="shared" si="18"/>
+        <v>21.05</v>
+      </c>
+      <c r="O104" s="2">
+        <f t="shared" si="19"/>
+        <v>14.14</v>
+      </c>
+      <c r="P104" s="2">
+        <f t="shared" si="20"/>
+        <v>10.200000000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A105" s="1">
+        <v>43105.159722222219</v>
+      </c>
+      <c r="B105" s="1">
+        <v>43105.290972222225</v>
+      </c>
+      <c r="C105" s="3">
+        <v>163</v>
+      </c>
+      <c r="D105" s="3">
+        <v>26</v>
+      </c>
+      <c r="E105" s="3">
+        <v>17</v>
+      </c>
+      <c r="F105" s="3">
+        <v>189</v>
+      </c>
+      <c r="G105" s="3">
+        <v>18</v>
+      </c>
+      <c r="H105" s="3">
+        <v>105</v>
+      </c>
+      <c r="I105" s="3">
+        <v>40</v>
+      </c>
+      <c r="J105" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K105" s="2">
+        <f t="shared" si="15"/>
+        <v>86.24</v>
+      </c>
+      <c r="L105" s="2">
+        <f t="shared" si="16"/>
+        <v>13.76</v>
+      </c>
+      <c r="M105" s="2">
+        <f t="shared" si="17"/>
+        <v>55.56</v>
+      </c>
+      <c r="N105" s="2">
+        <f t="shared" si="18"/>
+        <v>9.52</v>
+      </c>
+      <c r="O105" s="2">
+        <f t="shared" si="19"/>
+        <v>21.16</v>
+      </c>
+      <c r="P105" s="2">
+        <f t="shared" si="20"/>
+        <v>13.759999999999991</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A106" s="1">
+        <v>43105.990972222222</v>
+      </c>
+      <c r="B106" s="1">
+        <v>43106.248611111114</v>
+      </c>
+      <c r="C106" s="3">
+        <v>335</v>
+      </c>
+      <c r="D106" s="3">
+        <v>36</v>
+      </c>
+      <c r="E106" s="3">
+        <v>31</v>
+      </c>
+      <c r="F106" s="3">
+        <v>371</v>
+      </c>
+      <c r="G106" s="3">
+        <v>55</v>
+      </c>
+      <c r="H106" s="3">
+        <v>191</v>
+      </c>
+      <c r="I106" s="3">
+        <v>89</v>
+      </c>
+      <c r="J106" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K106" s="2">
+        <f t="shared" si="15"/>
+        <v>90.3</v>
+      </c>
+      <c r="L106" s="2">
+        <f t="shared" si="16"/>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="M106" s="2">
+        <f t="shared" si="17"/>
+        <v>51.48</v>
+      </c>
+      <c r="N106" s="2">
+        <f t="shared" si="18"/>
+        <v>14.82</v>
+      </c>
+      <c r="O106" s="2">
+        <f t="shared" si="19"/>
+        <v>23.99</v>
+      </c>
+      <c r="P106" s="2">
+        <f t="shared" si="20"/>
+        <v>9.710000000000008</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A107" s="1">
+        <v>43106.89166666667</v>
+      </c>
+      <c r="B107" s="1">
+        <v>43107.254166666666</v>
+      </c>
+      <c r="C107" s="3">
+        <v>450</v>
+      </c>
+      <c r="D107" s="3">
+        <v>72</v>
+      </c>
+      <c r="E107" s="3">
+        <v>38</v>
+      </c>
+      <c r="F107" s="3">
+        <v>522</v>
+      </c>
+      <c r="G107" s="3">
+        <v>79</v>
+      </c>
+      <c r="H107" s="3">
+        <v>279</v>
+      </c>
+      <c r="I107" s="3">
+        <v>92</v>
+      </c>
+      <c r="J107" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K107" s="2">
+        <f t="shared" si="15"/>
+        <v>86.21</v>
+      </c>
+      <c r="L107" s="2">
+        <f t="shared" si="16"/>
+        <v>13.79</v>
+      </c>
+      <c r="M107" s="2">
+        <f t="shared" si="17"/>
+        <v>53.45</v>
+      </c>
+      <c r="N107" s="2">
+        <f t="shared" si="18"/>
+        <v>15.13</v>
+      </c>
+      <c r="O107" s="2">
+        <f t="shared" si="19"/>
+        <v>17.62</v>
+      </c>
+      <c r="P107" s="2">
+        <f t="shared" si="20"/>
+        <v>13.799999999999997</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A108" s="1">
+        <v>43107.927777777775</v>
+      </c>
+      <c r="B108" s="1">
+        <v>43108.17083333333</v>
+      </c>
+      <c r="C108" s="3">
+        <v>300</v>
+      </c>
+      <c r="D108" s="3">
+        <v>50</v>
+      </c>
+      <c r="E108" s="3">
+        <v>19</v>
+      </c>
+      <c r="F108" s="3">
+        <v>350</v>
+      </c>
+      <c r="G108" s="3">
+        <v>41</v>
+      </c>
+      <c r="H108" s="3">
+        <v>189</v>
+      </c>
+      <c r="I108" s="3">
+        <v>70</v>
+      </c>
+      <c r="J108" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K108" s="2">
+        <f t="shared" si="15"/>
+        <v>85.71</v>
+      </c>
+      <c r="L108" s="2">
+        <f t="shared" si="16"/>
+        <v>14.29</v>
+      </c>
+      <c r="M108" s="2">
+        <f t="shared" si="17"/>
+        <v>54</v>
+      </c>
+      <c r="N108" s="2">
+        <f t="shared" si="18"/>
+        <v>11.71</v>
+      </c>
+      <c r="O108" s="2">
+        <f t="shared" si="19"/>
+        <v>20</v>
+      </c>
+      <c r="P108" s="2">
+        <f t="shared" si="20"/>
+        <v>14.289999999999992</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A109" s="1">
+        <v>43108.881249999999</v>
+      </c>
+      <c r="B109" s="1">
+        <v>43109.209027777775</v>
+      </c>
+      <c r="C109" s="3">
+        <v>406</v>
+      </c>
+      <c r="D109" s="3">
+        <v>66</v>
+      </c>
+      <c r="E109" s="3">
+        <v>28</v>
+      </c>
+      <c r="F109" s="3">
+        <v>472</v>
+      </c>
+      <c r="G109" s="3">
+        <v>48</v>
+      </c>
+      <c r="H109" s="3">
+        <v>242</v>
+      </c>
+      <c r="I109" s="3">
+        <v>116</v>
+      </c>
+      <c r="J109" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K109" s="2">
+        <f t="shared" si="15"/>
+        <v>86.02</v>
+      </c>
+      <c r="L109" s="2">
+        <f t="shared" si="16"/>
+        <v>13.98</v>
+      </c>
+      <c r="M109" s="2">
+        <f t="shared" si="17"/>
+        <v>51.27</v>
+      </c>
+      <c r="N109" s="2">
+        <f t="shared" si="18"/>
+        <v>10.17</v>
+      </c>
+      <c r="O109" s="2">
+        <f t="shared" si="19"/>
+        <v>24.58</v>
+      </c>
+      <c r="P109" s="2">
+        <f t="shared" si="20"/>
+        <v>13.97999999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A110" s="1">
+        <v>43109.900694444441</v>
+      </c>
+      <c r="B110" s="1">
+        <v>43110.206944444442</v>
+      </c>
+      <c r="C110" s="3">
+        <v>386</v>
+      </c>
+      <c r="D110" s="3">
+        <v>55</v>
+      </c>
+      <c r="E110" s="3">
+        <v>30</v>
+      </c>
+      <c r="F110" s="3">
+        <v>441</v>
+      </c>
+      <c r="G110" s="3">
+        <v>65</v>
+      </c>
+      <c r="H110" s="3">
+        <v>252</v>
+      </c>
+      <c r="I110" s="3">
+        <v>69</v>
+      </c>
+      <c r="J110" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K110" s="2">
+        <f t="shared" si="15"/>
+        <v>87.53</v>
+      </c>
+      <c r="L110" s="2">
+        <f t="shared" si="16"/>
+        <v>12.47</v>
+      </c>
+      <c r="M110" s="2">
+        <f t="shared" si="17"/>
+        <v>57.14</v>
+      </c>
+      <c r="N110" s="2">
+        <f t="shared" si="18"/>
+        <v>14.74</v>
+      </c>
+      <c r="O110" s="2">
+        <f t="shared" si="19"/>
+        <v>15.65</v>
+      </c>
+      <c r="P110" s="2">
+        <f t="shared" si="20"/>
+        <v>12.469999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A111" s="1">
+        <v>43110.887499999997</v>
+      </c>
+      <c r="B111" s="1">
+        <v>43111.185416666667</v>
+      </c>
+      <c r="C111" s="3">
+        <v>372</v>
+      </c>
+      <c r="D111" s="3">
+        <v>57</v>
+      </c>
+      <c r="E111" s="3">
+        <v>25</v>
+      </c>
+      <c r="F111" s="3">
+        <v>429</v>
+      </c>
+      <c r="G111" s="3">
+        <v>66</v>
+      </c>
+      <c r="H111" s="3">
+        <v>219</v>
+      </c>
+      <c r="I111" s="3">
+        <v>87</v>
+      </c>
+      <c r="J111" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K111" s="2">
+        <f t="shared" si="15"/>
+        <v>86.71</v>
+      </c>
+      <c r="L111" s="2">
+        <f t="shared" si="16"/>
+        <v>13.29</v>
+      </c>
+      <c r="M111" s="2">
+        <f t="shared" si="17"/>
+        <v>51.05</v>
+      </c>
+      <c r="N111" s="2">
+        <f t="shared" si="18"/>
+        <v>15.38</v>
+      </c>
+      <c r="O111" s="2">
+        <f t="shared" si="19"/>
+        <v>20.28</v>
+      </c>
+      <c r="P111" s="2">
+        <f t="shared" si="20"/>
+        <v>13.289999999999992</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A112" s="1">
+        <v>43111.897222222222</v>
+      </c>
+      <c r="B112" s="1">
+        <v>43112.169444444444</v>
+      </c>
+      <c r="C112" s="3">
+        <v>343</v>
+      </c>
+      <c r="D112" s="3">
+        <v>49</v>
+      </c>
+      <c r="E112" s="3">
+        <v>21</v>
+      </c>
+      <c r="F112" s="3">
+        <v>392</v>
+      </c>
+      <c r="G112" s="3">
+        <v>25</v>
+      </c>
+      <c r="H112" s="3">
+        <v>254</v>
+      </c>
+      <c r="I112" s="3">
+        <v>64</v>
+      </c>
+      <c r="J112" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K112" s="2">
+        <f t="shared" si="15"/>
+        <v>87.5</v>
+      </c>
+      <c r="L112" s="2">
+        <f t="shared" si="16"/>
+        <v>12.5</v>
+      </c>
+      <c r="M112" s="2">
+        <f t="shared" si="17"/>
+        <v>64.8</v>
+      </c>
+      <c r="N112" s="2">
+        <f t="shared" si="18"/>
+        <v>6.38</v>
+      </c>
+      <c r="O112" s="2">
+        <f t="shared" si="19"/>
+        <v>16.329999999999998</v>
+      </c>
+      <c r="P112" s="2">
+        <f t="shared" si="20"/>
+        <v>12.490000000000009</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A113" s="1">
+        <v>43112.917361111111</v>
+      </c>
+      <c r="B113" s="1">
+        <v>43113.275694444441</v>
+      </c>
+      <c r="C113" s="3">
+        <v>452</v>
+      </c>
+      <c r="D113" s="3">
+        <v>64</v>
+      </c>
+      <c r="E113" s="3">
+        <v>30</v>
+      </c>
+      <c r="F113" s="3">
+        <v>516</v>
+      </c>
+      <c r="G113" s="3">
+        <v>83</v>
+      </c>
+      <c r="H113" s="3">
+        <v>285</v>
+      </c>
+      <c r="I113" s="3">
+        <v>84</v>
+      </c>
+      <c r="J113" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K113" s="2">
+        <f t="shared" si="15"/>
+        <v>87.6</v>
+      </c>
+      <c r="L113" s="2">
+        <f t="shared" si="16"/>
+        <v>12.4</v>
+      </c>
+      <c r="M113" s="2">
+        <f t="shared" si="17"/>
+        <v>55.23</v>
+      </c>
+      <c r="N113" s="2">
+        <f t="shared" si="18"/>
+        <v>16.09</v>
+      </c>
+      <c r="O113" s="2">
+        <f t="shared" si="19"/>
+        <v>16.28</v>
+      </c>
+      <c r="P113" s="2">
+        <f t="shared" si="20"/>
+        <v>12.400000000000006</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A114" s="1">
+        <v>43113.910416666666</v>
+      </c>
+      <c r="B114" s="1">
+        <v>43114.220833333333</v>
+      </c>
+      <c r="C114" s="3">
+        <v>402</v>
+      </c>
+      <c r="D114" s="3">
+        <v>45</v>
+      </c>
+      <c r="E114" s="3">
+        <v>32</v>
+      </c>
+      <c r="F114" s="3">
+        <v>447</v>
+      </c>
+      <c r="G114" s="3">
+        <v>78</v>
+      </c>
+      <c r="H114" s="3">
+        <v>210</v>
+      </c>
+      <c r="I114" s="3">
+        <v>114</v>
+      </c>
+      <c r="J114" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K114" s="2">
+        <f t="shared" si="15"/>
+        <v>89.93</v>
+      </c>
+      <c r="L114" s="2">
+        <f t="shared" si="16"/>
+        <v>10.07</v>
+      </c>
+      <c r="M114" s="2">
+        <f t="shared" si="17"/>
+        <v>46.98</v>
+      </c>
+      <c r="N114" s="2">
+        <f t="shared" si="18"/>
+        <v>17.45</v>
+      </c>
+      <c r="O114" s="2">
+        <f t="shared" si="19"/>
+        <v>25.5</v>
+      </c>
+      <c r="P114" s="2">
+        <f t="shared" si="20"/>
+        <v>10.069999999999993</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A115" s="1">
+        <v>43114.881944444445</v>
+      </c>
+      <c r="B115" s="1">
+        <v>43115.207638888889</v>
+      </c>
+      <c r="C115" s="3">
+        <v>397</v>
+      </c>
+      <c r="D115" s="3">
+        <v>72</v>
+      </c>
+      <c r="E115" s="3">
+        <v>24</v>
+      </c>
+      <c r="F115" s="3">
+        <v>469</v>
+      </c>
+      <c r="G115" s="3">
+        <v>51</v>
+      </c>
+      <c r="H115" s="3">
+        <v>300</v>
+      </c>
+      <c r="I115" s="3">
+        <v>46</v>
+      </c>
+      <c r="J115" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K115" s="2">
+        <f t="shared" si="15"/>
+        <v>84.65</v>
+      </c>
+      <c r="L115" s="2">
+        <f t="shared" si="16"/>
+        <v>15.35</v>
+      </c>
+      <c r="M115" s="2">
+        <f t="shared" si="17"/>
+        <v>63.97</v>
+      </c>
+      <c r="N115" s="2">
+        <f t="shared" si="18"/>
+        <v>10.87</v>
+      </c>
+      <c r="O115" s="2">
+        <f t="shared" si="19"/>
+        <v>9.81</v>
+      </c>
+      <c r="P115" s="2">
+        <f t="shared" si="20"/>
+        <v>15.349999999999994</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>43115.918055555558</v>
+      </c>
+      <c r="B116" s="1">
+        <v>43116.263194444444</v>
+      </c>
+      <c r="C116" s="3">
+        <v>428</v>
+      </c>
+      <c r="D116" s="3">
+        <v>69</v>
+      </c>
+      <c r="E116" s="3">
+        <v>37</v>
+      </c>
+      <c r="F116" s="3">
+        <v>497</v>
+      </c>
+      <c r="G116" s="3">
+        <v>53</v>
+      </c>
+      <c r="H116" s="3">
+        <v>276</v>
+      </c>
+      <c r="I116" s="3">
+        <v>99</v>
+      </c>
+      <c r="J116" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K116" s="2">
+        <f t="shared" si="15"/>
+        <v>86.12</v>
+      </c>
+      <c r="L116" s="2">
+        <f t="shared" si="16"/>
+        <v>13.88</v>
+      </c>
+      <c r="M116" s="2">
+        <f t="shared" si="17"/>
+        <v>55.53</v>
+      </c>
+      <c r="N116" s="2">
+        <f t="shared" si="18"/>
+        <v>10.66</v>
+      </c>
+      <c r="O116" s="2">
+        <f t="shared" si="19"/>
+        <v>19.920000000000002</v>
+      </c>
+      <c r="P116" s="2">
+        <f t="shared" si="20"/>
+        <v>13.89</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A117" s="1">
+        <v>43116.893750000003</v>
+      </c>
+      <c r="B117" s="1">
+        <v>43117.207638888889</v>
+      </c>
+      <c r="C117" s="3">
+        <v>394</v>
+      </c>
+      <c r="D117" s="3">
+        <v>58</v>
+      </c>
+      <c r="E117" s="3">
+        <v>34</v>
+      </c>
+      <c r="F117" s="3">
+        <v>452</v>
+      </c>
+      <c r="G117" s="3">
+        <v>49</v>
+      </c>
+      <c r="H117" s="3">
+        <v>271</v>
+      </c>
+      <c r="I117" s="3">
+        <v>74</v>
+      </c>
+      <c r="J117" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K117" s="2">
+        <f t="shared" si="15"/>
+        <v>87.17</v>
+      </c>
+      <c r="L117" s="2">
+        <f t="shared" si="16"/>
+        <v>12.83</v>
+      </c>
+      <c r="M117" s="2">
+        <f t="shared" si="17"/>
+        <v>59.96</v>
+      </c>
+      <c r="N117" s="2">
+        <f t="shared" si="18"/>
+        <v>10.84</v>
+      </c>
+      <c r="O117" s="2">
+        <f t="shared" si="19"/>
+        <v>16.37</v>
+      </c>
+      <c r="P117" s="2">
+        <f t="shared" si="20"/>
+        <v>12.829999999999998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A118" s="1">
+        <v>43117.890277777777</v>
+      </c>
+      <c r="B118" s="1">
+        <v>43118.211805555555</v>
+      </c>
+      <c r="C118" s="3">
+        <v>409</v>
+      </c>
+      <c r="D118" s="3">
+        <v>54</v>
+      </c>
+      <c r="E118" s="3">
+        <v>30</v>
+      </c>
+      <c r="F118" s="3">
+        <v>463</v>
+      </c>
+      <c r="G118" s="3">
+        <v>61</v>
+      </c>
+      <c r="H118" s="3">
+        <v>248</v>
+      </c>
+      <c r="I118" s="3">
+        <v>100</v>
+      </c>
+      <c r="J118" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K118" s="2">
+        <f t="shared" si="15"/>
+        <v>88.34</v>
+      </c>
+      <c r="L118" s="2">
+        <f t="shared" si="16"/>
+        <v>11.66</v>
+      </c>
+      <c r="M118" s="2">
+        <f t="shared" si="17"/>
+        <v>53.56</v>
+      </c>
+      <c r="N118" s="2">
+        <f t="shared" si="18"/>
+        <v>13.17</v>
+      </c>
+      <c r="O118" s="2">
+        <f t="shared" si="19"/>
+        <v>21.6</v>
+      </c>
+      <c r="P118" s="2">
+        <f t="shared" si="20"/>
+        <v>11.669999999999987</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A119" s="1">
+        <v>43118.894444444442</v>
+      </c>
+      <c r="B119" s="1">
+        <v>43119.197222222225</v>
+      </c>
+      <c r="C119" s="3">
+        <v>407</v>
+      </c>
+      <c r="D119" s="3">
+        <v>24</v>
+      </c>
+      <c r="E119" s="3">
+        <v>1</v>
+      </c>
+      <c r="F119" s="3">
+        <v>436</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J119" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K119" s="2">
+        <f t="shared" si="15"/>
+        <v>93.35</v>
+      </c>
+      <c r="L119" s="2">
+        <f t="shared" si="16"/>
+        <v>5.5</v>
+      </c>
+      <c r="M119" s="2" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N119" s="2" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O119" s="2" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P119" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A120" s="1">
+        <v>43119.897222222222</v>
+      </c>
+      <c r="B120" s="1">
+        <v>43120.26666666667</v>
+      </c>
+      <c r="C120" s="3">
+        <v>455</v>
+      </c>
+      <c r="D120" s="3">
+        <v>77</v>
+      </c>
+      <c r="E120" s="3">
+        <v>30</v>
+      </c>
+      <c r="F120" s="3">
+        <v>532</v>
+      </c>
+      <c r="G120" s="3">
+        <v>66</v>
+      </c>
+      <c r="H120" s="3">
+        <v>265</v>
+      </c>
+      <c r="I120" s="3">
+        <v>124</v>
+      </c>
+      <c r="J120" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K120" s="2">
+        <f t="shared" si="15"/>
+        <v>85.53</v>
+      </c>
+      <c r="L120" s="2">
+        <f t="shared" si="16"/>
+        <v>14.47</v>
+      </c>
+      <c r="M120" s="2">
+        <f t="shared" si="17"/>
+        <v>49.81</v>
+      </c>
+      <c r="N120" s="2">
+        <f t="shared" si="18"/>
+        <v>12.41</v>
+      </c>
+      <c r="O120" s="2">
+        <f t="shared" si="19"/>
+        <v>23.31</v>
+      </c>
+      <c r="P120" s="2">
+        <f t="shared" si="20"/>
+        <v>14.469999999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A121" s="1">
+        <v>43120.92291666667</v>
+      </c>
+      <c r="B121" s="1">
+        <v>43121.251388888886</v>
+      </c>
+      <c r="C121" s="3">
+        <v>416</v>
+      </c>
+      <c r="D121" s="3">
+        <v>57</v>
+      </c>
+      <c r="E121" s="3">
+        <v>37</v>
+      </c>
+      <c r="F121" s="3">
+        <v>473</v>
+      </c>
+      <c r="G121" s="3">
+        <v>79</v>
+      </c>
+      <c r="H121" s="3">
+        <v>231</v>
+      </c>
+      <c r="I121" s="3">
+        <v>106</v>
+      </c>
+      <c r="J121" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K121" s="2">
+        <f t="shared" si="15"/>
+        <v>87.95</v>
+      </c>
+      <c r="L121" s="2">
+        <f t="shared" si="16"/>
+        <v>12.05</v>
+      </c>
+      <c r="M121" s="2">
+        <f t="shared" si="17"/>
+        <v>48.84</v>
+      </c>
+      <c r="N121" s="2">
+        <f t="shared" si="18"/>
+        <v>16.7</v>
+      </c>
+      <c r="O121" s="2">
+        <f t="shared" si="19"/>
+        <v>22.41</v>
+      </c>
+      <c r="P121" s="2">
+        <f t="shared" si="20"/>
+        <v>12.049999999999997</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A122" s="1">
+        <v>43121.89166666667</v>
+      </c>
+      <c r="B122" s="1">
+        <v>43122.210416666669</v>
+      </c>
+      <c r="C122" s="3">
+        <v>398</v>
+      </c>
+      <c r="D122" s="3">
+        <v>61</v>
+      </c>
+      <c r="E122" s="3">
+        <v>27</v>
+      </c>
+      <c r="F122" s="3">
+        <v>459</v>
+      </c>
+      <c r="G122" s="3">
+        <v>47</v>
+      </c>
+      <c r="H122" s="3">
+        <v>251</v>
+      </c>
+      <c r="I122" s="3">
+        <v>100</v>
+      </c>
+      <c r="J122" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K122" s="2">
+        <f t="shared" si="15"/>
+        <v>86.71</v>
+      </c>
+      <c r="L122" s="2">
+        <f t="shared" si="16"/>
+        <v>13.29</v>
+      </c>
+      <c r="M122" s="2">
+        <f t="shared" si="17"/>
+        <v>54.68</v>
+      </c>
+      <c r="N122" s="2">
+        <f t="shared" si="18"/>
+        <v>10.24</v>
+      </c>
+      <c r="O122" s="2">
+        <f t="shared" si="19"/>
+        <v>21.79</v>
+      </c>
+      <c r="P122" s="2">
+        <f t="shared" si="20"/>
+        <v>13.289999999999992</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A123" s="1">
+        <v>43122.900694444441</v>
+      </c>
+      <c r="B123" s="1">
+        <v>43123.222916666666</v>
+      </c>
+      <c r="C123" s="3">
+        <v>412</v>
+      </c>
+      <c r="D123" s="3">
+        <v>52</v>
+      </c>
+      <c r="E123" s="3">
+        <v>23</v>
+      </c>
+      <c r="F123" s="3">
+        <v>464</v>
+      </c>
+      <c r="G123" s="3">
+        <v>70</v>
+      </c>
+      <c r="H123" s="3">
+        <v>243</v>
+      </c>
+      <c r="I123" s="3">
+        <v>99</v>
+      </c>
+      <c r="J123" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K123" s="2">
+        <f t="shared" si="15"/>
+        <v>88.79</v>
+      </c>
+      <c r="L123" s="2">
+        <f t="shared" si="16"/>
+        <v>11.21</v>
+      </c>
+      <c r="M123" s="2">
+        <f t="shared" si="17"/>
+        <v>52.37</v>
+      </c>
+      <c r="N123" s="2">
+        <f t="shared" si="18"/>
+        <v>15.09</v>
+      </c>
+      <c r="O123" s="2">
+        <f t="shared" si="19"/>
+        <v>21.34</v>
+      </c>
+      <c r="P123" s="2">
+        <f t="shared" si="20"/>
+        <v>11.200000000000003</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A124" s="1">
+        <v>43123.909722222219</v>
+      </c>
+      <c r="B124" s="1">
+        <v>43124.254861111112</v>
+      </c>
+      <c r="C124" s="3">
+        <v>390</v>
+      </c>
+      <c r="D124" s="3">
+        <v>107</v>
+      </c>
+      <c r="E124" s="3">
+        <v>23</v>
+      </c>
+      <c r="F124" s="3">
+        <v>497</v>
+      </c>
+      <c r="G124" s="3">
+        <v>48</v>
+      </c>
+      <c r="H124" s="3">
+        <v>282</v>
+      </c>
+      <c r="I124" s="3">
+        <v>60</v>
+      </c>
+      <c r="J124" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K124" s="2">
+        <f t="shared" si="15"/>
+        <v>78.47</v>
+      </c>
+      <c r="L124" s="2">
+        <f t="shared" si="16"/>
+        <v>21.53</v>
+      </c>
+      <c r="M124" s="2">
+        <f t="shared" si="17"/>
+        <v>56.74</v>
+      </c>
+      <c r="N124" s="2">
+        <f t="shared" si="18"/>
+        <v>9.66</v>
+      </c>
+      <c r="O124" s="2">
+        <f t="shared" si="19"/>
+        <v>12.07</v>
+      </c>
+      <c r="P124" s="2">
+        <f t="shared" si="20"/>
+        <v>21.53</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A125" s="1">
+        <v>43124.738194444442</v>
+      </c>
+      <c r="B125" s="1">
+        <v>43125.15</v>
+      </c>
+      <c r="C125" s="3">
+        <v>511</v>
+      </c>
+      <c r="D125" s="3">
+        <v>82</v>
+      </c>
+      <c r="E125" s="3">
+        <v>36</v>
+      </c>
+      <c r="F125" s="3">
+        <v>593</v>
+      </c>
+      <c r="G125" s="3">
+        <v>33</v>
+      </c>
+      <c r="H125" s="3">
+        <v>407</v>
+      </c>
+      <c r="I125" s="3">
+        <v>71</v>
+      </c>
+      <c r="J125" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K125" s="2">
+        <f t="shared" si="15"/>
+        <v>86.17</v>
+      </c>
+      <c r="L125" s="2">
+        <f t="shared" si="16"/>
+        <v>13.83</v>
+      </c>
+      <c r="M125" s="2">
+        <f t="shared" si="17"/>
+        <v>68.63</v>
+      </c>
+      <c r="N125" s="2">
+        <f t="shared" si="18"/>
+        <v>5.56</v>
+      </c>
+      <c r="O125" s="2">
+        <f t="shared" si="19"/>
+        <v>11.97</v>
+      </c>
+      <c r="P125" s="2">
+        <f t="shared" si="20"/>
+        <v>13.840000000000003</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A126" s="1">
+        <v>43125.880555555559</v>
+      </c>
+      <c r="B126" s="1">
+        <v>43126.218055555553</v>
+      </c>
+      <c r="C126" s="3">
+        <v>434</v>
+      </c>
+      <c r="D126" s="3">
+        <v>52</v>
+      </c>
+      <c r="E126" s="3">
+        <v>25</v>
+      </c>
+      <c r="F126" s="3">
+        <v>486</v>
+      </c>
+      <c r="G126" s="3">
+        <v>98</v>
+      </c>
+      <c r="H126" s="3">
+        <v>249</v>
+      </c>
+      <c r="I126" s="3">
+        <v>87</v>
+      </c>
+      <c r="J126" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="K126" s="2">
+        <f t="shared" si="15"/>
+        <v>89.3</v>
+      </c>
+      <c r="L126" s="2">
+        <f t="shared" si="16"/>
+        <v>10.7</v>
+      </c>
+      <c r="M126" s="2">
+        <f t="shared" si="17"/>
+        <v>51.23</v>
+      </c>
+      <c r="N126" s="2">
+        <f t="shared" si="18"/>
+        <v>20.16</v>
+      </c>
+      <c r="O126" s="2">
+        <f t="shared" si="19"/>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="P126" s="2">
+        <f t="shared" si="20"/>
+        <v>10.710000000000008</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A127" s="1">
+        <v>43126.9375</v>
+      </c>
+      <c r="B127" s="1">
+        <v>43127.179861111108</v>
+      </c>
+      <c r="C127" s="3">
+        <v>302</v>
+      </c>
+      <c r="D127" s="3">
+        <v>47</v>
+      </c>
+      <c r="E127" s="3">
+        <v>26</v>
+      </c>
+      <c r="F127" s="3">
+        <v>349</v>
+      </c>
+      <c r="G127" s="3">
+        <v>48</v>
+      </c>
+      <c r="H127" s="3">
+        <v>178</v>
+      </c>
+      <c r="I127" s="3">
+        <v>76</v>
+      </c>
+      <c r="J127" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K127" s="2">
+        <f t="shared" si="15"/>
+        <v>86.53</v>
+      </c>
+      <c r="L127" s="2">
+        <f t="shared" si="16"/>
+        <v>13.47</v>
+      </c>
+      <c r="M127" s="2">
+        <f t="shared" si="17"/>
+        <v>51</v>
+      </c>
+      <c r="N127" s="2">
+        <f t="shared" si="18"/>
+        <v>13.75</v>
+      </c>
+      <c r="O127" s="2">
+        <f t="shared" si="19"/>
+        <v>21.78</v>
+      </c>
+      <c r="P127" s="2">
+        <f t="shared" si="20"/>
+        <v>13.469999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A128" s="1">
+        <v>43127.894444444442</v>
+      </c>
+      <c r="B128" s="1">
+        <v>43128.19027777778</v>
+      </c>
+      <c r="C128" s="3">
+        <v>359</v>
+      </c>
+      <c r="D128" s="3">
+        <v>67</v>
+      </c>
+      <c r="E128" s="3">
+        <v>30</v>
+      </c>
+      <c r="F128" s="3">
+        <v>426</v>
+      </c>
+      <c r="G128" s="3">
+        <v>50</v>
+      </c>
+      <c r="H128" s="3">
+        <v>214</v>
+      </c>
+      <c r="I128" s="3">
+        <v>95</v>
+      </c>
+      <c r="J128" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K128" s="2">
+        <f t="shared" si="15"/>
+        <v>84.27</v>
+      </c>
+      <c r="L128" s="2">
+        <f t="shared" si="16"/>
+        <v>15.73</v>
+      </c>
+      <c r="M128" s="2">
+        <f t="shared" si="17"/>
+        <v>50.23</v>
+      </c>
+      <c r="N128" s="2">
+        <f t="shared" si="18"/>
+        <v>11.74</v>
+      </c>
+      <c r="O128" s="2">
+        <f t="shared" si="19"/>
+        <v>22.3</v>
+      </c>
+      <c r="P128" s="2">
+        <f t="shared" si="20"/>
+        <v>15.730000000000004</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A129" s="1">
+        <v>43130.906944444447</v>
+      </c>
+      <c r="B129" s="1">
+        <v>43131.154166666667</v>
+      </c>
+      <c r="C129" s="3">
+        <v>312</v>
+      </c>
+      <c r="D129" s="3">
+        <v>44</v>
+      </c>
+      <c r="E129" s="3">
+        <v>19</v>
+      </c>
+      <c r="F129" s="3">
+        <v>356</v>
+      </c>
+      <c r="G129" s="3">
+        <v>56</v>
+      </c>
+      <c r="H129" s="3">
+        <v>200</v>
+      </c>
+      <c r="I129" s="3">
+        <v>56</v>
+      </c>
+      <c r="J129" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K129" s="2">
+        <f t="shared" si="15"/>
+        <v>87.64</v>
+      </c>
+      <c r="L129" s="2">
+        <f t="shared" si="16"/>
+        <v>12.36</v>
+      </c>
+      <c r="M129" s="2">
+        <f t="shared" si="17"/>
+        <v>56.18</v>
+      </c>
+      <c r="N129" s="2">
+        <f t="shared" si="18"/>
+        <v>15.73</v>
+      </c>
+      <c r="O129" s="2">
+        <f t="shared" si="19"/>
+        <v>15.73</v>
+      </c>
+      <c r="P129" s="2">
+        <f t="shared" si="20"/>
+        <v>12.36</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:P76">
-    <sortCondition ref="A2"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating February 2018 TotalSleep
</commit_message>
<xml_diff>
--- a/datasets/TotalSleep.xlsx
+++ b/datasets/TotalSleep.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23C1625-E038-4A8D-AB16-ADB67FD9D8F5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
   <si>
     <t>Start Time</t>
   </si>
@@ -70,6 +71,186 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>01-02-2018 9:53 pm</t>
+  </si>
+  <si>
+    <t>02-02-2018 4:42 am</t>
+  </si>
+  <si>
+    <t>02-02-2018 9:59 pm</t>
+  </si>
+  <si>
+    <t>03-02-2018 4:44 am</t>
+  </si>
+  <si>
+    <t>04-02-2018 10:14 pm</t>
+  </si>
+  <si>
+    <t>05-02-2018 4:01 am</t>
+  </si>
+  <si>
+    <t>04-02-2018 12:30 am</t>
+  </si>
+  <si>
+    <t>04-02-2018 6:03 am</t>
+  </si>
+  <si>
+    <t>05-02-2018 9:27 pm</t>
+  </si>
+  <si>
+    <t>06-02-2018 5:10 am</t>
+  </si>
+  <si>
+    <t>06-02-2018 9:12 pm</t>
+  </si>
+  <si>
+    <t>07-02-2018 2:04 am</t>
+  </si>
+  <si>
+    <t>07-02-2018 4:18 am</t>
+  </si>
+  <si>
+    <t>07-02-2018 6:01 am</t>
+  </si>
+  <si>
+    <t>07-02-2018 9:08 pm</t>
+  </si>
+  <si>
+    <t>08-02-2018 2:45 am</t>
+  </si>
+  <si>
+    <t>08-02-2018 8:47 pm</t>
+  </si>
+  <si>
+    <t>09-02-2018 4:16 am</t>
+  </si>
+  <si>
+    <t>09-02-2018 9:48 pm</t>
+  </si>
+  <si>
+    <t>10-02-2018 5:48 am</t>
+  </si>
+  <si>
+    <t>10-02-2018 8:25 pm</t>
+  </si>
+  <si>
+    <t>11-02-2018 4:27 am</t>
+  </si>
+  <si>
+    <t>11-02-2018 9:27 pm</t>
+  </si>
+  <si>
+    <t>12-02-2018 3:54 am</t>
+  </si>
+  <si>
+    <t>12-02-2018 9:30 pm</t>
+  </si>
+  <si>
+    <t>13-02-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>14-02-2018 2:00 am</t>
+  </si>
+  <si>
+    <t>14-02-2018 4:38 am</t>
+  </si>
+  <si>
+    <t>14-02-2018 9:13 pm</t>
+  </si>
+  <si>
+    <t>15-02-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>15-02-2018 9:50 pm</t>
+  </si>
+  <si>
+    <t>16-02-2018 4:07 am</t>
+  </si>
+  <si>
+    <t>16-02-2018 10:18 pm</t>
+  </si>
+  <si>
+    <t>17-02-2018 5:13 am</t>
+  </si>
+  <si>
+    <t>17-02-2018 10:12 pm</t>
+  </si>
+  <si>
+    <t>18-02-2018 5:08 am</t>
+  </si>
+  <si>
+    <t>18-02-2018 10:31 pm</t>
+  </si>
+  <si>
+    <t>19-02-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>19-02-2018 9:51 pm</t>
+  </si>
+  <si>
+    <t>20-02-2018 4:28 am</t>
+  </si>
+  <si>
+    <t>20-02-2018 11:00 pm</t>
+  </si>
+  <si>
+    <t>21-02-2018 5:05 am</t>
+  </si>
+  <si>
+    <t>21-02-2018 10:44 pm</t>
+  </si>
+  <si>
+    <t>22-02-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>22-02-2018 9:27 pm</t>
+  </si>
+  <si>
+    <t>23-02-2018 4:56 am</t>
+  </si>
+  <si>
+    <t>23-02-2018 9:53 pm</t>
+  </si>
+  <si>
+    <t>24-02-2018 6:02 am</t>
+  </si>
+  <si>
+    <t>25-02-2018 3:18 am</t>
+  </si>
+  <si>
+    <t>25-02-2018 9:04 am</t>
+  </si>
+  <si>
+    <t>25-02-2018 9:55 pm</t>
+  </si>
+  <si>
+    <t>26-02-2018 5:04 am</t>
+  </si>
+  <si>
+    <t>26-02-2018 9:54 pm</t>
+  </si>
+  <si>
+    <t>27-02-2018 4:51 am</t>
+  </si>
+  <si>
+    <t>27-02-2018 10:06 pm</t>
+  </si>
+  <si>
+    <t>28-02-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>31-01-2018 9:53 pm</t>
+  </si>
+  <si>
+    <t>01-02-2018 2:33 am</t>
+  </si>
+  <si>
+    <t>01-02-2018 2:44 pm</t>
+  </si>
+  <si>
+    <t>01-02-2018 4:12 pm</t>
   </si>
 </sst>
 </file>
@@ -214,6 +395,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -558,11 +740,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -919,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P129"/>
+  <dimension ref="A1:P159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P99" sqref="P99:P129"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P129" sqref="P129:P159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4670,31 +4853,31 @@
         <v>86</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ref="J66:J129" si="14">IF(C66&gt;=420,"Yes","No")</f>
+        <f t="shared" ref="J66:J130" si="14">IF(C66&gt;=420,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="K66" s="2">
-        <f t="shared" ref="K66:K129" si="15">ROUND((C66/F66)*100, 2)</f>
+        <f t="shared" ref="K66:K130" si="15">ROUND((C66/F66)*100, 2)</f>
         <v>88.02</v>
       </c>
       <c r="L66" s="2">
-        <f t="shared" ref="L66:L129" si="16">ROUND((D66/F66)*100,2)</f>
+        <f t="shared" ref="L66:L130" si="16">ROUND((D66/F66)*100,2)</f>
         <v>11.98</v>
       </c>
       <c r="M66" s="2">
-        <f t="shared" ref="M66:M129" si="17">ROUND((H66/F66)*100,2)</f>
+        <f t="shared" ref="M66:M130" si="17">ROUND((H66/F66)*100,2)</f>
         <v>50</v>
       </c>
       <c r="N66" s="2">
-        <f t="shared" ref="N66:N129" si="18">ROUND((G66/F66)*100,2)</f>
+        <f t="shared" ref="N66:N130" si="18">ROUND((G66/F66)*100,2)</f>
         <v>18.2</v>
       </c>
       <c r="O66" s="2">
-        <f t="shared" ref="O66:O129" si="19">ROUND((I66/F66)*100,2)</f>
+        <f t="shared" ref="O66:O130" si="19">ROUND((I66/F66)*100,2)</f>
         <v>19.82</v>
       </c>
       <c r="P66" s="2">
-        <f t="shared" ref="P66:P129" si="20">100-(O66+N66+M66)</f>
+        <f t="shared" ref="P66:P130" si="20">100-(O66+N66+M66)</f>
         <v>11.980000000000004</v>
       </c>
     </row>
@@ -8287,6 +8470,1716 @@
       <c r="P129" s="2">
         <f t="shared" si="20"/>
         <v>12.36</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C130" s="4">
+        <v>269</v>
+      </c>
+      <c r="D130" s="4">
+        <v>3</v>
+      </c>
+      <c r="E130" s="4">
+        <v>1</v>
+      </c>
+      <c r="F130" s="4">
+        <v>280</v>
+      </c>
+      <c r="G130" t="s">
+        <v>16</v>
+      </c>
+      <c r="H130" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130" t="s">
+        <v>16</v>
+      </c>
+      <c r="J130" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="K130" s="2">
+        <f t="shared" si="15"/>
+        <v>96.07</v>
+      </c>
+      <c r="L130" s="2">
+        <f t="shared" si="16"/>
+        <v>1.07</v>
+      </c>
+      <c r="M130" s="2" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N130" s="2" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O130" s="2" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P130" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C131" s="4">
+        <v>83</v>
+      </c>
+      <c r="D131" s="4">
+        <v>5</v>
+      </c>
+      <c r="E131" s="4">
+        <v>0</v>
+      </c>
+      <c r="F131" s="4">
+        <v>88</v>
+      </c>
+      <c r="G131" t="s">
+        <v>16</v>
+      </c>
+      <c r="H131" t="s">
+        <v>16</v>
+      </c>
+      <c r="I131" t="s">
+        <v>16</v>
+      </c>
+      <c r="J131" t="str">
+        <f t="shared" ref="J131:J159" si="21">IF(C131&gt;=420,"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="K131" s="2">
+        <f t="shared" ref="K131:K159" si="22">ROUND((C131/F131)*100, 2)</f>
+        <v>94.32</v>
+      </c>
+      <c r="L131" s="2">
+        <f t="shared" ref="L131:L159" si="23">ROUND((D131/F131)*100,2)</f>
+        <v>5.68</v>
+      </c>
+      <c r="M131" s="2" t="e">
+        <f t="shared" ref="M131:M159" si="24">ROUND((H131/F131)*100,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N131" s="2" t="e">
+        <f t="shared" ref="N131:N159" si="25">ROUND((G131/F131)*100,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O131" s="2" t="e">
+        <f t="shared" ref="O131:O159" si="26">ROUND((I131/F131)*100,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P131" s="2" t="e">
+        <f t="shared" ref="P131:P159" si="27">100-(O131+N131+M131)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C132" s="4">
+        <v>353</v>
+      </c>
+      <c r="D132" s="4">
+        <v>56</v>
+      </c>
+      <c r="E132" s="4">
+        <v>21</v>
+      </c>
+      <c r="F132" s="4">
+        <v>409</v>
+      </c>
+      <c r="G132" s="4">
+        <v>54</v>
+      </c>
+      <c r="H132" s="4">
+        <v>204</v>
+      </c>
+      <c r="I132" s="4">
+        <v>95</v>
+      </c>
+      <c r="J132" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K132" s="2">
+        <f t="shared" si="22"/>
+        <v>86.31</v>
+      </c>
+      <c r="L132" s="2">
+        <f t="shared" si="23"/>
+        <v>13.69</v>
+      </c>
+      <c r="M132" s="2">
+        <f t="shared" si="24"/>
+        <v>49.88</v>
+      </c>
+      <c r="N132" s="2">
+        <f t="shared" si="25"/>
+        <v>13.2</v>
+      </c>
+      <c r="O132" s="2">
+        <f t="shared" si="26"/>
+        <v>23.23</v>
+      </c>
+      <c r="P132" s="2">
+        <f t="shared" si="27"/>
+        <v>13.689999999999998</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C133" s="4">
+        <v>358</v>
+      </c>
+      <c r="D133" s="4">
+        <v>47</v>
+      </c>
+      <c r="E133" s="4">
+        <v>27</v>
+      </c>
+      <c r="F133" s="4">
+        <v>405</v>
+      </c>
+      <c r="G133" s="4">
+        <v>61</v>
+      </c>
+      <c r="H133" s="4">
+        <v>224</v>
+      </c>
+      <c r="I133" s="4">
+        <v>73</v>
+      </c>
+      <c r="J133" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K133" s="2">
+        <f t="shared" si="22"/>
+        <v>88.4</v>
+      </c>
+      <c r="L133" s="2">
+        <f t="shared" si="23"/>
+        <v>11.6</v>
+      </c>
+      <c r="M133" s="2">
+        <f t="shared" si="24"/>
+        <v>55.31</v>
+      </c>
+      <c r="N133" s="2">
+        <f t="shared" si="25"/>
+        <v>15.06</v>
+      </c>
+      <c r="O133" s="2">
+        <f t="shared" si="26"/>
+        <v>18.02</v>
+      </c>
+      <c r="P133" s="2">
+        <f t="shared" si="27"/>
+        <v>11.61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C134" s="4">
+        <v>309</v>
+      </c>
+      <c r="D134" s="4">
+        <v>37</v>
+      </c>
+      <c r="E134" s="4">
+        <v>17</v>
+      </c>
+      <c r="F134" s="4">
+        <v>346</v>
+      </c>
+      <c r="G134" s="4">
+        <v>19</v>
+      </c>
+      <c r="H134" s="4">
+        <v>224</v>
+      </c>
+      <c r="I134" s="4">
+        <v>66</v>
+      </c>
+      <c r="J134" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K134" s="2">
+        <f t="shared" si="22"/>
+        <v>89.31</v>
+      </c>
+      <c r="L134" s="2">
+        <f t="shared" si="23"/>
+        <v>10.69</v>
+      </c>
+      <c r="M134" s="2">
+        <f t="shared" si="24"/>
+        <v>64.739999999999995</v>
+      </c>
+      <c r="N134" s="2">
+        <f t="shared" si="25"/>
+        <v>5.49</v>
+      </c>
+      <c r="O134" s="2">
+        <f t="shared" si="26"/>
+        <v>19.079999999999998</v>
+      </c>
+      <c r="P134" s="2">
+        <f t="shared" si="27"/>
+        <v>10.689999999999998</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" s="4">
+        <v>299</v>
+      </c>
+      <c r="D135" s="4">
+        <v>34</v>
+      </c>
+      <c r="E135" s="4">
+        <v>22</v>
+      </c>
+      <c r="F135" s="4">
+        <v>333</v>
+      </c>
+      <c r="G135" s="4">
+        <v>65</v>
+      </c>
+      <c r="H135" s="4">
+        <v>171</v>
+      </c>
+      <c r="I135" s="4">
+        <v>63</v>
+      </c>
+      <c r="J135" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K135" s="2">
+        <f t="shared" si="22"/>
+        <v>89.79</v>
+      </c>
+      <c r="L135" s="2">
+        <f t="shared" si="23"/>
+        <v>10.210000000000001</v>
+      </c>
+      <c r="M135" s="2">
+        <f t="shared" si="24"/>
+        <v>51.35</v>
+      </c>
+      <c r="N135" s="2">
+        <f t="shared" si="25"/>
+        <v>19.52</v>
+      </c>
+      <c r="O135" s="2">
+        <f t="shared" si="26"/>
+        <v>18.920000000000002</v>
+      </c>
+      <c r="P135" s="2">
+        <f t="shared" si="27"/>
+        <v>10.210000000000008</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A136" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C136" s="4">
+        <v>413</v>
+      </c>
+      <c r="D136" s="4">
+        <v>50</v>
+      </c>
+      <c r="E136" s="4">
+        <v>32</v>
+      </c>
+      <c r="F136" s="4">
+        <v>463</v>
+      </c>
+      <c r="G136" s="4">
+        <v>57</v>
+      </c>
+      <c r="H136" s="4">
+        <v>256</v>
+      </c>
+      <c r="I136" s="4">
+        <v>100</v>
+      </c>
+      <c r="J136" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K136" s="2">
+        <f t="shared" si="22"/>
+        <v>89.2</v>
+      </c>
+      <c r="L136" s="2">
+        <f t="shared" si="23"/>
+        <v>10.8</v>
+      </c>
+      <c r="M136" s="2">
+        <f t="shared" si="24"/>
+        <v>55.29</v>
+      </c>
+      <c r="N136" s="2">
+        <f t="shared" si="25"/>
+        <v>12.31</v>
+      </c>
+      <c r="O136" s="2">
+        <f t="shared" si="26"/>
+        <v>21.6</v>
+      </c>
+      <c r="P136" s="2">
+        <f t="shared" si="27"/>
+        <v>10.799999999999997</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A137" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C137" s="4">
+        <v>260</v>
+      </c>
+      <c r="D137" s="4">
+        <v>32</v>
+      </c>
+      <c r="E137" s="4">
+        <v>23</v>
+      </c>
+      <c r="F137" s="4">
+        <v>292</v>
+      </c>
+      <c r="G137" s="4">
+        <v>45</v>
+      </c>
+      <c r="H137" s="4">
+        <v>143</v>
+      </c>
+      <c r="I137" s="4">
+        <v>72</v>
+      </c>
+      <c r="J137" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K137" s="2">
+        <f t="shared" si="22"/>
+        <v>89.04</v>
+      </c>
+      <c r="L137" s="2">
+        <f t="shared" si="23"/>
+        <v>10.96</v>
+      </c>
+      <c r="M137" s="2">
+        <f t="shared" si="24"/>
+        <v>48.97</v>
+      </c>
+      <c r="N137" s="2">
+        <f t="shared" si="25"/>
+        <v>15.41</v>
+      </c>
+      <c r="O137" s="2">
+        <f t="shared" si="26"/>
+        <v>24.66</v>
+      </c>
+      <c r="P137" s="2">
+        <f t="shared" si="27"/>
+        <v>10.960000000000008</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C138" s="4">
+        <v>96</v>
+      </c>
+      <c r="D138" s="4">
+        <v>7</v>
+      </c>
+      <c r="E138" s="4">
+        <v>0</v>
+      </c>
+      <c r="F138" s="4">
+        <v>103</v>
+      </c>
+      <c r="G138" t="s">
+        <v>16</v>
+      </c>
+      <c r="H138" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138" t="s">
+        <v>16</v>
+      </c>
+      <c r="J138" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K138" s="2">
+        <f t="shared" si="22"/>
+        <v>93.2</v>
+      </c>
+      <c r="L138" s="2">
+        <f t="shared" si="23"/>
+        <v>6.8</v>
+      </c>
+      <c r="M138" s="2" t="e">
+        <f t="shared" si="24"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N138" s="2" t="e">
+        <f t="shared" si="25"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O138" s="2" t="e">
+        <f t="shared" si="26"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P138" s="2" t="e">
+        <f t="shared" si="27"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C139" s="4">
+        <v>309</v>
+      </c>
+      <c r="D139" s="4">
+        <v>28</v>
+      </c>
+      <c r="E139" s="4">
+        <v>22</v>
+      </c>
+      <c r="F139" s="4">
+        <v>337</v>
+      </c>
+      <c r="G139" s="4">
+        <v>81</v>
+      </c>
+      <c r="H139" s="4">
+        <v>164</v>
+      </c>
+      <c r="I139" s="4">
+        <v>64</v>
+      </c>
+      <c r="J139" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K139" s="2">
+        <f t="shared" si="22"/>
+        <v>91.69</v>
+      </c>
+      <c r="L139" s="2">
+        <f t="shared" si="23"/>
+        <v>8.31</v>
+      </c>
+      <c r="M139" s="2">
+        <f t="shared" si="24"/>
+        <v>48.66</v>
+      </c>
+      <c r="N139" s="2">
+        <f t="shared" si="25"/>
+        <v>24.04</v>
+      </c>
+      <c r="O139" s="2">
+        <f t="shared" si="26"/>
+        <v>18.989999999999998</v>
+      </c>
+      <c r="P139" s="2">
+        <f t="shared" si="27"/>
+        <v>8.3100000000000023</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C140" s="4">
+        <v>391</v>
+      </c>
+      <c r="D140" s="4">
+        <v>58</v>
+      </c>
+      <c r="E140" s="4">
+        <v>33</v>
+      </c>
+      <c r="F140" s="4">
+        <v>449</v>
+      </c>
+      <c r="G140" s="4">
+        <v>61</v>
+      </c>
+      <c r="H140" s="4">
+        <v>237</v>
+      </c>
+      <c r="I140" s="4">
+        <v>93</v>
+      </c>
+      <c r="J140" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K140" s="2">
+        <f t="shared" si="22"/>
+        <v>87.08</v>
+      </c>
+      <c r="L140" s="2">
+        <f t="shared" si="23"/>
+        <v>12.92</v>
+      </c>
+      <c r="M140" s="2">
+        <f t="shared" si="24"/>
+        <v>52.78</v>
+      </c>
+      <c r="N140" s="2">
+        <f t="shared" si="25"/>
+        <v>13.59</v>
+      </c>
+      <c r="O140" s="2">
+        <f t="shared" si="26"/>
+        <v>20.71</v>
+      </c>
+      <c r="P140" s="2">
+        <f t="shared" si="27"/>
+        <v>12.920000000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C141" s="4">
+        <v>431</v>
+      </c>
+      <c r="D141" s="4">
+        <v>49</v>
+      </c>
+      <c r="E141" s="4">
+        <v>35</v>
+      </c>
+      <c r="F141" s="4">
+        <v>480</v>
+      </c>
+      <c r="G141" s="4">
+        <v>81</v>
+      </c>
+      <c r="H141" s="4">
+        <v>232</v>
+      </c>
+      <c r="I141" s="4">
+        <v>118</v>
+      </c>
+      <c r="J141" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K141" s="2">
+        <f t="shared" si="22"/>
+        <v>89.79</v>
+      </c>
+      <c r="L141" s="2">
+        <f t="shared" si="23"/>
+        <v>10.210000000000001</v>
+      </c>
+      <c r="M141" s="2">
+        <f t="shared" si="24"/>
+        <v>48.33</v>
+      </c>
+      <c r="N141" s="2">
+        <f t="shared" si="25"/>
+        <v>16.88</v>
+      </c>
+      <c r="O141" s="2">
+        <f t="shared" si="26"/>
+        <v>24.58</v>
+      </c>
+      <c r="P141" s="2">
+        <f t="shared" si="27"/>
+        <v>10.210000000000008</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C142" s="4">
+        <v>422</v>
+      </c>
+      <c r="D142" s="4">
+        <v>60</v>
+      </c>
+      <c r="E142" s="4">
+        <v>32</v>
+      </c>
+      <c r="F142" s="4">
+        <v>482</v>
+      </c>
+      <c r="G142" s="4">
+        <v>95</v>
+      </c>
+      <c r="H142" s="4">
+        <v>210</v>
+      </c>
+      <c r="I142" s="4">
+        <v>117</v>
+      </c>
+      <c r="J142" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K142" s="2">
+        <f t="shared" si="22"/>
+        <v>87.55</v>
+      </c>
+      <c r="L142" s="2">
+        <f t="shared" si="23"/>
+        <v>12.45</v>
+      </c>
+      <c r="M142" s="2">
+        <f t="shared" si="24"/>
+        <v>43.57</v>
+      </c>
+      <c r="N142" s="2">
+        <f t="shared" si="25"/>
+        <v>19.71</v>
+      </c>
+      <c r="O142" s="2">
+        <f t="shared" si="26"/>
+        <v>24.27</v>
+      </c>
+      <c r="P142" s="2">
+        <f t="shared" si="27"/>
+        <v>12.449999999999989</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A143" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C143" s="4">
+        <v>356</v>
+      </c>
+      <c r="D143" s="4">
+        <v>31</v>
+      </c>
+      <c r="E143" s="4">
+        <v>28</v>
+      </c>
+      <c r="F143" s="4">
+        <v>387</v>
+      </c>
+      <c r="G143" s="4">
+        <v>27</v>
+      </c>
+      <c r="H143" s="4">
+        <v>260</v>
+      </c>
+      <c r="I143" s="4">
+        <v>69</v>
+      </c>
+      <c r="J143" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K143" s="2">
+        <f t="shared" si="22"/>
+        <v>91.99</v>
+      </c>
+      <c r="L143" s="2">
+        <f t="shared" si="23"/>
+        <v>8.01</v>
+      </c>
+      <c r="M143" s="2">
+        <f t="shared" si="24"/>
+        <v>67.180000000000007</v>
+      </c>
+      <c r="N143" s="2">
+        <f t="shared" si="25"/>
+        <v>6.98</v>
+      </c>
+      <c r="O143" s="2">
+        <f t="shared" si="26"/>
+        <v>17.829999999999998</v>
+      </c>
+      <c r="P143" s="2">
+        <f t="shared" si="27"/>
+        <v>8.0099999999999909</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C144" s="4">
+        <v>436</v>
+      </c>
+      <c r="D144" s="4">
+        <v>12</v>
+      </c>
+      <c r="E144" s="4">
+        <v>1</v>
+      </c>
+      <c r="F144" s="4">
+        <v>448</v>
+      </c>
+      <c r="G144" t="s">
+        <v>16</v>
+      </c>
+      <c r="H144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144" t="s">
+        <v>16</v>
+      </c>
+      <c r="J144" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K144" s="2">
+        <f t="shared" si="22"/>
+        <v>97.32</v>
+      </c>
+      <c r="L144" s="2">
+        <f t="shared" si="23"/>
+        <v>2.68</v>
+      </c>
+      <c r="M144" s="2" t="e">
+        <f t="shared" si="24"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N144" s="2" t="e">
+        <f t="shared" si="25"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O144" s="2" t="e">
+        <f t="shared" si="26"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P144" s="2" t="e">
+        <f t="shared" si="27"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A145" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C145" s="4">
+        <v>139</v>
+      </c>
+      <c r="D145" s="4">
+        <v>19</v>
+      </c>
+      <c r="E145" s="4">
+        <v>7</v>
+      </c>
+      <c r="F145" s="4">
+        <v>158</v>
+      </c>
+      <c r="G145" t="s">
+        <v>16</v>
+      </c>
+      <c r="H145" t="s">
+        <v>16</v>
+      </c>
+      <c r="I145" t="s">
+        <v>16</v>
+      </c>
+      <c r="J145" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K145" s="2">
+        <f t="shared" si="22"/>
+        <v>87.97</v>
+      </c>
+      <c r="L145" s="2">
+        <f t="shared" si="23"/>
+        <v>12.03</v>
+      </c>
+      <c r="M145" s="2" t="e">
+        <f t="shared" si="24"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N145" s="2" t="e">
+        <f t="shared" si="25"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O145" s="2" t="e">
+        <f t="shared" si="26"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P145" s="2" t="e">
+        <f t="shared" si="27"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A146" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C146" s="4">
+        <v>426</v>
+      </c>
+      <c r="D146" s="4">
+        <v>39</v>
+      </c>
+      <c r="E146" s="4">
+        <v>34</v>
+      </c>
+      <c r="F146" s="4">
+        <v>465</v>
+      </c>
+      <c r="G146" s="4">
+        <v>81</v>
+      </c>
+      <c r="H146" s="4">
+        <v>259</v>
+      </c>
+      <c r="I146" s="4">
+        <v>86</v>
+      </c>
+      <c r="J146" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K146" s="2">
+        <f t="shared" si="22"/>
+        <v>91.61</v>
+      </c>
+      <c r="L146" s="2">
+        <f t="shared" si="23"/>
+        <v>8.39</v>
+      </c>
+      <c r="M146" s="2">
+        <f t="shared" si="24"/>
+        <v>55.7</v>
+      </c>
+      <c r="N146" s="2">
+        <f t="shared" si="25"/>
+        <v>17.420000000000002</v>
+      </c>
+      <c r="O146" s="2">
+        <f t="shared" si="26"/>
+        <v>18.489999999999998</v>
+      </c>
+      <c r="P146" s="2">
+        <f t="shared" si="27"/>
+        <v>8.39</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A147" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C147" s="4">
+        <v>337</v>
+      </c>
+      <c r="D147" s="4">
+        <v>40</v>
+      </c>
+      <c r="E147" s="4">
+        <v>29</v>
+      </c>
+      <c r="F147" s="4">
+        <v>377</v>
+      </c>
+      <c r="G147" s="4">
+        <v>76</v>
+      </c>
+      <c r="H147" s="4">
+        <v>184</v>
+      </c>
+      <c r="I147" s="4">
+        <v>77</v>
+      </c>
+      <c r="J147" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K147" s="2">
+        <f t="shared" si="22"/>
+        <v>89.39</v>
+      </c>
+      <c r="L147" s="2">
+        <f t="shared" si="23"/>
+        <v>10.61</v>
+      </c>
+      <c r="M147" s="2">
+        <f t="shared" si="24"/>
+        <v>48.81</v>
+      </c>
+      <c r="N147" s="2">
+        <f t="shared" si="25"/>
+        <v>20.16</v>
+      </c>
+      <c r="O147" s="2">
+        <f t="shared" si="26"/>
+        <v>20.420000000000002</v>
+      </c>
+      <c r="P147" s="2">
+        <f t="shared" si="27"/>
+        <v>10.61</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A148" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C148" s="4">
+        <v>379</v>
+      </c>
+      <c r="D148" s="4">
+        <v>36</v>
+      </c>
+      <c r="E148" s="4">
+        <v>26</v>
+      </c>
+      <c r="F148" s="4">
+        <v>415</v>
+      </c>
+      <c r="G148" s="4">
+        <v>100</v>
+      </c>
+      <c r="H148" s="4">
+        <v>173</v>
+      </c>
+      <c r="I148" s="4">
+        <v>106</v>
+      </c>
+      <c r="J148" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K148" s="2">
+        <f t="shared" si="22"/>
+        <v>91.33</v>
+      </c>
+      <c r="L148" s="2">
+        <f t="shared" si="23"/>
+        <v>8.67</v>
+      </c>
+      <c r="M148" s="2">
+        <f t="shared" si="24"/>
+        <v>41.69</v>
+      </c>
+      <c r="N148" s="2">
+        <f t="shared" si="25"/>
+        <v>24.1</v>
+      </c>
+      <c r="O148" s="2">
+        <f t="shared" si="26"/>
+        <v>25.54</v>
+      </c>
+      <c r="P148" s="2">
+        <f t="shared" si="27"/>
+        <v>8.6700000000000017</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A149" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C149" s="4">
+        <v>375</v>
+      </c>
+      <c r="D149" s="4">
+        <v>41</v>
+      </c>
+      <c r="E149" s="4">
+        <v>32</v>
+      </c>
+      <c r="F149" s="4">
+        <v>416</v>
+      </c>
+      <c r="G149" s="4">
+        <v>82</v>
+      </c>
+      <c r="H149" s="4">
+        <v>203</v>
+      </c>
+      <c r="I149" s="4">
+        <v>90</v>
+      </c>
+      <c r="J149" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K149" s="2">
+        <f t="shared" si="22"/>
+        <v>90.14</v>
+      </c>
+      <c r="L149" s="2">
+        <f t="shared" si="23"/>
+        <v>9.86</v>
+      </c>
+      <c r="M149" s="2">
+        <f t="shared" si="24"/>
+        <v>48.8</v>
+      </c>
+      <c r="N149" s="2">
+        <f t="shared" si="25"/>
+        <v>19.71</v>
+      </c>
+      <c r="O149" s="2">
+        <f t="shared" si="26"/>
+        <v>21.63</v>
+      </c>
+      <c r="P149" s="2">
+        <f t="shared" si="27"/>
+        <v>9.86</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C150" s="4">
+        <v>339</v>
+      </c>
+      <c r="D150" s="4">
+        <v>47</v>
+      </c>
+      <c r="E150" s="4">
+        <v>28</v>
+      </c>
+      <c r="F150" s="4">
+        <v>386</v>
+      </c>
+      <c r="G150" s="4">
+        <v>45</v>
+      </c>
+      <c r="H150" s="4">
+        <v>229</v>
+      </c>
+      <c r="I150" s="4">
+        <v>65</v>
+      </c>
+      <c r="J150" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K150" s="2">
+        <f t="shared" si="22"/>
+        <v>87.82</v>
+      </c>
+      <c r="L150" s="2">
+        <f t="shared" si="23"/>
+        <v>12.18</v>
+      </c>
+      <c r="M150" s="2">
+        <f t="shared" si="24"/>
+        <v>59.33</v>
+      </c>
+      <c r="N150" s="2">
+        <f t="shared" si="25"/>
+        <v>11.66</v>
+      </c>
+      <c r="O150" s="2">
+        <f t="shared" si="26"/>
+        <v>16.84</v>
+      </c>
+      <c r="P150" s="2">
+        <f t="shared" si="27"/>
+        <v>12.170000000000002</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A151" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C151" s="4">
+        <v>352</v>
+      </c>
+      <c r="D151" s="4">
+        <v>45</v>
+      </c>
+      <c r="E151" s="4">
+        <v>22</v>
+      </c>
+      <c r="F151" s="4">
+        <v>397</v>
+      </c>
+      <c r="G151" s="4">
+        <v>49</v>
+      </c>
+      <c r="H151" s="4">
+        <v>219</v>
+      </c>
+      <c r="I151" s="4">
+        <v>84</v>
+      </c>
+      <c r="J151" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K151" s="2">
+        <f t="shared" si="22"/>
+        <v>88.66</v>
+      </c>
+      <c r="L151" s="2">
+        <f t="shared" si="23"/>
+        <v>11.34</v>
+      </c>
+      <c r="M151" s="2">
+        <f t="shared" si="24"/>
+        <v>55.16</v>
+      </c>
+      <c r="N151" s="2">
+        <f t="shared" si="25"/>
+        <v>12.34</v>
+      </c>
+      <c r="O151" s="2">
+        <f t="shared" si="26"/>
+        <v>21.16</v>
+      </c>
+      <c r="P151" s="2">
+        <f t="shared" si="27"/>
+        <v>11.340000000000003</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C152" s="4">
+        <v>315</v>
+      </c>
+      <c r="D152" s="4">
+        <v>50</v>
+      </c>
+      <c r="E152" s="4">
+        <v>19</v>
+      </c>
+      <c r="F152" s="4">
+        <v>365</v>
+      </c>
+      <c r="G152" s="4">
+        <v>30</v>
+      </c>
+      <c r="H152" s="4">
+        <v>207</v>
+      </c>
+      <c r="I152" s="4">
+        <v>78</v>
+      </c>
+      <c r="J152" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K152" s="2">
+        <f t="shared" si="22"/>
+        <v>86.3</v>
+      </c>
+      <c r="L152" s="2">
+        <f t="shared" si="23"/>
+        <v>13.7</v>
+      </c>
+      <c r="M152" s="2">
+        <f t="shared" si="24"/>
+        <v>56.71</v>
+      </c>
+      <c r="N152" s="2">
+        <f t="shared" si="25"/>
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="O152" s="2">
+        <f t="shared" si="26"/>
+        <v>21.37</v>
+      </c>
+      <c r="P152" s="2">
+        <f t="shared" si="27"/>
+        <v>13.699999999999989</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C153" s="4">
+        <v>323</v>
+      </c>
+      <c r="D153" s="4">
+        <v>51</v>
+      </c>
+      <c r="E153" s="4">
+        <v>27</v>
+      </c>
+      <c r="F153" s="4">
+        <v>374</v>
+      </c>
+      <c r="G153" s="4">
+        <v>59</v>
+      </c>
+      <c r="H153" s="4">
+        <v>156</v>
+      </c>
+      <c r="I153" s="4">
+        <v>108</v>
+      </c>
+      <c r="J153" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K153" s="2">
+        <f t="shared" si="22"/>
+        <v>86.36</v>
+      </c>
+      <c r="L153" s="2">
+        <f t="shared" si="23"/>
+        <v>13.64</v>
+      </c>
+      <c r="M153" s="2">
+        <f t="shared" si="24"/>
+        <v>41.71</v>
+      </c>
+      <c r="N153" s="2">
+        <f t="shared" si="25"/>
+        <v>15.78</v>
+      </c>
+      <c r="O153" s="2">
+        <f t="shared" si="26"/>
+        <v>28.88</v>
+      </c>
+      <c r="P153" s="2">
+        <f t="shared" si="27"/>
+        <v>13.629999999999995</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C154" s="4">
+        <v>405</v>
+      </c>
+      <c r="D154" s="4">
+        <v>44</v>
+      </c>
+      <c r="E154" s="4">
+        <v>30</v>
+      </c>
+      <c r="F154" s="4">
+        <v>449</v>
+      </c>
+      <c r="G154" s="4">
+        <v>90</v>
+      </c>
+      <c r="H154" s="4">
+        <v>220</v>
+      </c>
+      <c r="I154" s="4">
+        <v>95</v>
+      </c>
+      <c r="J154" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K154" s="2">
+        <f t="shared" si="22"/>
+        <v>90.2</v>
+      </c>
+      <c r="L154" s="2">
+        <f t="shared" si="23"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M154" s="2">
+        <f t="shared" si="24"/>
+        <v>49</v>
+      </c>
+      <c r="N154" s="2">
+        <f t="shared" si="25"/>
+        <v>20.04</v>
+      </c>
+      <c r="O154" s="2">
+        <f t="shared" si="26"/>
+        <v>21.16</v>
+      </c>
+      <c r="P154" s="2">
+        <f t="shared" si="27"/>
+        <v>9.7999999999999972</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C155" s="4">
+        <v>437</v>
+      </c>
+      <c r="D155" s="4">
+        <v>52</v>
+      </c>
+      <c r="E155" s="4">
+        <v>37</v>
+      </c>
+      <c r="F155" s="4">
+        <v>489</v>
+      </c>
+      <c r="G155" s="4">
+        <v>82</v>
+      </c>
+      <c r="H155" s="4">
+        <v>255</v>
+      </c>
+      <c r="I155" s="4">
+        <v>100</v>
+      </c>
+      <c r="J155" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K155" s="2">
+        <f t="shared" si="22"/>
+        <v>89.37</v>
+      </c>
+      <c r="L155" s="2">
+        <f t="shared" si="23"/>
+        <v>10.63</v>
+      </c>
+      <c r="M155" s="2">
+        <f t="shared" si="24"/>
+        <v>52.15</v>
+      </c>
+      <c r="N155" s="2">
+        <f t="shared" si="25"/>
+        <v>16.77</v>
+      </c>
+      <c r="O155" s="2">
+        <f t="shared" si="26"/>
+        <v>20.45</v>
+      </c>
+      <c r="P155" s="2">
+        <f t="shared" si="27"/>
+        <v>10.629999999999995</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C156" s="4">
+        <v>291</v>
+      </c>
+      <c r="D156" s="4">
+        <v>55</v>
+      </c>
+      <c r="E156" s="4">
+        <v>18</v>
+      </c>
+      <c r="F156" s="4">
+        <v>346</v>
+      </c>
+      <c r="G156" s="4">
+        <v>30</v>
+      </c>
+      <c r="H156" s="4">
+        <v>179</v>
+      </c>
+      <c r="I156" s="4">
+        <v>82</v>
+      </c>
+      <c r="J156" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K156" s="2">
+        <f t="shared" si="22"/>
+        <v>84.1</v>
+      </c>
+      <c r="L156" s="2">
+        <f t="shared" si="23"/>
+        <v>15.9</v>
+      </c>
+      <c r="M156" s="2">
+        <f t="shared" si="24"/>
+        <v>51.73</v>
+      </c>
+      <c r="N156" s="2">
+        <f t="shared" si="25"/>
+        <v>8.67</v>
+      </c>
+      <c r="O156" s="2">
+        <f t="shared" si="26"/>
+        <v>23.7</v>
+      </c>
+      <c r="P156" s="2">
+        <f t="shared" si="27"/>
+        <v>15.900000000000006</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C157" s="4">
+        <v>371</v>
+      </c>
+      <c r="D157" s="4">
+        <v>58</v>
+      </c>
+      <c r="E157" s="4">
+        <v>32</v>
+      </c>
+      <c r="F157" s="4">
+        <v>429</v>
+      </c>
+      <c r="G157" s="4">
+        <v>42</v>
+      </c>
+      <c r="H157" s="4">
+        <v>242</v>
+      </c>
+      <c r="I157" s="4">
+        <v>87</v>
+      </c>
+      <c r="J157" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K157" s="2">
+        <f t="shared" si="22"/>
+        <v>86.48</v>
+      </c>
+      <c r="L157" s="2">
+        <f t="shared" si="23"/>
+        <v>13.52</v>
+      </c>
+      <c r="M157" s="2">
+        <f t="shared" si="24"/>
+        <v>56.41</v>
+      </c>
+      <c r="N157" s="2">
+        <f t="shared" si="25"/>
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="O157" s="2">
+        <f t="shared" si="26"/>
+        <v>20.28</v>
+      </c>
+      <c r="P157" s="2">
+        <f t="shared" si="27"/>
+        <v>13.52000000000001</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C158" s="4">
+        <v>371</v>
+      </c>
+      <c r="D158" s="4">
+        <v>46</v>
+      </c>
+      <c r="E158" s="4">
+        <v>27</v>
+      </c>
+      <c r="F158" s="4">
+        <v>417</v>
+      </c>
+      <c r="G158" s="4">
+        <v>65</v>
+      </c>
+      <c r="H158" s="4">
+        <v>193</v>
+      </c>
+      <c r="I158" s="4">
+        <v>113</v>
+      </c>
+      <c r="J158" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K158" s="2">
+        <f t="shared" si="22"/>
+        <v>88.97</v>
+      </c>
+      <c r="L158" s="2">
+        <f t="shared" si="23"/>
+        <v>11.03</v>
+      </c>
+      <c r="M158" s="2">
+        <f t="shared" si="24"/>
+        <v>46.28</v>
+      </c>
+      <c r="N158" s="2">
+        <f t="shared" si="25"/>
+        <v>15.59</v>
+      </c>
+      <c r="O158" s="2">
+        <f t="shared" si="26"/>
+        <v>27.1</v>
+      </c>
+      <c r="P158" s="2">
+        <f t="shared" si="27"/>
+        <v>11.030000000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C159" s="4">
+        <v>363</v>
+      </c>
+      <c r="D159" s="4">
+        <v>49</v>
+      </c>
+      <c r="E159" s="4">
+        <v>31</v>
+      </c>
+      <c r="F159" s="4">
+        <v>412</v>
+      </c>
+      <c r="G159" s="4">
+        <v>72</v>
+      </c>
+      <c r="H159" s="4">
+        <v>211</v>
+      </c>
+      <c r="I159" s="4">
+        <v>80</v>
+      </c>
+      <c r="J159" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K159" s="2">
+        <f t="shared" si="22"/>
+        <v>88.11</v>
+      </c>
+      <c r="L159" s="2">
+        <f t="shared" si="23"/>
+        <v>11.89</v>
+      </c>
+      <c r="M159" s="2">
+        <f t="shared" si="24"/>
+        <v>51.21</v>
+      </c>
+      <c r="N159" s="2">
+        <f t="shared" si="25"/>
+        <v>17.48</v>
+      </c>
+      <c r="O159" s="2">
+        <f t="shared" si="26"/>
+        <v>19.420000000000002</v>
+      </c>
+      <c r="P159" s="2">
+        <f t="shared" si="27"/>
+        <v>11.889999999999986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating TotalSleep file for March 2018
</commit_message>
<xml_diff>
--- a/datasets/TotalSleep.xlsx
+++ b/datasets/TotalSleep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23C1625-E038-4A8D-AB16-ADB67FD9D8F5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9C12E5-D228-40B1-AD7D-BC5A499AE7A1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>Start Time</t>
   </si>
@@ -70,9 +70,6 @@
     <t>% Unclassified</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>01-02-2018 9:53 pm</t>
   </si>
   <si>
@@ -109,12 +106,6 @@
     <t>07-02-2018 2:04 am</t>
   </si>
   <si>
-    <t>07-02-2018 4:18 am</t>
-  </si>
-  <si>
-    <t>07-02-2018 6:01 am</t>
-  </si>
-  <si>
     <t>07-02-2018 9:08 pm</t>
   </si>
   <si>
@@ -145,18 +136,6 @@
     <t>12-02-2018 3:54 am</t>
   </si>
   <si>
-    <t>12-02-2018 9:30 pm</t>
-  </si>
-  <si>
-    <t>13-02-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>14-02-2018 2:00 am</t>
-  </si>
-  <si>
-    <t>14-02-2018 4:38 am</t>
-  </si>
-  <si>
     <t>14-02-2018 9:13 pm</t>
   </si>
   <si>
@@ -241,16 +220,178 @@
     <t>28-02-2018 4:58 am</t>
   </si>
   <si>
-    <t>31-01-2018 9:53 pm</t>
-  </si>
-  <si>
-    <t>01-02-2018 2:33 am</t>
-  </si>
-  <si>
-    <t>01-02-2018 2:44 pm</t>
-  </si>
-  <si>
-    <t>01-02-2018 4:12 pm</t>
+    <t>28-02-2018 10:06 pm</t>
+  </si>
+  <si>
+    <t>01-03-2018 5:04 am</t>
+  </si>
+  <si>
+    <t>01-03-2018 10:04 pm</t>
+  </si>
+  <si>
+    <t>02-03-2018 5:02 am</t>
+  </si>
+  <si>
+    <t>02-03-2018 11:45 pm</t>
+  </si>
+  <si>
+    <t>03-03-2018 6:05 am</t>
+  </si>
+  <si>
+    <t>03-03-2018 9:11 pm</t>
+  </si>
+  <si>
+    <t>04-03-2018 5:29 am</t>
+  </si>
+  <si>
+    <t>04-03-2018 10:25 pm</t>
+  </si>
+  <si>
+    <t>05-03-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>05-03-2018 9:43 pm</t>
+  </si>
+  <si>
+    <t>06-03-2018 5:00 am</t>
+  </si>
+  <si>
+    <t>06-03-2018 9:54 pm</t>
+  </si>
+  <si>
+    <t>07-03-2018 4:59 am</t>
+  </si>
+  <si>
+    <t>07-03-2018 9:59 pm</t>
+  </si>
+  <si>
+    <t>08-03-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>08-03-2018 9:48 pm</t>
+  </si>
+  <si>
+    <t>09-03-2018 4:59 am</t>
+  </si>
+  <si>
+    <t>09-03-2018 10:46 pm</t>
+  </si>
+  <si>
+    <t>10-03-2018 7:57 am</t>
+  </si>
+  <si>
+    <t>10-03-2018 9:47 pm</t>
+  </si>
+  <si>
+    <t>11-03-2018 6:20 am</t>
+  </si>
+  <si>
+    <t>11-03-2018 9:11 pm</t>
+  </si>
+  <si>
+    <t>12-03-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>12-03-2018 9:40 pm</t>
+  </si>
+  <si>
+    <t>13-03-2018 5:01 am</t>
+  </si>
+  <si>
+    <t>13-03-2018 10:07 pm</t>
+  </si>
+  <si>
+    <t>14-03-2018 5:05 am</t>
+  </si>
+  <si>
+    <t>14-03-2018 9:10 pm</t>
+  </si>
+  <si>
+    <t>15-03-2018 4:33 am</t>
+  </si>
+  <si>
+    <t>15-03-2018 9:20 pm</t>
+  </si>
+  <si>
+    <t>16-03-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>16-03-2018 9:34 pm</t>
+  </si>
+  <si>
+    <t>17-03-2018 5:57 am</t>
+  </si>
+  <si>
+    <t>17-03-2018 10:02 pm</t>
+  </si>
+  <si>
+    <t>18-03-2018 5:39 am</t>
+  </si>
+  <si>
+    <t>18-03-2018 9:35 pm</t>
+  </si>
+  <si>
+    <t>19-03-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>19-03-2018 10:11 pm</t>
+  </si>
+  <si>
+    <t>20-03-2018 4:26 am</t>
+  </si>
+  <si>
+    <t>20-03-2018 9:45 pm</t>
+  </si>
+  <si>
+    <t>21-03-2018 5:03 am</t>
+  </si>
+  <si>
+    <t>21-03-2018 10:08 pm</t>
+  </si>
+  <si>
+    <t>22-03-2018 4:36 am</t>
+  </si>
+  <si>
+    <t>22-03-2018 10:44 pm</t>
+  </si>
+  <si>
+    <t>23-03-2018 4:54 am</t>
+  </si>
+  <si>
+    <t>24-03-2018 9:16 pm</t>
+  </si>
+  <si>
+    <t>25-03-2018 6:20 am</t>
+  </si>
+  <si>
+    <t>25-03-2018 10:59 pm</t>
+  </si>
+  <si>
+    <t>26-03-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>27-03-2018 10:18 pm</t>
+  </si>
+  <si>
+    <t>28-03-2018 4:44 am</t>
+  </si>
+  <si>
+    <t>28-03-2018 10:30 pm</t>
+  </si>
+  <si>
+    <t>29-03-2018 4:47 am</t>
+  </si>
+  <si>
+    <t>29-03-2018 10:49 pm</t>
+  </si>
+  <si>
+    <t>30-03-2018 5:05 am</t>
+  </si>
+  <si>
+    <t>30-03-2018 9:56 pm</t>
+  </si>
+  <si>
+    <t>31-03-2018 5:23 am</t>
   </si>
 </sst>
 </file>
@@ -1102,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P159"/>
+  <dimension ref="A1:P182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P129" sqref="P129:P159"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G119" sqref="A119:XFD119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4853,31 +4994,31 @@
         <v>86</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ref="J66:J130" si="14">IF(C66&gt;=420,"Yes","No")</f>
+        <f t="shared" ref="J66:J128" si="14">IF(C66&gt;=420,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="K66" s="2">
-        <f t="shared" ref="K66:K130" si="15">ROUND((C66/F66)*100, 2)</f>
+        <f t="shared" ref="K66:K128" si="15">ROUND((C66/F66)*100, 2)</f>
         <v>88.02</v>
       </c>
       <c r="L66" s="2">
-        <f t="shared" ref="L66:L130" si="16">ROUND((D66/F66)*100,2)</f>
+        <f t="shared" ref="L66:L128" si="16">ROUND((D66/F66)*100,2)</f>
         <v>11.98</v>
       </c>
       <c r="M66" s="2">
-        <f t="shared" ref="M66:M130" si="17">ROUND((H66/F66)*100,2)</f>
+        <f t="shared" ref="M66:M128" si="17">ROUND((H66/F66)*100,2)</f>
         <v>50</v>
       </c>
       <c r="N66" s="2">
-        <f t="shared" ref="N66:N130" si="18">ROUND((G66/F66)*100,2)</f>
+        <f t="shared" ref="N66:N128" si="18">ROUND((G66/F66)*100,2)</f>
         <v>18.2</v>
       </c>
       <c r="O66" s="2">
-        <f t="shared" ref="O66:O130" si="19">ROUND((I66/F66)*100,2)</f>
+        <f t="shared" ref="O66:O128" si="19">ROUND((I66/F66)*100,2)</f>
         <v>19.82</v>
       </c>
       <c r="P66" s="2">
-        <f t="shared" ref="P66:P130" si="20">100-(O66+N66+M66)</f>
+        <f t="shared" ref="P66:P128" si="20">100-(O66+N66+M66)</f>
         <v>11.980000000000004</v>
       </c>
     </row>
@@ -7847,145 +7988,145 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
-        <v>43118.894444444442</v>
+        <v>43119.897222222222</v>
       </c>
       <c r="B119" s="1">
-        <v>43119.197222222225</v>
+        <v>43120.26666666667</v>
       </c>
       <c r="C119" s="3">
-        <v>407</v>
+        <v>455</v>
       </c>
       <c r="D119" s="3">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E119" s="3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F119" s="3">
-        <v>436</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I119" s="3" t="s">
-        <v>16</v>
+        <v>532</v>
+      </c>
+      <c r="G119" s="3">
+        <v>66</v>
+      </c>
+      <c r="H119" s="3">
+        <v>265</v>
+      </c>
+      <c r="I119" s="3">
+        <v>124</v>
       </c>
       <c r="J119" t="str">
         <f t="shared" si="14"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="K119" s="2">
         <f t="shared" si="15"/>
-        <v>93.35</v>
+        <v>85.53</v>
       </c>
       <c r="L119" s="2">
         <f t="shared" si="16"/>
-        <v>5.5</v>
-      </c>
-      <c r="M119" s="2" t="e">
+        <v>14.47</v>
+      </c>
+      <c r="M119" s="2">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N119" s="2" t="e">
+        <v>49.81</v>
+      </c>
+      <c r="N119" s="2">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O119" s="2" t="e">
+        <v>12.41</v>
+      </c>
+      <c r="O119" s="2">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P119" s="2" t="e">
+        <v>23.31</v>
+      </c>
+      <c r="P119" s="2">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <v>14.469999999999999</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
-        <v>43119.897222222222</v>
+        <v>43120.92291666667</v>
       </c>
       <c r="B120" s="1">
-        <v>43120.26666666667</v>
+        <v>43121.251388888886</v>
       </c>
       <c r="C120" s="3">
-        <v>455</v>
+        <v>416</v>
       </c>
       <c r="D120" s="3">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E120" s="3">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F120" s="3">
-        <v>532</v>
+        <v>473</v>
       </c>
       <c r="G120" s="3">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="H120" s="3">
-        <v>265</v>
+        <v>231</v>
       </c>
       <c r="I120" s="3">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="J120" t="str">
         <f t="shared" si="14"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="K120" s="2">
         <f t="shared" si="15"/>
-        <v>85.53</v>
+        <v>87.95</v>
       </c>
       <c r="L120" s="2">
         <f t="shared" si="16"/>
-        <v>14.47</v>
+        <v>12.05</v>
       </c>
       <c r="M120" s="2">
         <f t="shared" si="17"/>
-        <v>49.81</v>
+        <v>48.84</v>
       </c>
       <c r="N120" s="2">
         <f t="shared" si="18"/>
-        <v>12.41</v>
+        <v>16.7</v>
       </c>
       <c r="O120" s="2">
         <f t="shared" si="19"/>
-        <v>23.31</v>
+        <v>22.41</v>
       </c>
       <c r="P120" s="2">
         <f t="shared" si="20"/>
-        <v>14.469999999999999</v>
+        <v>12.049999999999997</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
-        <v>43120.92291666667</v>
+        <v>43121.89166666667</v>
       </c>
       <c r="B121" s="1">
-        <v>43121.251388888886</v>
+        <v>43122.210416666669</v>
       </c>
       <c r="C121" s="3">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="D121" s="3">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E121" s="3">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F121" s="3">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="G121" s="3">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="H121" s="3">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="I121" s="3">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J121" t="str">
         <f t="shared" si="14"/>
@@ -7993,56 +8134,56 @@
       </c>
       <c r="K121" s="2">
         <f t="shared" si="15"/>
-        <v>87.95</v>
+        <v>86.71</v>
       </c>
       <c r="L121" s="2">
         <f t="shared" si="16"/>
-        <v>12.05</v>
+        <v>13.29</v>
       </c>
       <c r="M121" s="2">
         <f t="shared" si="17"/>
-        <v>48.84</v>
+        <v>54.68</v>
       </c>
       <c r="N121" s="2">
         <f t="shared" si="18"/>
-        <v>16.7</v>
+        <v>10.24</v>
       </c>
       <c r="O121" s="2">
         <f t="shared" si="19"/>
-        <v>22.41</v>
+        <v>21.79</v>
       </c>
       <c r="P121" s="2">
         <f t="shared" si="20"/>
-        <v>12.049999999999997</v>
+        <v>13.289999999999992</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
-        <v>43121.89166666667</v>
+        <v>43122.900694444441</v>
       </c>
       <c r="B122" s="1">
-        <v>43122.210416666669</v>
+        <v>43123.222916666666</v>
       </c>
       <c r="C122" s="3">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="D122" s="3">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E122" s="3">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F122" s="3">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="G122" s="3">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="H122" s="3">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="I122" s="3">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J122" t="str">
         <f t="shared" si="14"/>
@@ -8050,56 +8191,56 @@
       </c>
       <c r="K122" s="2">
         <f t="shared" si="15"/>
-        <v>86.71</v>
+        <v>88.79</v>
       </c>
       <c r="L122" s="2">
         <f t="shared" si="16"/>
-        <v>13.29</v>
+        <v>11.21</v>
       </c>
       <c r="M122" s="2">
         <f t="shared" si="17"/>
-        <v>54.68</v>
+        <v>52.37</v>
       </c>
       <c r="N122" s="2">
         <f t="shared" si="18"/>
-        <v>10.24</v>
+        <v>15.09</v>
       </c>
       <c r="O122" s="2">
         <f t="shared" si="19"/>
-        <v>21.79</v>
+        <v>21.34</v>
       </c>
       <c r="P122" s="2">
         <f t="shared" si="20"/>
-        <v>13.289999999999992</v>
+        <v>11.200000000000003</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
-        <v>43122.900694444441</v>
+        <v>43123.909722222219</v>
       </c>
       <c r="B123" s="1">
-        <v>43123.222916666666</v>
+        <v>43124.254861111112</v>
       </c>
       <c r="C123" s="3">
-        <v>412</v>
+        <v>390</v>
       </c>
       <c r="D123" s="3">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="E123" s="3">
         <v>23</v>
       </c>
       <c r="F123" s="3">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="G123" s="3">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="H123" s="3">
-        <v>243</v>
+        <v>282</v>
       </c>
       <c r="I123" s="3">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="J123" t="str">
         <f t="shared" si="14"/>
@@ -8107,113 +8248,113 @@
       </c>
       <c r="K123" s="2">
         <f t="shared" si="15"/>
-        <v>88.79</v>
+        <v>78.47</v>
       </c>
       <c r="L123" s="2">
         <f t="shared" si="16"/>
-        <v>11.21</v>
+        <v>21.53</v>
       </c>
       <c r="M123" s="2">
         <f t="shared" si="17"/>
-        <v>52.37</v>
+        <v>56.74</v>
       </c>
       <c r="N123" s="2">
         <f t="shared" si="18"/>
-        <v>15.09</v>
+        <v>9.66</v>
       </c>
       <c r="O123" s="2">
         <f t="shared" si="19"/>
-        <v>21.34</v>
+        <v>12.07</v>
       </c>
       <c r="P123" s="2">
         <f t="shared" si="20"/>
-        <v>11.200000000000003</v>
+        <v>21.53</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
-        <v>43123.909722222219</v>
+        <v>43124.738194444442</v>
       </c>
       <c r="B124" s="1">
-        <v>43124.254861111112</v>
+        <v>43125.15</v>
       </c>
       <c r="C124" s="3">
-        <v>390</v>
+        <v>511</v>
       </c>
       <c r="D124" s="3">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E124" s="3">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F124" s="3">
-        <v>497</v>
+        <v>593</v>
       </c>
       <c r="G124" s="3">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="H124" s="3">
-        <v>282</v>
+        <v>407</v>
       </c>
       <c r="I124" s="3">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="J124" t="str">
         <f t="shared" si="14"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="K124" s="2">
         <f t="shared" si="15"/>
-        <v>78.47</v>
+        <v>86.17</v>
       </c>
       <c r="L124" s="2">
         <f t="shared" si="16"/>
-        <v>21.53</v>
+        <v>13.83</v>
       </c>
       <c r="M124" s="2">
         <f t="shared" si="17"/>
-        <v>56.74</v>
+        <v>68.63</v>
       </c>
       <c r="N124" s="2">
         <f t="shared" si="18"/>
-        <v>9.66</v>
+        <v>5.56</v>
       </c>
       <c r="O124" s="2">
         <f t="shared" si="19"/>
-        <v>12.07</v>
+        <v>11.97</v>
       </c>
       <c r="P124" s="2">
         <f t="shared" si="20"/>
-        <v>21.53</v>
+        <v>13.840000000000003</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
-        <v>43124.738194444442</v>
+        <v>43125.880555555559</v>
       </c>
       <c r="B125" s="1">
-        <v>43125.15</v>
+        <v>43126.218055555553</v>
       </c>
       <c r="C125" s="3">
-        <v>511</v>
+        <v>434</v>
       </c>
       <c r="D125" s="3">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E125" s="3">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F125" s="3">
-        <v>593</v>
+        <v>486</v>
       </c>
       <c r="G125" s="3">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="H125" s="3">
-        <v>407</v>
+        <v>249</v>
       </c>
       <c r="I125" s="3">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="J125" t="str">
         <f t="shared" si="14"/>
@@ -8221,113 +8362,113 @@
       </c>
       <c r="K125" s="2">
         <f t="shared" si="15"/>
-        <v>86.17</v>
+        <v>89.3</v>
       </c>
       <c r="L125" s="2">
         <f t="shared" si="16"/>
-        <v>13.83</v>
+        <v>10.7</v>
       </c>
       <c r="M125" s="2">
         <f t="shared" si="17"/>
-        <v>68.63</v>
+        <v>51.23</v>
       </c>
       <c r="N125" s="2">
         <f t="shared" si="18"/>
-        <v>5.56</v>
+        <v>20.16</v>
       </c>
       <c r="O125" s="2">
         <f t="shared" si="19"/>
-        <v>11.97</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="P125" s="2">
         <f t="shared" si="20"/>
-        <v>13.840000000000003</v>
+        <v>10.710000000000008</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
-        <v>43125.880555555559</v>
+        <v>43126.9375</v>
       </c>
       <c r="B126" s="1">
-        <v>43126.218055555553</v>
+        <v>43127.179861111108</v>
       </c>
       <c r="C126" s="3">
-        <v>434</v>
+        <v>302</v>
       </c>
       <c r="D126" s="3">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E126" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F126" s="3">
-        <v>486</v>
+        <v>349</v>
       </c>
       <c r="G126" s="3">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="H126" s="3">
-        <v>249</v>
+        <v>178</v>
       </c>
       <c r="I126" s="3">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J126" t="str">
         <f t="shared" si="14"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="K126" s="2">
         <f t="shared" si="15"/>
-        <v>89.3</v>
+        <v>86.53</v>
       </c>
       <c r="L126" s="2">
         <f t="shared" si="16"/>
-        <v>10.7</v>
+        <v>13.47</v>
       </c>
       <c r="M126" s="2">
         <f t="shared" si="17"/>
-        <v>51.23</v>
+        <v>51</v>
       </c>
       <c r="N126" s="2">
         <f t="shared" si="18"/>
-        <v>20.16</v>
+        <v>13.75</v>
       </c>
       <c r="O126" s="2">
         <f t="shared" si="19"/>
-        <v>17.899999999999999</v>
+        <v>21.78</v>
       </c>
       <c r="P126" s="2">
         <f t="shared" si="20"/>
-        <v>10.710000000000008</v>
+        <v>13.469999999999999</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
-        <v>43126.9375</v>
+        <v>43127.894444444442</v>
       </c>
       <c r="B127" s="1">
-        <v>43127.179861111108</v>
+        <v>43128.19027777778</v>
       </c>
       <c r="C127" s="3">
-        <v>302</v>
+        <v>359</v>
       </c>
       <c r="D127" s="3">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="E127" s="3">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F127" s="3">
-        <v>349</v>
+        <v>426</v>
       </c>
       <c r="G127" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H127" s="3">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="I127" s="3">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="J127" t="str">
         <f t="shared" si="14"/>
@@ -8335,56 +8476,56 @@
       </c>
       <c r="K127" s="2">
         <f t="shared" si="15"/>
-        <v>86.53</v>
+        <v>84.27</v>
       </c>
       <c r="L127" s="2">
         <f t="shared" si="16"/>
-        <v>13.47</v>
+        <v>15.73</v>
       </c>
       <c r="M127" s="2">
         <f t="shared" si="17"/>
-        <v>51</v>
+        <v>50.23</v>
       </c>
       <c r="N127" s="2">
         <f t="shared" si="18"/>
-        <v>13.75</v>
+        <v>11.74</v>
       </c>
       <c r="O127" s="2">
         <f t="shared" si="19"/>
-        <v>21.78</v>
+        <v>22.3</v>
       </c>
       <c r="P127" s="2">
         <f t="shared" si="20"/>
-        <v>13.469999999999999</v>
+        <v>15.730000000000004</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
-        <v>43127.894444444442</v>
+        <v>43130.906944444447</v>
       </c>
       <c r="B128" s="1">
-        <v>43128.19027777778</v>
+        <v>43131.154166666667</v>
       </c>
       <c r="C128" s="3">
-        <v>359</v>
+        <v>312</v>
       </c>
       <c r="D128" s="3">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="E128" s="3">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F128" s="3">
-        <v>426</v>
+        <v>356</v>
       </c>
       <c r="G128" s="3">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H128" s="3">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="I128" s="3">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="J128" t="str">
         <f t="shared" si="14"/>
@@ -8392,227 +8533,227 @@
       </c>
       <c r="K128" s="2">
         <f t="shared" si="15"/>
-        <v>84.27</v>
+        <v>87.64</v>
       </c>
       <c r="L128" s="2">
         <f t="shared" si="16"/>
-        <v>15.73</v>
+        <v>12.36</v>
       </c>
       <c r="M128" s="2">
         <f t="shared" si="17"/>
-        <v>50.23</v>
+        <v>56.18</v>
       </c>
       <c r="N128" s="2">
         <f t="shared" si="18"/>
-        <v>11.74</v>
+        <v>15.73</v>
       </c>
       <c r="O128" s="2">
         <f t="shared" si="19"/>
-        <v>22.3</v>
+        <v>15.73</v>
       </c>
       <c r="P128" s="2">
         <f t="shared" si="20"/>
-        <v>15.730000000000004</v>
+        <v>12.36</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A129" s="1">
-        <v>43130.906944444447</v>
-      </c>
-      <c r="B129" s="1">
-        <v>43131.154166666667</v>
-      </c>
-      <c r="C129" s="3">
-        <v>312</v>
-      </c>
-      <c r="D129" s="3">
-        <v>44</v>
-      </c>
-      <c r="E129" s="3">
-        <v>19</v>
-      </c>
-      <c r="F129" s="3">
-        <v>356</v>
-      </c>
-      <c r="G129" s="3">
+      <c r="A129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" s="4">
+        <v>353</v>
+      </c>
+      <c r="D129" s="4">
         <v>56</v>
       </c>
-      <c r="H129" s="3">
-        <v>200</v>
-      </c>
-      <c r="I129" s="3">
-        <v>56</v>
+      <c r="E129" s="4">
+        <v>21</v>
+      </c>
+      <c r="F129" s="4">
+        <v>409</v>
+      </c>
+      <c r="G129" s="4">
+        <v>54</v>
+      </c>
+      <c r="H129" s="4">
+        <v>204</v>
+      </c>
+      <c r="I129" s="4">
+        <v>95</v>
       </c>
       <c r="J129" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="J129:J182" si="21">IF(C129&gt;=420,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="K129" s="2">
-        <f t="shared" si="15"/>
-        <v>87.64</v>
+        <f t="shared" ref="K129:K182" si="22">ROUND((C129/F129)*100, 2)</f>
+        <v>86.31</v>
       </c>
       <c r="L129" s="2">
-        <f t="shared" si="16"/>
-        <v>12.36</v>
+        <f t="shared" ref="L129:L182" si="23">ROUND((D129/F129)*100,2)</f>
+        <v>13.69</v>
       </c>
       <c r="M129" s="2">
-        <f t="shared" si="17"/>
-        <v>56.18</v>
+        <f t="shared" ref="M129:M182" si="24">ROUND((H129/F129)*100,2)</f>
+        <v>49.88</v>
       </c>
       <c r="N129" s="2">
-        <f t="shared" si="18"/>
-        <v>15.73</v>
+        <f t="shared" ref="N129:N182" si="25">ROUND((G129/F129)*100,2)</f>
+        <v>13.2</v>
       </c>
       <c r="O129" s="2">
-        <f t="shared" si="19"/>
-        <v>15.73</v>
+        <f t="shared" ref="O129:O182" si="26">ROUND((I129/F129)*100,2)</f>
+        <v>23.23</v>
       </c>
       <c r="P129" s="2">
-        <f t="shared" si="20"/>
-        <v>12.36</v>
+        <f t="shared" ref="P129:P182" si="27">100-(O129+N129+M129)</f>
+        <v>13.689999999999998</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C130" s="4">
+        <v>358</v>
+      </c>
+      <c r="D130" s="4">
+        <v>47</v>
+      </c>
+      <c r="E130" s="4">
+        <v>27</v>
+      </c>
+      <c r="F130" s="4">
+        <v>405</v>
+      </c>
+      <c r="G130" s="4">
+        <v>61</v>
+      </c>
+      <c r="H130" s="4">
+        <v>224</v>
+      </c>
+      <c r="I130" s="4">
         <v>73</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C130" s="4">
-        <v>269</v>
-      </c>
-      <c r="D130" s="4">
-        <v>3</v>
-      </c>
-      <c r="E130" s="4">
-        <v>1</v>
-      </c>
-      <c r="F130" s="4">
-        <v>280</v>
-      </c>
-      <c r="G130" t="s">
-        <v>16</v>
-      </c>
-      <c r="H130" t="s">
-        <v>16</v>
-      </c>
-      <c r="I130" t="s">
-        <v>16</v>
-      </c>
       <c r="J130" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>No</v>
       </c>
       <c r="K130" s="2">
-        <f t="shared" si="15"/>
-        <v>96.07</v>
+        <f t="shared" si="22"/>
+        <v>88.4</v>
       </c>
       <c r="L130" s="2">
-        <f t="shared" si="16"/>
-        <v>1.07</v>
-      </c>
-      <c r="M130" s="2" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N130" s="2" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O130" s="2" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P130" s="2" t="e">
-        <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <f t="shared" si="23"/>
+        <v>11.6</v>
+      </c>
+      <c r="M130" s="2">
+        <f t="shared" si="24"/>
+        <v>55.31</v>
+      </c>
+      <c r="N130" s="2">
+        <f t="shared" si="25"/>
+        <v>15.06</v>
+      </c>
+      <c r="O130" s="2">
+        <f t="shared" si="26"/>
+        <v>18.02</v>
+      </c>
+      <c r="P130" s="2">
+        <f t="shared" si="27"/>
+        <v>11.61</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="C131" s="4">
-        <v>83</v>
+        <v>309</v>
       </c>
       <c r="D131" s="4">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E131" s="4">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F131" s="4">
-        <v>88</v>
-      </c>
-      <c r="G131" t="s">
-        <v>16</v>
-      </c>
-      <c r="H131" t="s">
-        <v>16</v>
-      </c>
-      <c r="I131" t="s">
-        <v>16</v>
+        <v>346</v>
+      </c>
+      <c r="G131" s="4">
+        <v>19</v>
+      </c>
+      <c r="H131" s="4">
+        <v>224</v>
+      </c>
+      <c r="I131" s="4">
+        <v>66</v>
       </c>
       <c r="J131" t="str">
-        <f t="shared" ref="J131:J159" si="21">IF(C131&gt;=420,"Yes","No")</f>
+        <f t="shared" si="21"/>
         <v>No</v>
       </c>
       <c r="K131" s="2">
-        <f t="shared" ref="K131:K159" si="22">ROUND((C131/F131)*100, 2)</f>
-        <v>94.32</v>
+        <f t="shared" si="22"/>
+        <v>89.31</v>
       </c>
       <c r="L131" s="2">
-        <f t="shared" ref="L131:L159" si="23">ROUND((D131/F131)*100,2)</f>
-        <v>5.68</v>
-      </c>
-      <c r="M131" s="2" t="e">
-        <f t="shared" ref="M131:M159" si="24">ROUND((H131/F131)*100,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N131" s="2" t="e">
-        <f t="shared" ref="N131:N159" si="25">ROUND((G131/F131)*100,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O131" s="2" t="e">
-        <f t="shared" ref="O131:O159" si="26">ROUND((I131/F131)*100,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P131" s="2" t="e">
-        <f t="shared" ref="P131:P159" si="27">100-(O131+N131+M131)</f>
-        <v>#VALUE!</v>
+        <f t="shared" si="23"/>
+        <v>10.69</v>
+      </c>
+      <c r="M131" s="2">
+        <f t="shared" si="24"/>
+        <v>64.739999999999995</v>
+      </c>
+      <c r="N131" s="2">
+        <f t="shared" si="25"/>
+        <v>5.49</v>
+      </c>
+      <c r="O131" s="2">
+        <f t="shared" si="26"/>
+        <v>19.079999999999998</v>
+      </c>
+      <c r="P131" s="2">
+        <f t="shared" si="27"/>
+        <v>10.689999999999998</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C132" s="4">
-        <v>353</v>
+        <v>299</v>
       </c>
       <c r="D132" s="4">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E132" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F132" s="4">
-        <v>409</v>
+        <v>333</v>
       </c>
       <c r="G132" s="4">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="H132" s="4">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="I132" s="4">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="J132" t="str">
         <f t="shared" si="21"/>
@@ -8620,56 +8761,56 @@
       </c>
       <c r="K132" s="2">
         <f t="shared" si="22"/>
-        <v>86.31</v>
+        <v>89.79</v>
       </c>
       <c r="L132" s="2">
         <f t="shared" si="23"/>
-        <v>13.69</v>
+        <v>10.210000000000001</v>
       </c>
       <c r="M132" s="2">
         <f t="shared" si="24"/>
-        <v>49.88</v>
+        <v>51.35</v>
       </c>
       <c r="N132" s="2">
         <f t="shared" si="25"/>
-        <v>13.2</v>
+        <v>19.52</v>
       </c>
       <c r="O132" s="2">
         <f t="shared" si="26"/>
-        <v>23.23</v>
+        <v>18.920000000000002</v>
       </c>
       <c r="P132" s="2">
         <f t="shared" si="27"/>
-        <v>13.689999999999998</v>
+        <v>10.210000000000008</v>
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C133" s="4">
-        <v>358</v>
+        <v>413</v>
       </c>
       <c r="D133" s="4">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E133" s="4">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F133" s="4">
-        <v>405</v>
+        <v>463</v>
       </c>
       <c r="G133" s="4">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H133" s="4">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="I133" s="4">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="J133" t="str">
         <f t="shared" si="21"/>
@@ -8677,56 +8818,56 @@
       </c>
       <c r="K133" s="2">
         <f t="shared" si="22"/>
-        <v>88.4</v>
+        <v>89.2</v>
       </c>
       <c r="L133" s="2">
         <f t="shared" si="23"/>
-        <v>11.6</v>
+        <v>10.8</v>
       </c>
       <c r="M133" s="2">
         <f t="shared" si="24"/>
-        <v>55.31</v>
+        <v>55.29</v>
       </c>
       <c r="N133" s="2">
         <f t="shared" si="25"/>
-        <v>15.06</v>
+        <v>12.31</v>
       </c>
       <c r="O133" s="2">
         <f t="shared" si="26"/>
-        <v>18.02</v>
+        <v>21.6</v>
       </c>
       <c r="P133" s="2">
         <f t="shared" si="27"/>
-        <v>11.61</v>
+        <v>10.799999999999997</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C134" s="4">
-        <v>309</v>
+        <v>260</v>
       </c>
       <c r="D134" s="4">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E134" s="4">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F134" s="4">
-        <v>346</v>
+        <v>292</v>
       </c>
       <c r="G134" s="4">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="H134" s="4">
-        <v>224</v>
+        <v>143</v>
       </c>
       <c r="I134" s="4">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J134" t="str">
         <f t="shared" si="21"/>
@@ -8734,56 +8875,56 @@
       </c>
       <c r="K134" s="2">
         <f t="shared" si="22"/>
-        <v>89.31</v>
+        <v>89.04</v>
       </c>
       <c r="L134" s="2">
         <f t="shared" si="23"/>
-        <v>10.69</v>
+        <v>10.96</v>
       </c>
       <c r="M134" s="2">
         <f t="shared" si="24"/>
-        <v>64.739999999999995</v>
+        <v>48.97</v>
       </c>
       <c r="N134" s="2">
         <f t="shared" si="25"/>
-        <v>5.49</v>
+        <v>15.41</v>
       </c>
       <c r="O134" s="2">
         <f t="shared" si="26"/>
-        <v>19.079999999999998</v>
+        <v>24.66</v>
       </c>
       <c r="P134" s="2">
         <f t="shared" si="27"/>
-        <v>10.689999999999998</v>
+        <v>10.960000000000008</v>
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C135" s="4">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="D135" s="4">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E135" s="4">
         <v>22</v>
       </c>
       <c r="F135" s="4">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="G135" s="4">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="H135" s="4">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I135" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J135" t="str">
         <f t="shared" si="21"/>
@@ -8791,56 +8932,56 @@
       </c>
       <c r="K135" s="2">
         <f t="shared" si="22"/>
-        <v>89.79</v>
+        <v>91.69</v>
       </c>
       <c r="L135" s="2">
         <f t="shared" si="23"/>
-        <v>10.210000000000001</v>
+        <v>8.31</v>
       </c>
       <c r="M135" s="2">
         <f t="shared" si="24"/>
-        <v>51.35</v>
+        <v>48.66</v>
       </c>
       <c r="N135" s="2">
         <f t="shared" si="25"/>
-        <v>19.52</v>
+        <v>24.04</v>
       </c>
       <c r="O135" s="2">
         <f t="shared" si="26"/>
-        <v>18.920000000000002</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="P135" s="2">
         <f t="shared" si="27"/>
-        <v>10.210000000000008</v>
+        <v>8.3100000000000023</v>
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C136" s="4">
-        <v>413</v>
+        <v>391</v>
       </c>
       <c r="D136" s="4">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E136" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F136" s="4">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="G136" s="4">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H136" s="4">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="I136" s="4">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J136" t="str">
         <f t="shared" si="21"/>
@@ -8848,170 +8989,170 @@
       </c>
       <c r="K136" s="2">
         <f t="shared" si="22"/>
-        <v>89.2</v>
+        <v>87.08</v>
       </c>
       <c r="L136" s="2">
         <f t="shared" si="23"/>
-        <v>10.8</v>
+        <v>12.92</v>
       </c>
       <c r="M136" s="2">
         <f t="shared" si="24"/>
-        <v>55.29</v>
+        <v>52.78</v>
       </c>
       <c r="N136" s="2">
         <f t="shared" si="25"/>
-        <v>12.31</v>
+        <v>13.59</v>
       </c>
       <c r="O136" s="2">
         <f t="shared" si="26"/>
-        <v>21.6</v>
+        <v>20.71</v>
       </c>
       <c r="P136" s="2">
         <f t="shared" si="27"/>
-        <v>10.799999999999997</v>
+        <v>12.920000000000002</v>
       </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C137" s="4">
-        <v>260</v>
+        <v>431</v>
       </c>
       <c r="D137" s="4">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E137" s="4">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F137" s="4">
-        <v>292</v>
+        <v>480</v>
       </c>
       <c r="G137" s="4">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="H137" s="4">
-        <v>143</v>
+        <v>232</v>
       </c>
       <c r="I137" s="4">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="J137" t="str">
         <f t="shared" si="21"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="K137" s="2">
         <f t="shared" si="22"/>
-        <v>89.04</v>
+        <v>89.79</v>
       </c>
       <c r="L137" s="2">
         <f t="shared" si="23"/>
-        <v>10.96</v>
+        <v>10.210000000000001</v>
       </c>
       <c r="M137" s="2">
         <f t="shared" si="24"/>
-        <v>48.97</v>
+        <v>48.33</v>
       </c>
       <c r="N137" s="2">
         <f t="shared" si="25"/>
-        <v>15.41</v>
+        <v>16.88</v>
       </c>
       <c r="O137" s="2">
         <f t="shared" si="26"/>
-        <v>24.66</v>
+        <v>24.58</v>
       </c>
       <c r="P137" s="2">
         <f t="shared" si="27"/>
-        <v>10.960000000000008</v>
+        <v>10.210000000000008</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C138" s="4">
-        <v>96</v>
+        <v>422</v>
       </c>
       <c r="D138" s="4">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="E138" s="4">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F138" s="4">
-        <v>103</v>
-      </c>
-      <c r="G138" t="s">
-        <v>16</v>
-      </c>
-      <c r="H138" t="s">
-        <v>16</v>
-      </c>
-      <c r="I138" t="s">
-        <v>16</v>
+        <v>482</v>
+      </c>
+      <c r="G138" s="4">
+        <v>95</v>
+      </c>
+      <c r="H138" s="4">
+        <v>210</v>
+      </c>
+      <c r="I138" s="4">
+        <v>117</v>
       </c>
       <c r="J138" t="str">
         <f t="shared" si="21"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="K138" s="2">
         <f t="shared" si="22"/>
-        <v>93.2</v>
+        <v>87.55</v>
       </c>
       <c r="L138" s="2">
         <f t="shared" si="23"/>
-        <v>6.8</v>
-      </c>
-      <c r="M138" s="2" t="e">
+        <v>12.45</v>
+      </c>
+      <c r="M138" s="2">
         <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N138" s="2" t="e">
+        <v>43.57</v>
+      </c>
+      <c r="N138" s="2">
         <f t="shared" si="25"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O138" s="2" t="e">
+        <v>19.71</v>
+      </c>
+      <c r="O138" s="2">
         <f t="shared" si="26"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P138" s="2" t="e">
+        <v>24.27</v>
+      </c>
+      <c r="P138" s="2">
         <f t="shared" si="27"/>
-        <v>#VALUE!</v>
+        <v>12.449999999999989</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C139" s="4">
+        <v>356</v>
+      </c>
+      <c r="D139" s="4">
         <v>31</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C139" s="4">
-        <v>309</v>
-      </c>
-      <c r="D139" s="4">
+      <c r="E139" s="4">
         <v>28</v>
       </c>
-      <c r="E139" s="4">
-        <v>22</v>
-      </c>
       <c r="F139" s="4">
-        <v>337</v>
+        <v>387</v>
       </c>
       <c r="G139" s="4">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="H139" s="4">
-        <v>164</v>
+        <v>260</v>
       </c>
       <c r="I139" s="4">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="J139" t="str">
         <f t="shared" si="21"/>
@@ -9019,227 +9160,227 @@
       </c>
       <c r="K139" s="2">
         <f t="shared" si="22"/>
-        <v>91.69</v>
+        <v>91.99</v>
       </c>
       <c r="L139" s="2">
         <f t="shared" si="23"/>
-        <v>8.31</v>
+        <v>8.01</v>
       </c>
       <c r="M139" s="2">
         <f t="shared" si="24"/>
-        <v>48.66</v>
+        <v>67.180000000000007</v>
       </c>
       <c r="N139" s="2">
         <f t="shared" si="25"/>
-        <v>24.04</v>
+        <v>6.98</v>
       </c>
       <c r="O139" s="2">
         <f t="shared" si="26"/>
-        <v>18.989999999999998</v>
+        <v>17.829999999999998</v>
       </c>
       <c r="P139" s="2">
         <f t="shared" si="27"/>
-        <v>8.3100000000000023</v>
+        <v>8.0099999999999909</v>
       </c>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B140" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C140" s="4">
+        <v>426</v>
+      </c>
+      <c r="D140" s="4">
+        <v>39</v>
+      </c>
+      <c r="E140" s="4">
         <v>34</v>
       </c>
-      <c r="C140" s="4">
-        <v>391</v>
-      </c>
-      <c r="D140" s="4">
-        <v>58</v>
-      </c>
-      <c r="E140" s="4">
-        <v>33</v>
-      </c>
       <c r="F140" s="4">
-        <v>449</v>
+        <v>465</v>
       </c>
       <c r="G140" s="4">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="H140" s="4">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="I140" s="4">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J140" t="str">
         <f t="shared" si="21"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="K140" s="2">
         <f t="shared" si="22"/>
-        <v>87.08</v>
+        <v>91.61</v>
       </c>
       <c r="L140" s="2">
         <f t="shared" si="23"/>
-        <v>12.92</v>
+        <v>8.39</v>
       </c>
       <c r="M140" s="2">
         <f t="shared" si="24"/>
-        <v>52.78</v>
+        <v>55.7</v>
       </c>
       <c r="N140" s="2">
         <f t="shared" si="25"/>
-        <v>13.59</v>
+        <v>17.420000000000002</v>
       </c>
       <c r="O140" s="2">
         <f t="shared" si="26"/>
-        <v>20.71</v>
+        <v>18.489999999999998</v>
       </c>
       <c r="P140" s="2">
         <f t="shared" si="27"/>
-        <v>12.920000000000002</v>
+        <v>8.39</v>
       </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C141" s="4">
-        <v>431</v>
+        <v>337</v>
       </c>
       <c r="D141" s="4">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E141" s="4">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F141" s="4">
-        <v>480</v>
+        <v>377</v>
       </c>
       <c r="G141" s="4">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H141" s="4">
-        <v>232</v>
+        <v>184</v>
       </c>
       <c r="I141" s="4">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="J141" t="str">
         <f t="shared" si="21"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="K141" s="2">
         <f t="shared" si="22"/>
-        <v>89.79</v>
+        <v>89.39</v>
       </c>
       <c r="L141" s="2">
         <f t="shared" si="23"/>
-        <v>10.210000000000001</v>
+        <v>10.61</v>
       </c>
       <c r="M141" s="2">
         <f t="shared" si="24"/>
-        <v>48.33</v>
+        <v>48.81</v>
       </c>
       <c r="N141" s="2">
         <f t="shared" si="25"/>
-        <v>16.88</v>
+        <v>20.16</v>
       </c>
       <c r="O141" s="2">
         <f t="shared" si="26"/>
-        <v>24.58</v>
+        <v>20.420000000000002</v>
       </c>
       <c r="P141" s="2">
         <f t="shared" si="27"/>
-        <v>10.210000000000008</v>
+        <v>10.61</v>
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C142" s="4">
-        <v>422</v>
+        <v>379</v>
       </c>
       <c r="D142" s="4">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="E142" s="4">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F142" s="4">
-        <v>482</v>
+        <v>415</v>
       </c>
       <c r="G142" s="4">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H142" s="4">
-        <v>210</v>
+        <v>173</v>
       </c>
       <c r="I142" s="4">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="J142" t="str">
         <f t="shared" si="21"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="K142" s="2">
         <f t="shared" si="22"/>
-        <v>87.55</v>
+        <v>91.33</v>
       </c>
       <c r="L142" s="2">
         <f t="shared" si="23"/>
-        <v>12.45</v>
+        <v>8.67</v>
       </c>
       <c r="M142" s="2">
         <f t="shared" si="24"/>
-        <v>43.57</v>
+        <v>41.69</v>
       </c>
       <c r="N142" s="2">
         <f t="shared" si="25"/>
-        <v>19.71</v>
+        <v>24.1</v>
       </c>
       <c r="O142" s="2">
         <f t="shared" si="26"/>
-        <v>24.27</v>
+        <v>25.54</v>
       </c>
       <c r="P142" s="2">
         <f t="shared" si="27"/>
-        <v>12.449999999999989</v>
+        <v>8.6700000000000017</v>
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C143" s="4">
-        <v>356</v>
+        <v>375</v>
       </c>
       <c r="D143" s="4">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E143" s="4">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F143" s="4">
-        <v>387</v>
+        <v>416</v>
       </c>
       <c r="G143" s="4">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="H143" s="4">
-        <v>260</v>
+        <v>203</v>
       </c>
       <c r="I143" s="4">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="J143" t="str">
         <f t="shared" si="21"/>
@@ -9247,113 +9388,113 @@
       </c>
       <c r="K143" s="2">
         <f t="shared" si="22"/>
-        <v>91.99</v>
+        <v>90.14</v>
       </c>
       <c r="L143" s="2">
         <f t="shared" si="23"/>
-        <v>8.01</v>
+        <v>9.86</v>
       </c>
       <c r="M143" s="2">
         <f t="shared" si="24"/>
-        <v>67.180000000000007</v>
+        <v>48.8</v>
       </c>
       <c r="N143" s="2">
         <f t="shared" si="25"/>
-        <v>6.98</v>
+        <v>19.71</v>
       </c>
       <c r="O143" s="2">
         <f t="shared" si="26"/>
-        <v>17.829999999999998</v>
+        <v>21.63</v>
       </c>
       <c r="P143" s="2">
         <f t="shared" si="27"/>
-        <v>8.0099999999999909</v>
+        <v>9.86</v>
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C144" s="4">
-        <v>436</v>
+        <v>339</v>
       </c>
       <c r="D144" s="4">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E144" s="4">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F144" s="4">
-        <v>448</v>
-      </c>
-      <c r="G144" t="s">
-        <v>16</v>
-      </c>
-      <c r="H144" t="s">
-        <v>16</v>
-      </c>
-      <c r="I144" t="s">
-        <v>16</v>
+        <v>386</v>
+      </c>
+      <c r="G144" s="4">
+        <v>45</v>
+      </c>
+      <c r="H144" s="4">
+        <v>229</v>
+      </c>
+      <c r="I144" s="4">
+        <v>65</v>
       </c>
       <c r="J144" t="str">
         <f t="shared" si="21"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="K144" s="2">
         <f t="shared" si="22"/>
-        <v>97.32</v>
+        <v>87.82</v>
       </c>
       <c r="L144" s="2">
         <f t="shared" si="23"/>
-        <v>2.68</v>
-      </c>
-      <c r="M144" s="2" t="e">
+        <v>12.18</v>
+      </c>
+      <c r="M144" s="2">
         <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N144" s="2" t="e">
+        <v>59.33</v>
+      </c>
+      <c r="N144" s="2">
         <f t="shared" si="25"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O144" s="2" t="e">
+        <v>11.66</v>
+      </c>
+      <c r="O144" s="2">
         <f t="shared" si="26"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P144" s="2" t="e">
+        <v>16.84</v>
+      </c>
+      <c r="P144" s="2">
         <f t="shared" si="27"/>
-        <v>#VALUE!</v>
+        <v>12.170000000000002</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C145" s="4">
-        <v>139</v>
+        <v>352</v>
       </c>
       <c r="D145" s="4">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E145" s="4">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F145" s="4">
-        <v>158</v>
-      </c>
-      <c r="G145" t="s">
-        <v>16</v>
-      </c>
-      <c r="H145" t="s">
-        <v>16</v>
-      </c>
-      <c r="I145" t="s">
-        <v>16</v>
+        <v>397</v>
+      </c>
+      <c r="G145" s="4">
+        <v>49</v>
+      </c>
+      <c r="H145" s="4">
+        <v>219</v>
+      </c>
+      <c r="I145" s="4">
+        <v>84</v>
       </c>
       <c r="J145" t="str">
         <f t="shared" si="21"/>
@@ -9361,113 +9502,113 @@
       </c>
       <c r="K145" s="2">
         <f t="shared" si="22"/>
-        <v>87.97</v>
+        <v>88.66</v>
       </c>
       <c r="L145" s="2">
         <f t="shared" si="23"/>
-        <v>12.03</v>
-      </c>
-      <c r="M145" s="2" t="e">
+        <v>11.34</v>
+      </c>
+      <c r="M145" s="2">
         <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N145" s="2" t="e">
+        <v>55.16</v>
+      </c>
+      <c r="N145" s="2">
         <f t="shared" si="25"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O145" s="2" t="e">
+        <v>12.34</v>
+      </c>
+      <c r="O145" s="2">
         <f t="shared" si="26"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P145" s="2" t="e">
+        <v>21.16</v>
+      </c>
+      <c r="P145" s="2">
         <f t="shared" si="27"/>
-        <v>#VALUE!</v>
+        <v>11.340000000000003</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C146" s="4">
-        <v>426</v>
+        <v>315</v>
       </c>
       <c r="D146" s="4">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E146" s="4">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F146" s="4">
-        <v>465</v>
+        <v>365</v>
       </c>
       <c r="G146" s="4">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="H146" s="4">
-        <v>259</v>
+        <v>207</v>
       </c>
       <c r="I146" s="4">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J146" t="str">
         <f t="shared" si="21"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="K146" s="2">
         <f t="shared" si="22"/>
-        <v>91.61</v>
+        <v>86.3</v>
       </c>
       <c r="L146" s="2">
         <f t="shared" si="23"/>
-        <v>8.39</v>
+        <v>13.7</v>
       </c>
       <c r="M146" s="2">
         <f t="shared" si="24"/>
-        <v>55.7</v>
+        <v>56.71</v>
       </c>
       <c r="N146" s="2">
         <f t="shared" si="25"/>
-        <v>17.420000000000002</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="O146" s="2">
         <f t="shared" si="26"/>
-        <v>18.489999999999998</v>
+        <v>21.37</v>
       </c>
       <c r="P146" s="2">
         <f t="shared" si="27"/>
-        <v>8.39</v>
+        <v>13.699999999999989</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C147" s="4">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="D147" s="4">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E147" s="4">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F147" s="4">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G147" s="4">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="H147" s="4">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="I147" s="4">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="J147" t="str">
         <f t="shared" si="21"/>
@@ -9475,56 +9616,56 @@
       </c>
       <c r="K147" s="2">
         <f t="shared" si="22"/>
-        <v>89.39</v>
+        <v>86.36</v>
       </c>
       <c r="L147" s="2">
         <f t="shared" si="23"/>
-        <v>10.61</v>
+        <v>13.64</v>
       </c>
       <c r="M147" s="2">
         <f t="shared" si="24"/>
-        <v>48.81</v>
+        <v>41.71</v>
       </c>
       <c r="N147" s="2">
         <f t="shared" si="25"/>
-        <v>20.16</v>
+        <v>15.78</v>
       </c>
       <c r="O147" s="2">
         <f t="shared" si="26"/>
-        <v>20.420000000000002</v>
+        <v>28.88</v>
       </c>
       <c r="P147" s="2">
         <f t="shared" si="27"/>
-        <v>10.61</v>
+        <v>13.629999999999995</v>
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C148" s="4">
-        <v>379</v>
+        <v>405</v>
       </c>
       <c r="D148" s="4">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E148" s="4">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F148" s="4">
-        <v>415</v>
+        <v>449</v>
       </c>
       <c r="G148" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H148" s="4">
-        <v>173</v>
+        <v>220</v>
       </c>
       <c r="I148" s="4">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="J148" t="str">
         <f t="shared" si="21"/>
@@ -9532,113 +9673,113 @@
       </c>
       <c r="K148" s="2">
         <f t="shared" si="22"/>
-        <v>91.33</v>
+        <v>90.2</v>
       </c>
       <c r="L148" s="2">
         <f t="shared" si="23"/>
-        <v>8.67</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="M148" s="2">
         <f t="shared" si="24"/>
-        <v>41.69</v>
+        <v>49</v>
       </c>
       <c r="N148" s="2">
         <f t="shared" si="25"/>
-        <v>24.1</v>
+        <v>20.04</v>
       </c>
       <c r="O148" s="2">
         <f t="shared" si="26"/>
-        <v>25.54</v>
+        <v>21.16</v>
       </c>
       <c r="P148" s="2">
         <f t="shared" si="27"/>
-        <v>8.6700000000000017</v>
+        <v>9.7999999999999972</v>
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B149" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C149" s="4">
+        <v>437</v>
+      </c>
+      <c r="D149" s="4">
         <v>52</v>
       </c>
-      <c r="C149" s="4">
-        <v>375</v>
-      </c>
-      <c r="D149" s="4">
-        <v>41</v>
-      </c>
       <c r="E149" s="4">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F149" s="4">
-        <v>416</v>
+        <v>489</v>
       </c>
       <c r="G149" s="4">
         <v>82</v>
       </c>
       <c r="H149" s="4">
-        <v>203</v>
+        <v>255</v>
       </c>
       <c r="I149" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J149" t="str">
         <f t="shared" si="21"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="K149" s="2">
         <f t="shared" si="22"/>
-        <v>90.14</v>
+        <v>89.37</v>
       </c>
       <c r="L149" s="2">
         <f t="shared" si="23"/>
-        <v>9.86</v>
+        <v>10.63</v>
       </c>
       <c r="M149" s="2">
         <f t="shared" si="24"/>
-        <v>48.8</v>
+        <v>52.15</v>
       </c>
       <c r="N149" s="2">
         <f t="shared" si="25"/>
-        <v>19.71</v>
+        <v>16.77</v>
       </c>
       <c r="O149" s="2">
         <f t="shared" si="26"/>
-        <v>21.63</v>
+        <v>20.45</v>
       </c>
       <c r="P149" s="2">
         <f t="shared" si="27"/>
-        <v>9.86</v>
+        <v>10.629999999999995</v>
       </c>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C150" s="4">
-        <v>339</v>
+        <v>291</v>
       </c>
       <c r="D150" s="4">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E150" s="4">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F150" s="4">
-        <v>386</v>
+        <v>346</v>
       </c>
       <c r="G150" s="4">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H150" s="4">
-        <v>229</v>
+        <v>179</v>
       </c>
       <c r="I150" s="4">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="J150" t="str">
         <f t="shared" si="21"/>
@@ -9646,56 +9787,56 @@
       </c>
       <c r="K150" s="2">
         <f t="shared" si="22"/>
-        <v>87.82</v>
+        <v>84.1</v>
       </c>
       <c r="L150" s="2">
         <f t="shared" si="23"/>
-        <v>12.18</v>
+        <v>15.9</v>
       </c>
       <c r="M150" s="2">
         <f t="shared" si="24"/>
-        <v>59.33</v>
+        <v>51.73</v>
       </c>
       <c r="N150" s="2">
         <f t="shared" si="25"/>
-        <v>11.66</v>
+        <v>8.67</v>
       </c>
       <c r="O150" s="2">
         <f t="shared" si="26"/>
-        <v>16.84</v>
+        <v>23.7</v>
       </c>
       <c r="P150" s="2">
         <f t="shared" si="27"/>
-        <v>12.170000000000002</v>
+        <v>15.900000000000006</v>
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C151" s="4">
-        <v>352</v>
+        <v>371</v>
       </c>
       <c r="D151" s="4">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E151" s="4">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F151" s="4">
-        <v>397</v>
+        <v>429</v>
       </c>
       <c r="G151" s="4">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H151" s="4">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="I151" s="4">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J151" t="str">
         <f t="shared" si="21"/>
@@ -9703,56 +9844,56 @@
       </c>
       <c r="K151" s="2">
         <f t="shared" si="22"/>
-        <v>88.66</v>
+        <v>86.48</v>
       </c>
       <c r="L151" s="2">
         <f t="shared" si="23"/>
-        <v>11.34</v>
+        <v>13.52</v>
       </c>
       <c r="M151" s="2">
         <f t="shared" si="24"/>
-        <v>55.16</v>
+        <v>56.41</v>
       </c>
       <c r="N151" s="2">
         <f t="shared" si="25"/>
-        <v>12.34</v>
+        <v>9.7899999999999991</v>
       </c>
       <c r="O151" s="2">
         <f t="shared" si="26"/>
-        <v>21.16</v>
+        <v>20.28</v>
       </c>
       <c r="P151" s="2">
         <f t="shared" si="27"/>
-        <v>11.340000000000003</v>
+        <v>13.52000000000001</v>
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C152" s="4">
-        <v>315</v>
+        <v>371</v>
       </c>
       <c r="D152" s="4">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E152" s="4">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F152" s="4">
-        <v>365</v>
+        <v>417</v>
       </c>
       <c r="G152" s="4">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="H152" s="4">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="I152" s="4">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="J152" t="str">
         <f t="shared" si="21"/>
@@ -9760,56 +9901,56 @@
       </c>
       <c r="K152" s="2">
         <f t="shared" si="22"/>
-        <v>86.3</v>
+        <v>88.97</v>
       </c>
       <c r="L152" s="2">
         <f t="shared" si="23"/>
-        <v>13.7</v>
+        <v>11.03</v>
       </c>
       <c r="M152" s="2">
         <f t="shared" si="24"/>
-        <v>56.71</v>
+        <v>46.28</v>
       </c>
       <c r="N152" s="2">
         <f t="shared" si="25"/>
-        <v>8.2200000000000006</v>
+        <v>15.59</v>
       </c>
       <c r="O152" s="2">
         <f t="shared" si="26"/>
-        <v>21.37</v>
+        <v>27.1</v>
       </c>
       <c r="P152" s="2">
         <f t="shared" si="27"/>
-        <v>13.699999999999989</v>
+        <v>11.030000000000001</v>
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C153" s="4">
-        <v>323</v>
+        <v>363</v>
       </c>
       <c r="D153" s="4">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E153" s="4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F153" s="4">
-        <v>374</v>
+        <v>412</v>
       </c>
       <c r="G153" s="4">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="H153" s="4">
-        <v>156</v>
+        <v>211</v>
       </c>
       <c r="I153" s="4">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="J153" t="str">
         <f t="shared" si="21"/>
@@ -9817,56 +9958,56 @@
       </c>
       <c r="K153" s="2">
         <f t="shared" si="22"/>
-        <v>86.36</v>
+        <v>88.11</v>
       </c>
       <c r="L153" s="2">
         <f t="shared" si="23"/>
-        <v>13.64</v>
+        <v>11.89</v>
       </c>
       <c r="M153" s="2">
         <f t="shared" si="24"/>
-        <v>41.71</v>
+        <v>51.21</v>
       </c>
       <c r="N153" s="2">
         <f t="shared" si="25"/>
-        <v>15.78</v>
+        <v>17.48</v>
       </c>
       <c r="O153" s="2">
         <f t="shared" si="26"/>
-        <v>28.88</v>
+        <v>19.420000000000002</v>
       </c>
       <c r="P153" s="2">
         <f t="shared" si="27"/>
-        <v>13.629999999999995</v>
+        <v>11.889999999999986</v>
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A154" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>62</v>
+      <c r="A154" t="s">
+        <v>66</v>
+      </c>
+      <c r="B154" t="s">
+        <v>67</v>
       </c>
       <c r="C154" s="4">
-        <v>405</v>
+        <v>372</v>
       </c>
       <c r="D154" s="4">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E154" s="4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F154" s="4">
-        <v>449</v>
+        <v>418</v>
       </c>
       <c r="G154" s="4">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="H154" s="4">
-        <v>220</v>
+        <v>241</v>
       </c>
       <c r="I154" s="4">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="J154" t="str">
         <f t="shared" si="21"/>
@@ -9874,113 +10015,113 @@
       </c>
       <c r="K154" s="2">
         <f t="shared" si="22"/>
-        <v>90.2</v>
+        <v>89</v>
       </c>
       <c r="L154" s="2">
         <f t="shared" si="23"/>
-        <v>9.8000000000000007</v>
+        <v>11</v>
       </c>
       <c r="M154" s="2">
         <f t="shared" si="24"/>
-        <v>49</v>
+        <v>57.66</v>
       </c>
       <c r="N154" s="2">
         <f t="shared" si="25"/>
-        <v>20.04</v>
+        <v>16.27</v>
       </c>
       <c r="O154" s="2">
         <f t="shared" si="26"/>
-        <v>21.16</v>
+        <v>15.07</v>
       </c>
       <c r="P154" s="2">
         <f t="shared" si="27"/>
-        <v>9.7999999999999972</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A155" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>64</v>
+      <c r="A155" t="s">
+        <v>68</v>
+      </c>
+      <c r="B155" t="s">
+        <v>69</v>
       </c>
       <c r="C155" s="4">
-        <v>437</v>
+        <v>368</v>
       </c>
       <c r="D155" s="4">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E155" s="4">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F155" s="4">
-        <v>489</v>
+        <v>417</v>
       </c>
       <c r="G155" s="4">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="H155" s="4">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="I155" s="4">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J155" t="str">
         <f t="shared" si="21"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="K155" s="2">
         <f t="shared" si="22"/>
-        <v>89.37</v>
+        <v>88.25</v>
       </c>
       <c r="L155" s="2">
         <f t="shared" si="23"/>
-        <v>10.63</v>
+        <v>11.75</v>
       </c>
       <c r="M155" s="2">
         <f t="shared" si="24"/>
-        <v>52.15</v>
+        <v>57.07</v>
       </c>
       <c r="N155" s="2">
         <f t="shared" si="25"/>
-        <v>16.77</v>
+        <v>7.91</v>
       </c>
       <c r="O155" s="2">
         <f t="shared" si="26"/>
-        <v>20.45</v>
+        <v>23.26</v>
       </c>
       <c r="P155" s="2">
         <f t="shared" si="27"/>
-        <v>10.629999999999995</v>
+        <v>11.759999999999991</v>
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A156" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>66</v>
+      <c r="A156" t="s">
+        <v>70</v>
+      </c>
+      <c r="B156" t="s">
+        <v>71</v>
       </c>
       <c r="C156" s="4">
-        <v>291</v>
+        <v>326</v>
       </c>
       <c r="D156" s="4">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E156" s="4">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F156" s="4">
-        <v>346</v>
+        <v>380</v>
       </c>
       <c r="G156" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="H156" s="4">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I156" s="4">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="J156" t="str">
         <f t="shared" si="21"/>
@@ -9988,110 +10129,110 @@
       </c>
       <c r="K156" s="2">
         <f t="shared" si="22"/>
-        <v>84.1</v>
+        <v>85.79</v>
       </c>
       <c r="L156" s="2">
         <f t="shared" si="23"/>
-        <v>15.9</v>
+        <v>14.21</v>
       </c>
       <c r="M156" s="2">
         <f t="shared" si="24"/>
-        <v>51.73</v>
+        <v>45</v>
       </c>
       <c r="N156" s="2">
         <f t="shared" si="25"/>
-        <v>8.67</v>
+        <v>22.37</v>
       </c>
       <c r="O156" s="2">
         <f t="shared" si="26"/>
-        <v>23.7</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="P156" s="2">
         <f t="shared" si="27"/>
-        <v>15.900000000000006</v>
+        <v>14.209999999999994</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A157" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>68</v>
+      <c r="A157" t="s">
+        <v>72</v>
+      </c>
+      <c r="B157" t="s">
+        <v>73</v>
       </c>
       <c r="C157" s="4">
-        <v>371</v>
+        <v>440</v>
       </c>
       <c r="D157" s="4">
         <v>58</v>
       </c>
       <c r="E157" s="4">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F157" s="4">
-        <v>429</v>
+        <v>498</v>
       </c>
       <c r="G157" s="4">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H157" s="4">
-        <v>242</v>
+        <v>275</v>
       </c>
       <c r="I157" s="4">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J157" t="str">
         <f t="shared" si="21"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="K157" s="2">
         <f t="shared" si="22"/>
-        <v>86.48</v>
+        <v>88.35</v>
       </c>
       <c r="L157" s="2">
         <f t="shared" si="23"/>
-        <v>13.52</v>
+        <v>11.65</v>
       </c>
       <c r="M157" s="2">
         <f t="shared" si="24"/>
-        <v>56.41</v>
+        <v>55.22</v>
       </c>
       <c r="N157" s="2">
         <f t="shared" si="25"/>
-        <v>9.7899999999999991</v>
+        <v>13.45</v>
       </c>
       <c r="O157" s="2">
         <f t="shared" si="26"/>
-        <v>20.28</v>
+        <v>19.68</v>
       </c>
       <c r="P157" s="2">
         <f t="shared" si="27"/>
-        <v>13.52000000000001</v>
+        <v>11.650000000000006</v>
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A158" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>70</v>
+      <c r="A158" t="s">
+        <v>74</v>
+      </c>
+      <c r="B158" t="s">
+        <v>75</v>
       </c>
       <c r="C158" s="4">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="D158" s="4">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E158" s="4">
         <v>27</v>
       </c>
       <c r="F158" s="4">
-        <v>417</v>
+        <v>393</v>
       </c>
       <c r="G158" s="4">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H158" s="4">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I158" s="4">
         <v>113</v>
@@ -10102,56 +10243,56 @@
       </c>
       <c r="K158" s="2">
         <f t="shared" si="22"/>
-        <v>88.97</v>
+        <v>90.33</v>
       </c>
       <c r="L158" s="2">
         <f t="shared" si="23"/>
-        <v>11.03</v>
+        <v>9.67</v>
       </c>
       <c r="M158" s="2">
         <f t="shared" si="24"/>
-        <v>46.28</v>
+        <v>46.82</v>
       </c>
       <c r="N158" s="2">
         <f t="shared" si="25"/>
-        <v>15.59</v>
+        <v>14.76</v>
       </c>
       <c r="O158" s="2">
         <f t="shared" si="26"/>
-        <v>27.1</v>
+        <v>28.75</v>
       </c>
       <c r="P158" s="2">
         <f t="shared" si="27"/>
-        <v>11.030000000000001</v>
+        <v>9.6700000000000017</v>
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A159" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>72</v>
+      <c r="A159" t="s">
+        <v>76</v>
+      </c>
+      <c r="B159" t="s">
+        <v>77</v>
       </c>
       <c r="C159" s="4">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="D159" s="4">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E159" s="4">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F159" s="4">
-        <v>412</v>
+        <v>437</v>
       </c>
       <c r="G159" s="4">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="H159" s="4">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="I159" s="4">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J159" t="str">
         <f t="shared" si="21"/>
@@ -10159,27 +10300,1338 @@
       </c>
       <c r="K159" s="2">
         <f t="shared" si="22"/>
-        <v>88.11</v>
+        <v>85.35</v>
       </c>
       <c r="L159" s="2">
         <f t="shared" si="23"/>
-        <v>11.89</v>
+        <v>14.65</v>
       </c>
       <c r="M159" s="2">
         <f t="shared" si="24"/>
-        <v>51.21</v>
+        <v>56.75</v>
       </c>
       <c r="N159" s="2">
         <f t="shared" si="25"/>
-        <v>17.48</v>
+        <v>11.67</v>
       </c>
       <c r="O159" s="2">
         <f t="shared" si="26"/>
-        <v>19.420000000000002</v>
+        <v>16.93</v>
       </c>
       <c r="P159" s="2">
         <f t="shared" si="27"/>
-        <v>11.889999999999986</v>
+        <v>14.650000000000006</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>78</v>
+      </c>
+      <c r="B160" t="s">
+        <v>79</v>
+      </c>
+      <c r="C160" s="4">
+        <v>375</v>
+      </c>
+      <c r="D160" s="4">
+        <v>50</v>
+      </c>
+      <c r="E160" s="4">
+        <v>26</v>
+      </c>
+      <c r="F160" s="4">
+        <v>425</v>
+      </c>
+      <c r="G160" s="4">
+        <v>61</v>
+      </c>
+      <c r="H160" s="4">
+        <v>221</v>
+      </c>
+      <c r="I160" s="4">
+        <v>93</v>
+      </c>
+      <c r="J160" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K160" s="2">
+        <f t="shared" si="22"/>
+        <v>88.24</v>
+      </c>
+      <c r="L160" s="2">
+        <f t="shared" si="23"/>
+        <v>11.76</v>
+      </c>
+      <c r="M160" s="2">
+        <f t="shared" si="24"/>
+        <v>52</v>
+      </c>
+      <c r="N160" s="2">
+        <f t="shared" si="25"/>
+        <v>14.35</v>
+      </c>
+      <c r="O160" s="2">
+        <f t="shared" si="26"/>
+        <v>21.88</v>
+      </c>
+      <c r="P160" s="2">
+        <f t="shared" si="27"/>
+        <v>11.77000000000001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>80</v>
+      </c>
+      <c r="B161" t="s">
+        <v>81</v>
+      </c>
+      <c r="C161" s="4">
+        <v>363</v>
+      </c>
+      <c r="D161" s="4">
+        <v>56</v>
+      </c>
+      <c r="E161" s="4">
+        <v>29</v>
+      </c>
+      <c r="F161" s="4">
+        <v>419</v>
+      </c>
+      <c r="G161" s="4">
+        <v>47</v>
+      </c>
+      <c r="H161" s="4">
+        <v>232</v>
+      </c>
+      <c r="I161" s="4">
+        <v>84</v>
+      </c>
+      <c r="J161" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K161" s="2">
+        <f t="shared" si="22"/>
+        <v>86.63</v>
+      </c>
+      <c r="L161" s="2">
+        <f t="shared" si="23"/>
+        <v>13.37</v>
+      </c>
+      <c r="M161" s="2">
+        <f t="shared" si="24"/>
+        <v>55.37</v>
+      </c>
+      <c r="N161" s="2">
+        <f t="shared" si="25"/>
+        <v>11.22</v>
+      </c>
+      <c r="O161" s="2">
+        <f t="shared" si="26"/>
+        <v>20.05</v>
+      </c>
+      <c r="P161" s="2">
+        <f t="shared" si="27"/>
+        <v>13.36</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>82</v>
+      </c>
+      <c r="B162" t="s">
+        <v>83</v>
+      </c>
+      <c r="C162" s="4">
+        <v>396</v>
+      </c>
+      <c r="D162" s="4">
+        <v>35</v>
+      </c>
+      <c r="E162" s="4">
+        <v>26</v>
+      </c>
+      <c r="F162" s="4">
+        <v>431</v>
+      </c>
+      <c r="G162" s="4">
+        <v>75</v>
+      </c>
+      <c r="H162" s="4">
+        <v>216</v>
+      </c>
+      <c r="I162" s="4">
+        <v>105</v>
+      </c>
+      <c r="J162" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K162" s="2">
+        <f t="shared" si="22"/>
+        <v>91.88</v>
+      </c>
+      <c r="L162" s="2">
+        <f t="shared" si="23"/>
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="M162" s="2">
+        <f t="shared" si="24"/>
+        <v>50.12</v>
+      </c>
+      <c r="N162" s="2">
+        <f t="shared" si="25"/>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="O162" s="2">
+        <f t="shared" si="26"/>
+        <v>24.36</v>
+      </c>
+      <c r="P162" s="2">
+        <f t="shared" si="27"/>
+        <v>8.1200000000000045</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>84</v>
+      </c>
+      <c r="B163" t="s">
+        <v>85</v>
+      </c>
+      <c r="C163" s="4">
+        <v>476</v>
+      </c>
+      <c r="D163" s="4">
+        <v>75</v>
+      </c>
+      <c r="E163" s="4">
+        <v>22</v>
+      </c>
+      <c r="F163" s="4">
+        <v>551</v>
+      </c>
+      <c r="G163" s="4">
+        <v>85</v>
+      </c>
+      <c r="H163" s="4">
+        <v>283</v>
+      </c>
+      <c r="I163" s="4">
+        <v>108</v>
+      </c>
+      <c r="J163" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K163" s="2">
+        <f t="shared" si="22"/>
+        <v>86.39</v>
+      </c>
+      <c r="L163" s="2">
+        <f t="shared" si="23"/>
+        <v>13.61</v>
+      </c>
+      <c r="M163" s="2">
+        <f t="shared" si="24"/>
+        <v>51.36</v>
+      </c>
+      <c r="N163" s="2">
+        <f t="shared" si="25"/>
+        <v>15.43</v>
+      </c>
+      <c r="O163" s="2">
+        <f t="shared" si="26"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="P163" s="2">
+        <f t="shared" si="27"/>
+        <v>13.61</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>86</v>
+      </c>
+      <c r="B164" t="s">
+        <v>87</v>
+      </c>
+      <c r="C164" s="4">
+        <v>420</v>
+      </c>
+      <c r="D164" s="4">
+        <v>93</v>
+      </c>
+      <c r="E164" s="4">
+        <v>18</v>
+      </c>
+      <c r="F164" s="4">
+        <v>513</v>
+      </c>
+      <c r="G164" s="4">
+        <v>43</v>
+      </c>
+      <c r="H164" s="4">
+        <v>308</v>
+      </c>
+      <c r="I164" s="4">
+        <v>69</v>
+      </c>
+      <c r="J164" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K164" s="2">
+        <f t="shared" si="22"/>
+        <v>81.87</v>
+      </c>
+      <c r="L164" s="2">
+        <f t="shared" si="23"/>
+        <v>18.13</v>
+      </c>
+      <c r="M164" s="2">
+        <f t="shared" si="24"/>
+        <v>60.04</v>
+      </c>
+      <c r="N164" s="2">
+        <f t="shared" si="25"/>
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="O164" s="2">
+        <f t="shared" si="26"/>
+        <v>13.45</v>
+      </c>
+      <c r="P164" s="2">
+        <f t="shared" si="27"/>
+        <v>18.129999999999995</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>88</v>
+      </c>
+      <c r="B165" t="s">
+        <v>89</v>
+      </c>
+      <c r="C165" s="4">
+        <v>411</v>
+      </c>
+      <c r="D165" s="4">
+        <v>56</v>
+      </c>
+      <c r="E165" s="4">
+        <v>35</v>
+      </c>
+      <c r="F165" s="4">
+        <v>467</v>
+      </c>
+      <c r="G165" s="4">
+        <v>41</v>
+      </c>
+      <c r="H165" s="4">
+        <v>282</v>
+      </c>
+      <c r="I165" s="4">
+        <v>88</v>
+      </c>
+      <c r="J165" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K165" s="2">
+        <f t="shared" si="22"/>
+        <v>88.01</v>
+      </c>
+      <c r="L165" s="2">
+        <f t="shared" si="23"/>
+        <v>11.99</v>
+      </c>
+      <c r="M165" s="2">
+        <f t="shared" si="24"/>
+        <v>60.39</v>
+      </c>
+      <c r="N165" s="2">
+        <f t="shared" si="25"/>
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="O165" s="2">
+        <f t="shared" si="26"/>
+        <v>18.84</v>
+      </c>
+      <c r="P165" s="2">
+        <f t="shared" si="27"/>
+        <v>11.990000000000009</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>90</v>
+      </c>
+      <c r="B166" t="s">
+        <v>91</v>
+      </c>
+      <c r="C166" s="4">
+        <v>382</v>
+      </c>
+      <c r="D166" s="4">
+        <v>59</v>
+      </c>
+      <c r="E166" s="4">
+        <v>32</v>
+      </c>
+      <c r="F166" s="4">
+        <v>441</v>
+      </c>
+      <c r="G166" s="4">
+        <v>45</v>
+      </c>
+      <c r="H166" s="4">
+        <v>234</v>
+      </c>
+      <c r="I166" s="4">
+        <v>103</v>
+      </c>
+      <c r="J166" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K166" s="2">
+        <f t="shared" si="22"/>
+        <v>86.62</v>
+      </c>
+      <c r="L166" s="2">
+        <f t="shared" si="23"/>
+        <v>13.38</v>
+      </c>
+      <c r="M166" s="2">
+        <f t="shared" si="24"/>
+        <v>53.06</v>
+      </c>
+      <c r="N166" s="2">
+        <f t="shared" si="25"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="O166" s="2">
+        <f t="shared" si="26"/>
+        <v>23.36</v>
+      </c>
+      <c r="P166" s="2">
+        <f t="shared" si="27"/>
+        <v>13.379999999999995</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>92</v>
+      </c>
+      <c r="B167" t="s">
+        <v>93</v>
+      </c>
+      <c r="C167" s="4">
+        <v>365</v>
+      </c>
+      <c r="D167" s="4">
+        <v>53</v>
+      </c>
+      <c r="E167" s="4">
+        <v>29</v>
+      </c>
+      <c r="F167" s="4">
+        <v>418</v>
+      </c>
+      <c r="G167" s="4">
+        <v>81</v>
+      </c>
+      <c r="H167" s="4">
+        <v>191</v>
+      </c>
+      <c r="I167" s="4">
+        <v>93</v>
+      </c>
+      <c r="J167" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K167" s="2">
+        <f t="shared" si="22"/>
+        <v>87.32</v>
+      </c>
+      <c r="L167" s="2">
+        <f t="shared" si="23"/>
+        <v>12.68</v>
+      </c>
+      <c r="M167" s="2">
+        <f t="shared" si="24"/>
+        <v>45.69</v>
+      </c>
+      <c r="N167" s="2">
+        <f t="shared" si="25"/>
+        <v>19.38</v>
+      </c>
+      <c r="O167" s="2">
+        <f t="shared" si="26"/>
+        <v>22.25</v>
+      </c>
+      <c r="P167" s="2">
+        <f t="shared" si="27"/>
+        <v>12.680000000000007</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>94</v>
+      </c>
+      <c r="B168" t="s">
+        <v>95</v>
+      </c>
+      <c r="C168" s="4">
+        <v>390</v>
+      </c>
+      <c r="D168" s="4">
+        <v>52</v>
+      </c>
+      <c r="E168" s="4">
+        <v>23</v>
+      </c>
+      <c r="F168" s="4">
+        <v>442</v>
+      </c>
+      <c r="G168" s="4">
+        <v>60</v>
+      </c>
+      <c r="H168" s="4">
+        <v>240</v>
+      </c>
+      <c r="I168" s="4">
+        <v>90</v>
+      </c>
+      <c r="J168" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K168" s="2">
+        <f t="shared" si="22"/>
+        <v>88.24</v>
+      </c>
+      <c r="L168" s="2">
+        <f t="shared" si="23"/>
+        <v>11.76</v>
+      </c>
+      <c r="M168" s="2">
+        <f t="shared" si="24"/>
+        <v>54.3</v>
+      </c>
+      <c r="N168" s="2">
+        <f t="shared" si="25"/>
+        <v>13.57</v>
+      </c>
+      <c r="O168" s="2">
+        <f t="shared" si="26"/>
+        <v>20.36</v>
+      </c>
+      <c r="P168" s="2">
+        <f t="shared" si="27"/>
+        <v>11.77000000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>96</v>
+      </c>
+      <c r="B169" t="s">
+        <v>97</v>
+      </c>
+      <c r="C169" s="4">
+        <v>420</v>
+      </c>
+      <c r="D169" s="4">
+        <v>38</v>
+      </c>
+      <c r="E169" s="4">
+        <v>28</v>
+      </c>
+      <c r="F169" s="4">
+        <v>458</v>
+      </c>
+      <c r="G169" s="4">
+        <v>110</v>
+      </c>
+      <c r="H169" s="4">
+        <v>202</v>
+      </c>
+      <c r="I169" s="4">
+        <v>108</v>
+      </c>
+      <c r="J169" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K169" s="2">
+        <f t="shared" si="22"/>
+        <v>91.7</v>
+      </c>
+      <c r="L169" s="2">
+        <f t="shared" si="23"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M169" s="2">
+        <f t="shared" si="24"/>
+        <v>44.1</v>
+      </c>
+      <c r="N169" s="2">
+        <f t="shared" si="25"/>
+        <v>24.02</v>
+      </c>
+      <c r="O169" s="2">
+        <f t="shared" si="26"/>
+        <v>23.58</v>
+      </c>
+      <c r="P169" s="2">
+        <f t="shared" si="27"/>
+        <v>8.3000000000000114</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>98</v>
+      </c>
+      <c r="B170" t="s">
+        <v>99</v>
+      </c>
+      <c r="C170" s="4">
+        <v>436</v>
+      </c>
+      <c r="D170" s="4">
+        <v>67</v>
+      </c>
+      <c r="E170" s="4">
+        <v>27</v>
+      </c>
+      <c r="F170" s="4">
+        <v>503</v>
+      </c>
+      <c r="G170" s="4">
+        <v>118</v>
+      </c>
+      <c r="H170" s="4">
+        <v>219</v>
+      </c>
+      <c r="I170" s="4">
+        <v>99</v>
+      </c>
+      <c r="J170" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K170" s="2">
+        <f t="shared" si="22"/>
+        <v>86.68</v>
+      </c>
+      <c r="L170" s="2">
+        <f t="shared" si="23"/>
+        <v>13.32</v>
+      </c>
+      <c r="M170" s="2">
+        <f t="shared" si="24"/>
+        <v>43.54</v>
+      </c>
+      <c r="N170" s="2">
+        <f t="shared" si="25"/>
+        <v>23.46</v>
+      </c>
+      <c r="O170" s="2">
+        <f t="shared" si="26"/>
+        <v>19.68</v>
+      </c>
+      <c r="P170" s="2">
+        <f t="shared" si="27"/>
+        <v>13.319999999999993</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>100</v>
+      </c>
+      <c r="B171" t="s">
+        <v>101</v>
+      </c>
+      <c r="C171" s="4">
+        <v>384</v>
+      </c>
+      <c r="D171" s="4">
+        <v>73</v>
+      </c>
+      <c r="E171" s="4">
+        <v>31</v>
+      </c>
+      <c r="F171" s="4">
+        <v>457</v>
+      </c>
+      <c r="G171" s="4">
+        <v>39</v>
+      </c>
+      <c r="H171" s="4">
+        <v>269</v>
+      </c>
+      <c r="I171" s="4">
+        <v>76</v>
+      </c>
+      <c r="J171" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K171" s="2">
+        <f t="shared" si="22"/>
+        <v>84.03</v>
+      </c>
+      <c r="L171" s="2">
+        <f t="shared" si="23"/>
+        <v>15.97</v>
+      </c>
+      <c r="M171" s="2">
+        <f t="shared" si="24"/>
+        <v>58.86</v>
+      </c>
+      <c r="N171" s="2">
+        <f t="shared" si="25"/>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="O171" s="2">
+        <f t="shared" si="26"/>
+        <v>16.63</v>
+      </c>
+      <c r="P171" s="2">
+        <f t="shared" si="27"/>
+        <v>15.980000000000004</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>102</v>
+      </c>
+      <c r="B172" t="s">
+        <v>103</v>
+      </c>
+      <c r="C172" s="4">
+        <v>391</v>
+      </c>
+      <c r="D172" s="4">
+        <v>52</v>
+      </c>
+      <c r="E172" s="4">
+        <v>25</v>
+      </c>
+      <c r="F172" s="4">
+        <v>443</v>
+      </c>
+      <c r="G172" s="4">
+        <v>49</v>
+      </c>
+      <c r="H172" s="4">
+        <v>256</v>
+      </c>
+      <c r="I172" s="4">
+        <v>86</v>
+      </c>
+      <c r="J172" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K172" s="2">
+        <f t="shared" si="22"/>
+        <v>88.26</v>
+      </c>
+      <c r="L172" s="2">
+        <f t="shared" si="23"/>
+        <v>11.74</v>
+      </c>
+      <c r="M172" s="2">
+        <f t="shared" si="24"/>
+        <v>57.79</v>
+      </c>
+      <c r="N172" s="2">
+        <f t="shared" si="25"/>
+        <v>11.06</v>
+      </c>
+      <c r="O172" s="2">
+        <f t="shared" si="26"/>
+        <v>19.41</v>
+      </c>
+      <c r="P172" s="2">
+        <f t="shared" si="27"/>
+        <v>11.740000000000009</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>104</v>
+      </c>
+      <c r="B173" t="s">
+        <v>105</v>
+      </c>
+      <c r="C173" s="4">
+        <v>325</v>
+      </c>
+      <c r="D173" s="4">
+        <v>50</v>
+      </c>
+      <c r="E173" s="4">
+        <v>27</v>
+      </c>
+      <c r="F173" s="4">
+        <v>375</v>
+      </c>
+      <c r="G173" s="4">
+        <v>67</v>
+      </c>
+      <c r="H173" s="4">
+        <v>183</v>
+      </c>
+      <c r="I173" s="4">
+        <v>75</v>
+      </c>
+      <c r="J173" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K173" s="2">
+        <f t="shared" si="22"/>
+        <v>86.67</v>
+      </c>
+      <c r="L173" s="2">
+        <f t="shared" si="23"/>
+        <v>13.33</v>
+      </c>
+      <c r="M173" s="2">
+        <f t="shared" si="24"/>
+        <v>48.8</v>
+      </c>
+      <c r="N173" s="2">
+        <f t="shared" si="25"/>
+        <v>17.87</v>
+      </c>
+      <c r="O173" s="2">
+        <f t="shared" si="26"/>
+        <v>20</v>
+      </c>
+      <c r="P173" s="2">
+        <f t="shared" si="27"/>
+        <v>13.329999999999998</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>106</v>
+      </c>
+      <c r="B174" t="s">
+        <v>107</v>
+      </c>
+      <c r="C174" s="4">
+        <v>389</v>
+      </c>
+      <c r="D174" s="4">
+        <v>49</v>
+      </c>
+      <c r="E174" s="4">
+        <v>31</v>
+      </c>
+      <c r="F174" s="4">
+        <v>438</v>
+      </c>
+      <c r="G174" s="4">
+        <v>66</v>
+      </c>
+      <c r="H174" s="4">
+        <v>254</v>
+      </c>
+      <c r="I174" s="4">
+        <v>69</v>
+      </c>
+      <c r="J174" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K174" s="2">
+        <f t="shared" si="22"/>
+        <v>88.81</v>
+      </c>
+      <c r="L174" s="2">
+        <f t="shared" si="23"/>
+        <v>11.19</v>
+      </c>
+      <c r="M174" s="2">
+        <f t="shared" si="24"/>
+        <v>57.99</v>
+      </c>
+      <c r="N174" s="2">
+        <f t="shared" si="25"/>
+        <v>15.07</v>
+      </c>
+      <c r="O174" s="2">
+        <f t="shared" si="26"/>
+        <v>15.75</v>
+      </c>
+      <c r="P174" s="2">
+        <f t="shared" si="27"/>
+        <v>11.189999999999998</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>108</v>
+      </c>
+      <c r="B175" t="s">
+        <v>109</v>
+      </c>
+      <c r="C175" s="4">
+        <v>349</v>
+      </c>
+      <c r="D175" s="4">
+        <v>39</v>
+      </c>
+      <c r="E175" s="4">
+        <v>13</v>
+      </c>
+      <c r="F175" s="4">
+        <v>388</v>
+      </c>
+      <c r="G175" s="4">
+        <v>79</v>
+      </c>
+      <c r="H175" s="4">
+        <v>199</v>
+      </c>
+      <c r="I175" s="4">
+        <v>71</v>
+      </c>
+      <c r="J175" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K175" s="2">
+        <f t="shared" si="22"/>
+        <v>89.95</v>
+      </c>
+      <c r="L175" s="2">
+        <f t="shared" si="23"/>
+        <v>10.050000000000001</v>
+      </c>
+      <c r="M175" s="2">
+        <f t="shared" si="24"/>
+        <v>51.29</v>
+      </c>
+      <c r="N175" s="2">
+        <f t="shared" si="25"/>
+        <v>20.36</v>
+      </c>
+      <c r="O175" s="2">
+        <f t="shared" si="26"/>
+        <v>18.3</v>
+      </c>
+      <c r="P175" s="2">
+        <f t="shared" si="27"/>
+        <v>10.050000000000011</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>110</v>
+      </c>
+      <c r="B176" t="s">
+        <v>111</v>
+      </c>
+      <c r="C176" s="4">
+        <v>334</v>
+      </c>
+      <c r="D176" s="4">
+        <v>36</v>
+      </c>
+      <c r="E176" s="4">
+        <v>21</v>
+      </c>
+      <c r="F176" s="4">
+        <v>370</v>
+      </c>
+      <c r="G176" s="4">
+        <v>42</v>
+      </c>
+      <c r="H176" s="4">
+        <v>217</v>
+      </c>
+      <c r="I176" s="4">
+        <v>75</v>
+      </c>
+      <c r="J176" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K176" s="2">
+        <f t="shared" si="22"/>
+        <v>90.27</v>
+      </c>
+      <c r="L176" s="2">
+        <f t="shared" si="23"/>
+        <v>9.73</v>
+      </c>
+      <c r="M176" s="2">
+        <f t="shared" si="24"/>
+        <v>58.65</v>
+      </c>
+      <c r="N176" s="2">
+        <f t="shared" si="25"/>
+        <v>11.35</v>
+      </c>
+      <c r="O176" s="2">
+        <f t="shared" si="26"/>
+        <v>20.27</v>
+      </c>
+      <c r="P176" s="2">
+        <f t="shared" si="27"/>
+        <v>9.730000000000004</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>112</v>
+      </c>
+      <c r="B177" t="s">
+        <v>113</v>
+      </c>
+      <c r="C177" s="4">
+        <v>491</v>
+      </c>
+      <c r="D177" s="4">
+        <v>53</v>
+      </c>
+      <c r="E177" s="4">
+        <v>23</v>
+      </c>
+      <c r="F177" s="4">
+        <v>544</v>
+      </c>
+      <c r="G177" s="4">
+        <v>55</v>
+      </c>
+      <c r="H177" s="4">
+        <v>324</v>
+      </c>
+      <c r="I177" s="4">
+        <v>112</v>
+      </c>
+      <c r="J177" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+      <c r="K177" s="2">
+        <f t="shared" si="22"/>
+        <v>90.26</v>
+      </c>
+      <c r="L177" s="2">
+        <f t="shared" si="23"/>
+        <v>9.74</v>
+      </c>
+      <c r="M177" s="2">
+        <f t="shared" si="24"/>
+        <v>59.56</v>
+      </c>
+      <c r="N177" s="2">
+        <f t="shared" si="25"/>
+        <v>10.11</v>
+      </c>
+      <c r="O177" s="2">
+        <f t="shared" si="26"/>
+        <v>20.59</v>
+      </c>
+      <c r="P177" s="2">
+        <f t="shared" si="27"/>
+        <v>9.7399999999999949</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>114</v>
+      </c>
+      <c r="B178" t="s">
+        <v>115</v>
+      </c>
+      <c r="C178" s="4">
+        <v>325</v>
+      </c>
+      <c r="D178" s="4">
+        <v>34</v>
+      </c>
+      <c r="E178" s="4">
+        <v>26</v>
+      </c>
+      <c r="F178" s="4">
+        <v>359</v>
+      </c>
+      <c r="G178" s="4">
+        <v>73</v>
+      </c>
+      <c r="H178" s="4">
+        <v>204</v>
+      </c>
+      <c r="I178" s="4">
+        <v>48</v>
+      </c>
+      <c r="J178" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K178" s="2">
+        <f t="shared" si="22"/>
+        <v>90.53</v>
+      </c>
+      <c r="L178" s="2">
+        <f t="shared" si="23"/>
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="M178" s="2">
+        <f t="shared" si="24"/>
+        <v>56.82</v>
+      </c>
+      <c r="N178" s="2">
+        <f t="shared" si="25"/>
+        <v>20.329999999999998</v>
+      </c>
+      <c r="O178" s="2">
+        <f t="shared" si="26"/>
+        <v>13.37</v>
+      </c>
+      <c r="P178" s="2">
+        <f t="shared" si="27"/>
+        <v>9.480000000000004</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>116</v>
+      </c>
+      <c r="B179" t="s">
+        <v>117</v>
+      </c>
+      <c r="C179" s="4">
+        <v>354</v>
+      </c>
+      <c r="D179" s="4">
+        <v>32</v>
+      </c>
+      <c r="E179" s="4">
+        <v>27</v>
+      </c>
+      <c r="F179" s="4">
+        <v>386</v>
+      </c>
+      <c r="G179" s="4">
+        <v>43</v>
+      </c>
+      <c r="H179" s="4">
+        <v>257</v>
+      </c>
+      <c r="I179" s="4">
+        <v>54</v>
+      </c>
+      <c r="J179" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K179" s="2">
+        <f t="shared" si="22"/>
+        <v>91.71</v>
+      </c>
+      <c r="L179" s="2">
+        <f t="shared" si="23"/>
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="M179" s="2">
+        <f t="shared" si="24"/>
+        <v>66.58</v>
+      </c>
+      <c r="N179" s="2">
+        <f t="shared" si="25"/>
+        <v>11.14</v>
+      </c>
+      <c r="O179" s="2">
+        <f t="shared" si="26"/>
+        <v>13.99</v>
+      </c>
+      <c r="P179" s="2">
+        <f t="shared" si="27"/>
+        <v>8.289999999999992</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>118</v>
+      </c>
+      <c r="B180" t="s">
+        <v>119</v>
+      </c>
+      <c r="C180" s="4">
+        <v>327</v>
+      </c>
+      <c r="D180" s="4">
+        <v>50</v>
+      </c>
+      <c r="E180" s="4">
+        <v>23</v>
+      </c>
+      <c r="F180" s="4">
+        <v>377</v>
+      </c>
+      <c r="G180" s="4">
+        <v>58</v>
+      </c>
+      <c r="H180" s="4">
+        <v>209</v>
+      </c>
+      <c r="I180" s="4">
+        <v>60</v>
+      </c>
+      <c r="J180" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K180" s="2">
+        <f t="shared" si="22"/>
+        <v>86.74</v>
+      </c>
+      <c r="L180" s="2">
+        <f t="shared" si="23"/>
+        <v>13.26</v>
+      </c>
+      <c r="M180" s="2">
+        <f t="shared" si="24"/>
+        <v>55.44</v>
+      </c>
+      <c r="N180" s="2">
+        <f t="shared" si="25"/>
+        <v>15.38</v>
+      </c>
+      <c r="O180" s="2">
+        <f t="shared" si="26"/>
+        <v>15.92</v>
+      </c>
+      <c r="P180" s="2">
+        <f t="shared" si="27"/>
+        <v>13.260000000000005</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>120</v>
+      </c>
+      <c r="B181" t="s">
+        <v>121</v>
+      </c>
+      <c r="C181" s="4">
+        <v>329</v>
+      </c>
+      <c r="D181" s="4">
+        <v>47</v>
+      </c>
+      <c r="E181" s="4">
+        <v>21</v>
+      </c>
+      <c r="F181" s="4">
+        <v>376</v>
+      </c>
+      <c r="G181" s="4">
+        <v>49</v>
+      </c>
+      <c r="H181" s="4">
+        <v>200</v>
+      </c>
+      <c r="I181" s="4">
+        <v>80</v>
+      </c>
+      <c r="J181" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K181" s="2">
+        <f t="shared" si="22"/>
+        <v>87.5</v>
+      </c>
+      <c r="L181" s="2">
+        <f t="shared" si="23"/>
+        <v>12.5</v>
+      </c>
+      <c r="M181" s="2">
+        <f t="shared" si="24"/>
+        <v>53.19</v>
+      </c>
+      <c r="N181" s="2">
+        <f t="shared" si="25"/>
+        <v>13.03</v>
+      </c>
+      <c r="O181" s="2">
+        <f t="shared" si="26"/>
+        <v>21.28</v>
+      </c>
+      <c r="P181" s="2">
+        <f t="shared" si="27"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>122</v>
+      </c>
+      <c r="B182" t="s">
+        <v>123</v>
+      </c>
+      <c r="C182" s="4">
+        <v>406</v>
+      </c>
+      <c r="D182" s="4">
+        <v>41</v>
+      </c>
+      <c r="E182" s="4">
+        <v>29</v>
+      </c>
+      <c r="F182" s="4">
+        <v>447</v>
+      </c>
+      <c r="G182" s="4">
+        <v>72</v>
+      </c>
+      <c r="H182" s="4">
+        <v>251</v>
+      </c>
+      <c r="I182" s="4">
+        <v>83</v>
+      </c>
+      <c r="J182" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K182" s="2">
+        <f t="shared" si="22"/>
+        <v>90.83</v>
+      </c>
+      <c r="L182" s="2">
+        <f t="shared" si="23"/>
+        <v>9.17</v>
+      </c>
+      <c r="M182" s="2">
+        <f t="shared" si="24"/>
+        <v>56.15</v>
+      </c>
+      <c r="N182" s="2">
+        <f t="shared" si="25"/>
+        <v>16.11</v>
+      </c>
+      <c r="O182" s="2">
+        <f t="shared" si="26"/>
+        <v>18.57</v>
+      </c>
+      <c r="P182" s="2">
+        <f t="shared" si="27"/>
+        <v>9.1700000000000017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the TotalSleep file 01/05/2018
</commit_message>
<xml_diff>
--- a/datasets/TotalSleep.xlsx
+++ b/datasets/TotalSleep.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9C12E5-D228-40B1-AD7D-BC5A499AE7A1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DF64D75-56E8-494D-BC2C-AF6D2C800D78}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TotalSleep" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="183">
   <si>
     <t>Start Time</t>
   </si>
@@ -392,13 +392,190 @@
   </si>
   <si>
     <t>31-03-2018 5:23 am</t>
+  </si>
+  <si>
+    <t>31-03-2018 10:21 pm</t>
+  </si>
+  <si>
+    <t>01-04-2018 5:03 am</t>
+  </si>
+  <si>
+    <t>01-04-2018 10:00 pm</t>
+  </si>
+  <si>
+    <t>02-04-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>02-04-2018 9:51 pm</t>
+  </si>
+  <si>
+    <t>03-04-2018 4:13 am</t>
+  </si>
+  <si>
+    <t>04-04-2018 11:01 pm</t>
+  </si>
+  <si>
+    <t>05-04-2018 3:13 am</t>
+  </si>
+  <si>
+    <t>05-04-2018 10:12 pm</t>
+  </si>
+  <si>
+    <t>06-04-2018 4:39 am</t>
+  </si>
+  <si>
+    <t>06-04-2018 9:49 pm</t>
+  </si>
+  <si>
+    <t>07-04-2018 5:14 am</t>
+  </si>
+  <si>
+    <t>08-04-2018 12:28 am</t>
+  </si>
+  <si>
+    <t>08-04-2018 6:27 am</t>
+  </si>
+  <si>
+    <t>08-04-2018 9:43 pm</t>
+  </si>
+  <si>
+    <t>09-04-2018 5:03 am</t>
+  </si>
+  <si>
+    <t>09-04-2018 10:32 pm</t>
+  </si>
+  <si>
+    <t>10-04-2018 4:45 am</t>
+  </si>
+  <si>
+    <t>10-04-2018 10:46 pm</t>
+  </si>
+  <si>
+    <t>11-04-2018 5:03 am</t>
+  </si>
+  <si>
+    <t>11-04-2018 10:25 pm</t>
+  </si>
+  <si>
+    <t>12-04-2018 5:30 am</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>12-04-2018 10:41 pm</t>
+  </si>
+  <si>
+    <t>13-04-2018 5:10 am</t>
+  </si>
+  <si>
+    <t>13-04-2018 10:11 pm</t>
+  </si>
+  <si>
+    <t>14-04-2018 3:48 am</t>
+  </si>
+  <si>
+    <t>14-04-2018 11:07 pm</t>
+  </si>
+  <si>
+    <t>15-04-2018 5:22 am</t>
+  </si>
+  <si>
+    <t>15-04-2018 10:20 pm</t>
+  </si>
+  <si>
+    <t>16-04-2018 4:42 am</t>
+  </si>
+  <si>
+    <t>16-04-2018 10:48 pm</t>
+  </si>
+  <si>
+    <t>17-04-2018 4:57 am</t>
+  </si>
+  <si>
+    <t>17-04-2018 10:39 pm</t>
+  </si>
+  <si>
+    <t>18-04-2018 4:58 am</t>
+  </si>
+  <si>
+    <t>18-04-2018 9:45 pm</t>
+  </si>
+  <si>
+    <t>19-04-2018 4:55 am</t>
+  </si>
+  <si>
+    <t>19-04-2018 9:41 pm</t>
+  </si>
+  <si>
+    <t>20-04-2018 4:48 am</t>
+  </si>
+  <si>
+    <t>20-04-2018 10:00 pm</t>
+  </si>
+  <si>
+    <t>21-04-2018 6:29 am</t>
+  </si>
+  <si>
+    <t>21-04-2018 9:12 pm</t>
+  </si>
+  <si>
+    <t>22-04-2018 5:01 am</t>
+  </si>
+  <si>
+    <t>22-04-2018 9:53 pm</t>
+  </si>
+  <si>
+    <t>23-04-2018 5:06 am</t>
+  </si>
+  <si>
+    <t>23-04-2018 11:58 pm</t>
+  </si>
+  <si>
+    <t>24-04-2018 5:00 am</t>
+  </si>
+  <si>
+    <t>24-04-2018 9:35 pm</t>
+  </si>
+  <si>
+    <t>25-04-2018 6:52 am</t>
+  </si>
+  <si>
+    <t>25-04-2018 9:58 pm</t>
+  </si>
+  <si>
+    <t>26-04-2018 5:02 am</t>
+  </si>
+  <si>
+    <t>26-04-2018 10:13 pm</t>
+  </si>
+  <si>
+    <t>27-04-2018 5:05 am</t>
+  </si>
+  <si>
+    <t>27-04-2018 11:14 pm</t>
+  </si>
+  <si>
+    <t>28-04-2018 5:25 am</t>
+  </si>
+  <si>
+    <t>28-04-2018 10:14 pm</t>
+  </si>
+  <si>
+    <t>29-04-2018 6:05 am</t>
+  </si>
+  <si>
+    <t>29-04-2018 9:42 pm</t>
+  </si>
+  <si>
+    <t>30-04-2018 4:39 am</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,6 +714,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="33">
@@ -836,7 +1017,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -880,15 +1061,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -927,6 +1111,7 @@
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 3" xfId="43" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1243,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P182"/>
+  <dimension ref="A1:P211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G119" sqref="A119:XFD119"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P182" sqref="P182:P211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8585,31 +8770,31 @@
         <v>95</v>
       </c>
       <c r="J129" t="str">
-        <f t="shared" ref="J129:J182" si="21">IF(C129&gt;=420,"Yes","No")</f>
+        <f t="shared" ref="J129:J192" si="21">IF(C129&gt;=420,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="K129" s="2">
-        <f t="shared" ref="K129:K182" si="22">ROUND((C129/F129)*100, 2)</f>
+        <f t="shared" ref="K129:K192" si="22">ROUND((C129/F129)*100, 2)</f>
         <v>86.31</v>
       </c>
       <c r="L129" s="2">
-        <f t="shared" ref="L129:L182" si="23">ROUND((D129/F129)*100,2)</f>
+        <f t="shared" ref="L129:L192" si="23">ROUND((D129/F129)*100,2)</f>
         <v>13.69</v>
       </c>
       <c r="M129" s="2">
-        <f t="shared" ref="M129:M182" si="24">ROUND((H129/F129)*100,2)</f>
+        <f t="shared" ref="M129:M192" si="24">ROUND((H129/F129)*100,2)</f>
         <v>49.88</v>
       </c>
       <c r="N129" s="2">
-        <f t="shared" ref="N129:N182" si="25">ROUND((G129/F129)*100,2)</f>
+        <f t="shared" ref="N129:N192" si="25">ROUND((G129/F129)*100,2)</f>
         <v>13.2</v>
       </c>
       <c r="O129" s="2">
-        <f t="shared" ref="O129:O182" si="26">ROUND((I129/F129)*100,2)</f>
+        <f t="shared" ref="O129:O192" si="26">ROUND((I129/F129)*100,2)</f>
         <v>23.23</v>
       </c>
       <c r="P129" s="2">
-        <f t="shared" ref="P129:P182" si="27">100-(O129+N129+M129)</f>
+        <f t="shared" ref="P129:P192" si="27">100-(O129+N129+M129)</f>
         <v>13.689999999999998</v>
       </c>
     </row>
@@ -11632,6 +11817,1659 @@
       <c r="P182" s="2">
         <f t="shared" si="27"/>
         <v>9.1700000000000017</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A183" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C183" s="6">
+        <v>355</v>
+      </c>
+      <c r="D183" s="6">
+        <v>47</v>
+      </c>
+      <c r="E183" s="6">
+        <v>14</v>
+      </c>
+      <c r="F183" s="6">
+        <v>402</v>
+      </c>
+      <c r="G183" s="6">
+        <v>55</v>
+      </c>
+      <c r="H183" s="6">
+        <v>218</v>
+      </c>
+      <c r="I183" s="6">
+        <v>82</v>
+      </c>
+      <c r="J183" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K183" s="2">
+        <f t="shared" si="22"/>
+        <v>88.31</v>
+      </c>
+      <c r="L183" s="2">
+        <f t="shared" si="23"/>
+        <v>11.69</v>
+      </c>
+      <c r="M183" s="2">
+        <f t="shared" si="24"/>
+        <v>54.23</v>
+      </c>
+      <c r="N183" s="2">
+        <f t="shared" si="25"/>
+        <v>13.68</v>
+      </c>
+      <c r="O183" s="2">
+        <f t="shared" si="26"/>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="P183" s="2">
+        <f t="shared" si="27"/>
+        <v>11.689999999999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A184" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C184" s="6">
+        <v>373</v>
+      </c>
+      <c r="D184" s="6">
+        <v>45</v>
+      </c>
+      <c r="E184" s="6">
+        <v>33</v>
+      </c>
+      <c r="F184" s="6">
+        <v>418</v>
+      </c>
+      <c r="G184" s="6">
+        <v>40</v>
+      </c>
+      <c r="H184" s="6">
+        <v>236</v>
+      </c>
+      <c r="I184" s="6">
+        <v>97</v>
+      </c>
+      <c r="J184" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K184" s="2">
+        <f t="shared" si="22"/>
+        <v>89.23</v>
+      </c>
+      <c r="L184" s="2">
+        <f t="shared" si="23"/>
+        <v>10.77</v>
+      </c>
+      <c r="M184" s="2">
+        <f t="shared" si="24"/>
+        <v>56.46</v>
+      </c>
+      <c r="N184" s="2">
+        <f t="shared" si="25"/>
+        <v>9.57</v>
+      </c>
+      <c r="O184" s="2">
+        <f t="shared" si="26"/>
+        <v>23.21</v>
+      </c>
+      <c r="P184" s="2">
+        <f t="shared" si="27"/>
+        <v>10.759999999999991</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A185" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C185" s="6">
+        <v>322</v>
+      </c>
+      <c r="D185" s="6">
+        <v>60</v>
+      </c>
+      <c r="E185" s="6">
+        <v>20</v>
+      </c>
+      <c r="F185" s="6">
+        <v>382</v>
+      </c>
+      <c r="G185" s="6">
+        <v>44</v>
+      </c>
+      <c r="H185" s="6">
+        <v>236</v>
+      </c>
+      <c r="I185" s="6">
+        <v>42</v>
+      </c>
+      <c r="J185" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K185" s="2">
+        <f t="shared" si="22"/>
+        <v>84.29</v>
+      </c>
+      <c r="L185" s="2">
+        <f t="shared" si="23"/>
+        <v>15.71</v>
+      </c>
+      <c r="M185" s="2">
+        <f t="shared" si="24"/>
+        <v>61.78</v>
+      </c>
+      <c r="N185" s="2">
+        <f t="shared" si="25"/>
+        <v>11.52</v>
+      </c>
+      <c r="O185" s="2">
+        <f t="shared" si="26"/>
+        <v>10.99</v>
+      </c>
+      <c r="P185" s="2">
+        <f t="shared" si="27"/>
+        <v>15.710000000000008</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A186" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C186" s="6">
+        <v>235</v>
+      </c>
+      <c r="D186" s="6">
+        <v>16</v>
+      </c>
+      <c r="E186" s="6">
+        <v>18</v>
+      </c>
+      <c r="F186" s="6">
+        <v>251</v>
+      </c>
+      <c r="G186" s="6">
+        <v>43</v>
+      </c>
+      <c r="H186" s="6">
+        <v>135</v>
+      </c>
+      <c r="I186" s="6">
+        <v>57</v>
+      </c>
+      <c r="J186" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K186" s="2">
+        <f t="shared" si="22"/>
+        <v>93.63</v>
+      </c>
+      <c r="L186" s="2">
+        <f t="shared" si="23"/>
+        <v>6.37</v>
+      </c>
+      <c r="M186" s="2">
+        <f t="shared" si="24"/>
+        <v>53.78</v>
+      </c>
+      <c r="N186" s="2">
+        <f t="shared" si="25"/>
+        <v>17.13</v>
+      </c>
+      <c r="O186" s="2">
+        <f t="shared" si="26"/>
+        <v>22.71</v>
+      </c>
+      <c r="P186" s="2">
+        <f t="shared" si="27"/>
+        <v>6.3799999999999955</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A187" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C187" s="6">
+        <v>343</v>
+      </c>
+      <c r="D187" s="6">
+        <v>44</v>
+      </c>
+      <c r="E187" s="6">
+        <v>31</v>
+      </c>
+      <c r="F187" s="6">
+        <v>387</v>
+      </c>
+      <c r="G187" s="6">
+        <v>77</v>
+      </c>
+      <c r="H187" s="6">
+        <v>207</v>
+      </c>
+      <c r="I187" s="6">
+        <v>59</v>
+      </c>
+      <c r="J187" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K187" s="2">
+        <f t="shared" si="22"/>
+        <v>88.63</v>
+      </c>
+      <c r="L187" s="2">
+        <f t="shared" si="23"/>
+        <v>11.37</v>
+      </c>
+      <c r="M187" s="2">
+        <f t="shared" si="24"/>
+        <v>53.49</v>
+      </c>
+      <c r="N187" s="2">
+        <f t="shared" si="25"/>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="O187" s="2">
+        <f t="shared" si="26"/>
+        <v>15.25</v>
+      </c>
+      <c r="P187" s="2">
+        <f t="shared" si="27"/>
+        <v>11.36</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A188" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C188" s="6">
+        <v>398</v>
+      </c>
+      <c r="D188" s="6">
+        <v>47</v>
+      </c>
+      <c r="E188" s="6">
+        <v>28</v>
+      </c>
+      <c r="F188" s="6">
+        <v>445</v>
+      </c>
+      <c r="G188" s="6">
+        <v>70</v>
+      </c>
+      <c r="H188" s="6">
+        <v>245</v>
+      </c>
+      <c r="I188" s="6">
+        <v>83</v>
+      </c>
+      <c r="J188" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K188" s="2">
+        <f t="shared" si="22"/>
+        <v>89.44</v>
+      </c>
+      <c r="L188" s="2">
+        <f t="shared" si="23"/>
+        <v>10.56</v>
+      </c>
+      <c r="M188" s="2">
+        <f t="shared" si="24"/>
+        <v>55.06</v>
+      </c>
+      <c r="N188" s="2">
+        <f t="shared" si="25"/>
+        <v>15.73</v>
+      </c>
+      <c r="O188" s="2">
+        <f t="shared" si="26"/>
+        <v>18.649999999999999</v>
+      </c>
+      <c r="P188" s="2">
+        <f t="shared" si="27"/>
+        <v>10.560000000000002</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A189" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C189" s="6">
+        <v>319</v>
+      </c>
+      <c r="D189" s="6">
+        <v>40</v>
+      </c>
+      <c r="E189" s="6">
+        <v>24</v>
+      </c>
+      <c r="F189" s="6">
+        <v>359</v>
+      </c>
+      <c r="G189" s="6">
+        <v>69</v>
+      </c>
+      <c r="H189" s="6">
+        <v>176</v>
+      </c>
+      <c r="I189" s="6">
+        <v>74</v>
+      </c>
+      <c r="J189" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K189" s="2">
+        <f t="shared" si="22"/>
+        <v>88.86</v>
+      </c>
+      <c r="L189" s="2">
+        <f t="shared" si="23"/>
+        <v>11.14</v>
+      </c>
+      <c r="M189" s="2">
+        <f t="shared" si="24"/>
+        <v>49.03</v>
+      </c>
+      <c r="N189" s="2">
+        <f t="shared" si="25"/>
+        <v>19.22</v>
+      </c>
+      <c r="O189" s="2">
+        <f t="shared" si="26"/>
+        <v>20.61</v>
+      </c>
+      <c r="P189" s="2">
+        <f t="shared" si="27"/>
+        <v>11.14</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A190" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C190" s="6">
+        <v>388</v>
+      </c>
+      <c r="D190" s="6">
+        <v>52</v>
+      </c>
+      <c r="E190" s="6">
+        <v>32</v>
+      </c>
+      <c r="F190" s="6">
+        <v>440</v>
+      </c>
+      <c r="G190" s="6">
+        <v>88</v>
+      </c>
+      <c r="H190" s="6">
+        <v>218</v>
+      </c>
+      <c r="I190" s="6">
+        <v>82</v>
+      </c>
+      <c r="J190" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K190" s="2">
+        <f t="shared" si="22"/>
+        <v>88.18</v>
+      </c>
+      <c r="L190" s="2">
+        <f t="shared" si="23"/>
+        <v>11.82</v>
+      </c>
+      <c r="M190" s="2">
+        <f t="shared" si="24"/>
+        <v>49.55</v>
+      </c>
+      <c r="N190" s="2">
+        <f t="shared" si="25"/>
+        <v>20</v>
+      </c>
+      <c r="O190" s="2">
+        <f t="shared" si="26"/>
+        <v>18.64</v>
+      </c>
+      <c r="P190" s="2">
+        <f t="shared" si="27"/>
+        <v>11.810000000000002</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A191" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C191" s="6">
+        <v>333</v>
+      </c>
+      <c r="D191" s="6">
+        <v>39</v>
+      </c>
+      <c r="E191" s="6">
+        <v>20</v>
+      </c>
+      <c r="F191" s="6">
+        <v>372</v>
+      </c>
+      <c r="G191" s="6">
+        <v>35</v>
+      </c>
+      <c r="H191" s="6">
+        <v>221</v>
+      </c>
+      <c r="I191" s="6">
+        <v>77</v>
+      </c>
+      <c r="J191" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K191" s="2">
+        <f t="shared" si="22"/>
+        <v>89.52</v>
+      </c>
+      <c r="L191" s="2">
+        <f t="shared" si="23"/>
+        <v>10.48</v>
+      </c>
+      <c r="M191" s="2">
+        <f t="shared" si="24"/>
+        <v>59.41</v>
+      </c>
+      <c r="N191" s="2">
+        <f t="shared" si="25"/>
+        <v>9.41</v>
+      </c>
+      <c r="O191" s="2">
+        <f t="shared" si="26"/>
+        <v>20.7</v>
+      </c>
+      <c r="P191" s="2">
+        <f t="shared" si="27"/>
+        <v>10.480000000000004</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A192" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C192" s="6">
+        <v>320</v>
+      </c>
+      <c r="D192" s="6">
+        <v>57</v>
+      </c>
+      <c r="E192" s="6">
+        <v>28</v>
+      </c>
+      <c r="F192" s="6">
+        <v>377</v>
+      </c>
+      <c r="G192" s="6">
+        <v>65</v>
+      </c>
+      <c r="H192" s="6">
+        <v>162</v>
+      </c>
+      <c r="I192" s="6">
+        <v>93</v>
+      </c>
+      <c r="J192" t="str">
+        <f t="shared" si="21"/>
+        <v>No</v>
+      </c>
+      <c r="K192" s="2">
+        <f t="shared" si="22"/>
+        <v>84.88</v>
+      </c>
+      <c r="L192" s="2">
+        <f t="shared" si="23"/>
+        <v>15.12</v>
+      </c>
+      <c r="M192" s="2">
+        <f t="shared" si="24"/>
+        <v>42.97</v>
+      </c>
+      <c r="N192" s="2">
+        <f t="shared" si="25"/>
+        <v>17.239999999999998</v>
+      </c>
+      <c r="O192" s="2">
+        <f t="shared" si="26"/>
+        <v>24.67</v>
+      </c>
+      <c r="P192" s="2">
+        <f t="shared" si="27"/>
+        <v>15.120000000000005</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A193" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C193" s="6">
+        <v>396</v>
+      </c>
+      <c r="D193" s="6">
+        <v>25</v>
+      </c>
+      <c r="E193" s="6">
+        <v>3</v>
+      </c>
+      <c r="F193" s="6">
+        <v>425</v>
+      </c>
+      <c r="G193" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H193" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I193" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J193" t="str">
+        <f t="shared" ref="J193:J211" si="28">IF(C193&gt;=420,"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="K193" s="2">
+        <f t="shared" ref="K193:K211" si="29">ROUND((C193/F193)*100, 2)</f>
+        <v>93.18</v>
+      </c>
+      <c r="L193" s="2">
+        <f t="shared" ref="L193:L211" si="30">ROUND((D193/F193)*100,2)</f>
+        <v>5.88</v>
+      </c>
+      <c r="M193" s="2" t="e">
+        <f t="shared" ref="M193:M211" si="31">ROUND((H193/F193)*100,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N193" s="2" t="e">
+        <f t="shared" ref="N193:N211" si="32">ROUND((G193/F193)*100,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O193" s="2" t="e">
+        <f t="shared" ref="O193:O211" si="33">ROUND((I193/F193)*100,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P193" s="2" t="e">
+        <f t="shared" ref="P193:P211" si="34">100-(O193+N193+M193)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A194" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C194" s="6">
+        <v>340</v>
+      </c>
+      <c r="D194" s="6">
+        <v>49</v>
+      </c>
+      <c r="E194" s="6">
+        <v>21</v>
+      </c>
+      <c r="F194" s="6">
+        <v>389</v>
+      </c>
+      <c r="G194" s="6">
+        <v>62</v>
+      </c>
+      <c r="H194" s="6">
+        <v>193</v>
+      </c>
+      <c r="I194" s="6">
+        <v>85</v>
+      </c>
+      <c r="J194" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K194" s="2">
+        <f t="shared" si="29"/>
+        <v>87.4</v>
+      </c>
+      <c r="L194" s="2">
+        <f t="shared" si="30"/>
+        <v>12.6</v>
+      </c>
+      <c r="M194" s="2">
+        <f t="shared" si="31"/>
+        <v>49.61</v>
+      </c>
+      <c r="N194" s="2">
+        <f t="shared" si="32"/>
+        <v>15.94</v>
+      </c>
+      <c r="O194" s="2">
+        <f t="shared" si="33"/>
+        <v>21.85</v>
+      </c>
+      <c r="P194" s="2">
+        <f t="shared" si="34"/>
+        <v>12.599999999999994</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A195" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C195" s="6">
+        <v>291</v>
+      </c>
+      <c r="D195" s="6">
+        <v>46</v>
+      </c>
+      <c r="E195" s="6">
+        <v>20</v>
+      </c>
+      <c r="F195" s="6">
+        <v>337</v>
+      </c>
+      <c r="G195" s="6">
+        <v>31</v>
+      </c>
+      <c r="H195" s="6">
+        <v>173</v>
+      </c>
+      <c r="I195" s="6">
+        <v>87</v>
+      </c>
+      <c r="J195" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K195" s="2">
+        <f t="shared" si="29"/>
+        <v>86.35</v>
+      </c>
+      <c r="L195" s="2">
+        <f t="shared" si="30"/>
+        <v>13.65</v>
+      </c>
+      <c r="M195" s="2">
+        <f t="shared" si="31"/>
+        <v>51.34</v>
+      </c>
+      <c r="N195" s="2">
+        <f t="shared" si="32"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="O195" s="2">
+        <f t="shared" si="33"/>
+        <v>25.82</v>
+      </c>
+      <c r="P195" s="2">
+        <f t="shared" si="34"/>
+        <v>13.64</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A196" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C196" s="6">
+        <v>342</v>
+      </c>
+      <c r="D196" s="6">
+        <v>33</v>
+      </c>
+      <c r="E196" s="6">
+        <v>25</v>
+      </c>
+      <c r="F196" s="6">
+        <v>375</v>
+      </c>
+      <c r="G196" s="6">
+        <v>49</v>
+      </c>
+      <c r="H196" s="6">
+        <v>196</v>
+      </c>
+      <c r="I196" s="6">
+        <v>97</v>
+      </c>
+      <c r="J196" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K196" s="2">
+        <f t="shared" si="29"/>
+        <v>91.2</v>
+      </c>
+      <c r="L196" s="2">
+        <f t="shared" si="30"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="M196" s="2">
+        <f t="shared" si="31"/>
+        <v>52.27</v>
+      </c>
+      <c r="N196" s="2">
+        <f t="shared" si="32"/>
+        <v>13.07</v>
+      </c>
+      <c r="O196" s="2">
+        <f t="shared" si="33"/>
+        <v>25.87</v>
+      </c>
+      <c r="P196" s="2">
+        <f t="shared" si="34"/>
+        <v>8.789999999999992</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A197" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C197" s="6">
+        <v>335</v>
+      </c>
+      <c r="D197" s="6">
+        <v>46</v>
+      </c>
+      <c r="E197" s="6">
+        <v>26</v>
+      </c>
+      <c r="F197" s="6">
+        <v>381</v>
+      </c>
+      <c r="G197" s="6">
+        <v>30</v>
+      </c>
+      <c r="H197" s="6">
+        <v>220</v>
+      </c>
+      <c r="I197" s="6">
+        <v>85</v>
+      </c>
+      <c r="J197" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K197" s="2">
+        <f t="shared" si="29"/>
+        <v>87.93</v>
+      </c>
+      <c r="L197" s="2">
+        <f t="shared" si="30"/>
+        <v>12.07</v>
+      </c>
+      <c r="M197" s="2">
+        <f t="shared" si="31"/>
+        <v>57.74</v>
+      </c>
+      <c r="N197" s="2">
+        <f t="shared" si="32"/>
+        <v>7.87</v>
+      </c>
+      <c r="O197" s="2">
+        <f t="shared" si="33"/>
+        <v>22.31</v>
+      </c>
+      <c r="P197" s="2">
+        <f t="shared" si="34"/>
+        <v>12.079999999999998</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A198" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C198" s="6">
+        <v>343</v>
+      </c>
+      <c r="D198" s="6">
+        <v>26</v>
+      </c>
+      <c r="E198" s="6">
+        <v>23</v>
+      </c>
+      <c r="F198" s="6">
+        <v>369</v>
+      </c>
+      <c r="G198" s="6">
+        <v>68</v>
+      </c>
+      <c r="H198" s="6">
+        <v>199</v>
+      </c>
+      <c r="I198" s="6">
+        <v>76</v>
+      </c>
+      <c r="J198" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K198" s="2">
+        <f t="shared" si="29"/>
+        <v>92.95</v>
+      </c>
+      <c r="L198" s="2">
+        <f t="shared" si="30"/>
+        <v>7.05</v>
+      </c>
+      <c r="M198" s="2">
+        <f t="shared" si="31"/>
+        <v>53.93</v>
+      </c>
+      <c r="N198" s="2">
+        <f t="shared" si="32"/>
+        <v>18.43</v>
+      </c>
+      <c r="O198" s="2">
+        <f t="shared" si="33"/>
+        <v>20.6</v>
+      </c>
+      <c r="P198" s="2">
+        <f t="shared" si="34"/>
+        <v>7.039999999999992</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A199" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C199" s="6">
+        <v>340</v>
+      </c>
+      <c r="D199" s="6">
+        <v>39</v>
+      </c>
+      <c r="E199" s="6">
+        <v>23</v>
+      </c>
+      <c r="F199" s="6">
+        <v>379</v>
+      </c>
+      <c r="G199" s="6">
+        <v>54</v>
+      </c>
+      <c r="H199" s="6">
+        <v>204</v>
+      </c>
+      <c r="I199" s="6">
+        <v>82</v>
+      </c>
+      <c r="J199" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K199" s="2">
+        <f t="shared" si="29"/>
+        <v>89.71</v>
+      </c>
+      <c r="L199" s="2">
+        <f t="shared" si="30"/>
+        <v>10.29</v>
+      </c>
+      <c r="M199" s="2">
+        <f t="shared" si="31"/>
+        <v>53.83</v>
+      </c>
+      <c r="N199" s="2">
+        <f t="shared" si="32"/>
+        <v>14.25</v>
+      </c>
+      <c r="O199" s="2">
+        <f t="shared" si="33"/>
+        <v>21.64</v>
+      </c>
+      <c r="P199" s="2">
+        <f t="shared" si="34"/>
+        <v>10.280000000000001</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A200" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C200" s="6">
+        <v>391</v>
+      </c>
+      <c r="D200" s="6">
+        <v>39</v>
+      </c>
+      <c r="E200" s="6">
+        <v>18</v>
+      </c>
+      <c r="F200" s="6">
+        <v>430</v>
+      </c>
+      <c r="G200" s="6">
+        <v>109</v>
+      </c>
+      <c r="H200" s="6">
+        <v>189</v>
+      </c>
+      <c r="I200" s="6">
+        <v>93</v>
+      </c>
+      <c r="J200" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K200" s="2">
+        <f t="shared" si="29"/>
+        <v>90.93</v>
+      </c>
+      <c r="L200" s="2">
+        <f t="shared" si="30"/>
+        <v>9.07</v>
+      </c>
+      <c r="M200" s="2">
+        <f t="shared" si="31"/>
+        <v>43.95</v>
+      </c>
+      <c r="N200" s="2">
+        <f t="shared" si="32"/>
+        <v>25.35</v>
+      </c>
+      <c r="O200" s="2">
+        <f t="shared" si="33"/>
+        <v>21.63</v>
+      </c>
+      <c r="P200" s="2">
+        <f t="shared" si="34"/>
+        <v>9.0699999999999932</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A201" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C201" s="6">
+        <v>384</v>
+      </c>
+      <c r="D201" s="6">
+        <v>43</v>
+      </c>
+      <c r="E201" s="6">
+        <v>27</v>
+      </c>
+      <c r="F201" s="6">
+        <v>427</v>
+      </c>
+      <c r="G201" s="6">
+        <v>58</v>
+      </c>
+      <c r="H201" s="6">
+        <v>252</v>
+      </c>
+      <c r="I201" s="6">
+        <v>74</v>
+      </c>
+      <c r="J201" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K201" s="2">
+        <f t="shared" si="29"/>
+        <v>89.93</v>
+      </c>
+      <c r="L201" s="2">
+        <f t="shared" si="30"/>
+        <v>10.07</v>
+      </c>
+      <c r="M201" s="2">
+        <f t="shared" si="31"/>
+        <v>59.02</v>
+      </c>
+      <c r="N201" s="2">
+        <f t="shared" si="32"/>
+        <v>13.58</v>
+      </c>
+      <c r="O201" s="2">
+        <f t="shared" si="33"/>
+        <v>17.329999999999998</v>
+      </c>
+      <c r="P201" s="2">
+        <f t="shared" si="34"/>
+        <v>10.069999999999993</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A202" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C202" s="6">
+        <v>425</v>
+      </c>
+      <c r="D202" s="6">
+        <v>84</v>
+      </c>
+      <c r="E202" s="6">
+        <v>29</v>
+      </c>
+      <c r="F202" s="6">
+        <v>509</v>
+      </c>
+      <c r="G202" s="6">
+        <v>53</v>
+      </c>
+      <c r="H202" s="6">
+        <v>248</v>
+      </c>
+      <c r="I202" s="6">
+        <v>124</v>
+      </c>
+      <c r="J202" t="str">
+        <f t="shared" si="28"/>
+        <v>Yes</v>
+      </c>
+      <c r="K202" s="2">
+        <f t="shared" si="29"/>
+        <v>83.5</v>
+      </c>
+      <c r="L202" s="2">
+        <f t="shared" si="30"/>
+        <v>16.5</v>
+      </c>
+      <c r="M202" s="2">
+        <f t="shared" si="31"/>
+        <v>48.72</v>
+      </c>
+      <c r="N202" s="2">
+        <f t="shared" si="32"/>
+        <v>10.41</v>
+      </c>
+      <c r="O202" s="2">
+        <f t="shared" si="33"/>
+        <v>24.36</v>
+      </c>
+      <c r="P202" s="2">
+        <f t="shared" si="34"/>
+        <v>16.510000000000005</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A203" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B203" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C203" s="6">
+        <v>425</v>
+      </c>
+      <c r="D203" s="6">
+        <v>44</v>
+      </c>
+      <c r="E203" s="6">
+        <v>31</v>
+      </c>
+      <c r="F203" s="6">
+        <v>469</v>
+      </c>
+      <c r="G203" s="6">
+        <v>64</v>
+      </c>
+      <c r="H203" s="6">
+        <v>287</v>
+      </c>
+      <c r="I203" s="6">
+        <v>74</v>
+      </c>
+      <c r="J203" t="str">
+        <f t="shared" si="28"/>
+        <v>Yes</v>
+      </c>
+      <c r="K203" s="2">
+        <f t="shared" si="29"/>
+        <v>90.62</v>
+      </c>
+      <c r="L203" s="2">
+        <f t="shared" si="30"/>
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="M203" s="2">
+        <f t="shared" si="31"/>
+        <v>61.19</v>
+      </c>
+      <c r="N203" s="2">
+        <f t="shared" si="32"/>
+        <v>13.65</v>
+      </c>
+      <c r="O203" s="2">
+        <f t="shared" si="33"/>
+        <v>15.78</v>
+      </c>
+      <c r="P203" s="2">
+        <f t="shared" si="34"/>
+        <v>9.3799999999999955</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A204" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C204" s="6">
+        <v>395</v>
+      </c>
+      <c r="D204" s="6">
+        <v>38</v>
+      </c>
+      <c r="E204" s="6">
+        <v>26</v>
+      </c>
+      <c r="F204" s="6">
+        <v>433</v>
+      </c>
+      <c r="G204" s="6">
+        <v>77</v>
+      </c>
+      <c r="H204" s="6">
+        <v>212</v>
+      </c>
+      <c r="I204" s="6">
+        <v>106</v>
+      </c>
+      <c r="J204" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K204" s="2">
+        <f t="shared" si="29"/>
+        <v>91.22</v>
+      </c>
+      <c r="L204" s="2">
+        <f t="shared" si="30"/>
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="M204" s="2">
+        <f t="shared" si="31"/>
+        <v>48.96</v>
+      </c>
+      <c r="N204" s="2">
+        <f t="shared" si="32"/>
+        <v>17.78</v>
+      </c>
+      <c r="O204" s="2">
+        <f t="shared" si="33"/>
+        <v>24.48</v>
+      </c>
+      <c r="P204" s="2">
+        <f t="shared" si="34"/>
+        <v>8.7800000000000011</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A205" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C205" s="6">
+        <v>276</v>
+      </c>
+      <c r="D205" s="6">
+        <v>26</v>
+      </c>
+      <c r="E205" s="6">
+        <v>30</v>
+      </c>
+      <c r="F205" s="6">
+        <v>302</v>
+      </c>
+      <c r="G205" s="6">
+        <v>17</v>
+      </c>
+      <c r="H205" s="6">
+        <v>195</v>
+      </c>
+      <c r="I205" s="6">
+        <v>64</v>
+      </c>
+      <c r="J205" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K205" s="2">
+        <f t="shared" si="29"/>
+        <v>91.39</v>
+      </c>
+      <c r="L205" s="2">
+        <f t="shared" si="30"/>
+        <v>8.61</v>
+      </c>
+      <c r="M205" s="2">
+        <f t="shared" si="31"/>
+        <v>64.569999999999993</v>
+      </c>
+      <c r="N205" s="2">
+        <f t="shared" si="32"/>
+        <v>5.63</v>
+      </c>
+      <c r="O205" s="2">
+        <f t="shared" si="33"/>
+        <v>21.19</v>
+      </c>
+      <c r="P205" s="2">
+        <f t="shared" si="34"/>
+        <v>8.6100000000000136</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A206" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C206" s="6">
+        <v>443</v>
+      </c>
+      <c r="D206" s="6">
+        <v>114</v>
+      </c>
+      <c r="E206" s="6">
+        <v>28</v>
+      </c>
+      <c r="F206" s="6">
+        <v>557</v>
+      </c>
+      <c r="G206" s="6">
+        <v>85</v>
+      </c>
+      <c r="H206" s="6">
+        <v>232</v>
+      </c>
+      <c r="I206" s="6">
+        <v>126</v>
+      </c>
+      <c r="J206" t="str">
+        <f t="shared" si="28"/>
+        <v>Yes</v>
+      </c>
+      <c r="K206" s="2">
+        <f t="shared" si="29"/>
+        <v>79.53</v>
+      </c>
+      <c r="L206" s="2">
+        <f t="shared" si="30"/>
+        <v>20.47</v>
+      </c>
+      <c r="M206" s="2">
+        <f t="shared" si="31"/>
+        <v>41.65</v>
+      </c>
+      <c r="N206" s="2">
+        <f t="shared" si="32"/>
+        <v>15.26</v>
+      </c>
+      <c r="O206" s="2">
+        <f t="shared" si="33"/>
+        <v>22.62</v>
+      </c>
+      <c r="P206" s="2">
+        <f t="shared" si="34"/>
+        <v>20.47</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A207" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C207" s="6">
+        <v>385</v>
+      </c>
+      <c r="D207" s="6">
+        <v>39</v>
+      </c>
+      <c r="E207" s="6">
+        <v>26</v>
+      </c>
+      <c r="F207" s="6">
+        <v>424</v>
+      </c>
+      <c r="G207" s="6">
+        <v>76</v>
+      </c>
+      <c r="H207" s="6">
+        <v>203</v>
+      </c>
+      <c r="I207" s="6">
+        <v>106</v>
+      </c>
+      <c r="J207" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K207" s="2">
+        <f t="shared" si="29"/>
+        <v>90.8</v>
+      </c>
+      <c r="L207" s="2">
+        <f t="shared" si="30"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="M207" s="2">
+        <f t="shared" si="31"/>
+        <v>47.88</v>
+      </c>
+      <c r="N207" s="2">
+        <f t="shared" si="32"/>
+        <v>17.920000000000002</v>
+      </c>
+      <c r="O207" s="2">
+        <f t="shared" si="33"/>
+        <v>25</v>
+      </c>
+      <c r="P207" s="2">
+        <f t="shared" si="34"/>
+        <v>9.1999999999999886</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A208" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C208" s="6">
+        <v>357</v>
+      </c>
+      <c r="D208" s="6">
+        <v>55</v>
+      </c>
+      <c r="E208" s="6">
+        <v>31</v>
+      </c>
+      <c r="F208" s="6">
+        <v>412</v>
+      </c>
+      <c r="G208" s="6">
+        <v>50</v>
+      </c>
+      <c r="H208" s="6">
+        <v>225</v>
+      </c>
+      <c r="I208" s="6">
+        <v>82</v>
+      </c>
+      <c r="J208" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K208" s="2">
+        <f t="shared" si="29"/>
+        <v>86.65</v>
+      </c>
+      <c r="L208" s="2">
+        <f t="shared" si="30"/>
+        <v>13.35</v>
+      </c>
+      <c r="M208" s="2">
+        <f t="shared" si="31"/>
+        <v>54.61</v>
+      </c>
+      <c r="N208" s="2">
+        <f t="shared" si="32"/>
+        <v>12.14</v>
+      </c>
+      <c r="O208" s="2">
+        <f t="shared" si="33"/>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="P208" s="2">
+        <f t="shared" si="34"/>
+        <v>13.349999999999994</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A209" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C209" s="6">
+        <v>335</v>
+      </c>
+      <c r="D209" s="6">
+        <v>36</v>
+      </c>
+      <c r="E209" s="6">
+        <v>26</v>
+      </c>
+      <c r="F209" s="6">
+        <v>371</v>
+      </c>
+      <c r="G209" s="6">
+        <v>54</v>
+      </c>
+      <c r="H209" s="6">
+        <v>197</v>
+      </c>
+      <c r="I209" s="6">
+        <v>84</v>
+      </c>
+      <c r="J209" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K209" s="2">
+        <f t="shared" si="29"/>
+        <v>90.3</v>
+      </c>
+      <c r="L209" s="2">
+        <f t="shared" si="30"/>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="M209" s="2">
+        <f t="shared" si="31"/>
+        <v>53.1</v>
+      </c>
+      <c r="N209" s="2">
+        <f t="shared" si="32"/>
+        <v>14.56</v>
+      </c>
+      <c r="O209" s="2">
+        <f t="shared" si="33"/>
+        <v>22.64</v>
+      </c>
+      <c r="P209" s="2">
+        <f t="shared" si="34"/>
+        <v>9.6999999999999886</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A210" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B210" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C210" s="6">
+        <v>423</v>
+      </c>
+      <c r="D210" s="6">
+        <v>47</v>
+      </c>
+      <c r="E210" s="6">
+        <v>35</v>
+      </c>
+      <c r="F210" s="6">
+        <v>470</v>
+      </c>
+      <c r="G210" s="6">
+        <v>77</v>
+      </c>
+      <c r="H210" s="6">
+        <v>258</v>
+      </c>
+      <c r="I210" s="6">
+        <v>88</v>
+      </c>
+      <c r="J210" t="str">
+        <f t="shared" si="28"/>
+        <v>Yes</v>
+      </c>
+      <c r="K210" s="2">
+        <f t="shared" si="29"/>
+        <v>90</v>
+      </c>
+      <c r="L210" s="2">
+        <f t="shared" si="30"/>
+        <v>10</v>
+      </c>
+      <c r="M210" s="2">
+        <f t="shared" si="31"/>
+        <v>54.89</v>
+      </c>
+      <c r="N210" s="2">
+        <f t="shared" si="32"/>
+        <v>16.38</v>
+      </c>
+      <c r="O210" s="2">
+        <f t="shared" si="33"/>
+        <v>18.72</v>
+      </c>
+      <c r="P210" s="2">
+        <f t="shared" si="34"/>
+        <v>10.010000000000005</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A211" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B211" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C211" s="6">
+        <v>384</v>
+      </c>
+      <c r="D211" s="6">
+        <v>33</v>
+      </c>
+      <c r="E211" s="6">
+        <v>25</v>
+      </c>
+      <c r="F211" s="6">
+        <v>417</v>
+      </c>
+      <c r="G211" s="6">
+        <v>78</v>
+      </c>
+      <c r="H211" s="6">
+        <v>216</v>
+      </c>
+      <c r="I211" s="6">
+        <v>90</v>
+      </c>
+      <c r="J211" t="str">
+        <f t="shared" si="28"/>
+        <v>No</v>
+      </c>
+      <c r="K211" s="2">
+        <f t="shared" si="29"/>
+        <v>92.09</v>
+      </c>
+      <c r="L211" s="2">
+        <f t="shared" si="30"/>
+        <v>7.91</v>
+      </c>
+      <c r="M211" s="2">
+        <f t="shared" si="31"/>
+        <v>51.8</v>
+      </c>
+      <c r="N211" s="2">
+        <f t="shared" si="32"/>
+        <v>18.71</v>
+      </c>
+      <c r="O211" s="2">
+        <f t="shared" si="33"/>
+        <v>21.58</v>
+      </c>
+      <c r="P211" s="2">
+        <f t="shared" si="34"/>
+        <v>7.9099999999999966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reformatting start and end time column in TotalSleep files. Adding summary statistics to each dataset in Jupyter. Finished data cleaning TotalSleep dataset in Jupyter
</commit_message>
<xml_diff>
--- a/datasets/TotalSleep.xlsx
+++ b/datasets/TotalSleep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DF64D75-56E8-494D-BC2C-AF6D2C800D78}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB5317D2-C76E-479E-B958-5B856DF26908}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Start Time</t>
   </si>
@@ -70,511 +70,16 @@
     <t>% Unclassified</t>
   </si>
   <si>
-    <t>01-02-2018 9:53 pm</t>
-  </si>
-  <si>
-    <t>02-02-2018 4:42 am</t>
-  </si>
-  <si>
-    <t>02-02-2018 9:59 pm</t>
-  </si>
-  <si>
-    <t>03-02-2018 4:44 am</t>
-  </si>
-  <si>
-    <t>04-02-2018 10:14 pm</t>
-  </si>
-  <si>
-    <t>05-02-2018 4:01 am</t>
-  </si>
-  <si>
-    <t>04-02-2018 12:30 am</t>
-  </si>
-  <si>
-    <t>04-02-2018 6:03 am</t>
-  </si>
-  <si>
-    <t>05-02-2018 9:27 pm</t>
-  </si>
-  <si>
-    <t>06-02-2018 5:10 am</t>
-  </si>
-  <si>
-    <t>06-02-2018 9:12 pm</t>
-  </si>
-  <si>
-    <t>07-02-2018 2:04 am</t>
-  </si>
-  <si>
-    <t>07-02-2018 9:08 pm</t>
-  </si>
-  <si>
-    <t>08-02-2018 2:45 am</t>
-  </si>
-  <si>
-    <t>08-02-2018 8:47 pm</t>
-  </si>
-  <si>
-    <t>09-02-2018 4:16 am</t>
-  </si>
-  <si>
-    <t>09-02-2018 9:48 pm</t>
-  </si>
-  <si>
-    <t>10-02-2018 5:48 am</t>
-  </si>
-  <si>
-    <t>10-02-2018 8:25 pm</t>
-  </si>
-  <si>
-    <t>11-02-2018 4:27 am</t>
-  </si>
-  <si>
-    <t>11-02-2018 9:27 pm</t>
-  </si>
-  <si>
-    <t>12-02-2018 3:54 am</t>
-  </si>
-  <si>
-    <t>14-02-2018 9:13 pm</t>
-  </si>
-  <si>
-    <t>15-02-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>15-02-2018 9:50 pm</t>
-  </si>
-  <si>
-    <t>16-02-2018 4:07 am</t>
-  </si>
-  <si>
-    <t>16-02-2018 10:18 pm</t>
-  </si>
-  <si>
-    <t>17-02-2018 5:13 am</t>
-  </si>
-  <si>
-    <t>17-02-2018 10:12 pm</t>
-  </si>
-  <si>
-    <t>18-02-2018 5:08 am</t>
-  </si>
-  <si>
-    <t>18-02-2018 10:31 pm</t>
-  </si>
-  <si>
-    <t>19-02-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>19-02-2018 9:51 pm</t>
-  </si>
-  <si>
-    <t>20-02-2018 4:28 am</t>
-  </si>
-  <si>
-    <t>20-02-2018 11:00 pm</t>
-  </si>
-  <si>
-    <t>21-02-2018 5:05 am</t>
-  </si>
-  <si>
-    <t>21-02-2018 10:44 pm</t>
-  </si>
-  <si>
-    <t>22-02-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>22-02-2018 9:27 pm</t>
-  </si>
-  <si>
-    <t>23-02-2018 4:56 am</t>
-  </si>
-  <si>
-    <t>23-02-2018 9:53 pm</t>
-  </si>
-  <si>
-    <t>24-02-2018 6:02 am</t>
-  </si>
-  <si>
-    <t>25-02-2018 3:18 am</t>
-  </si>
-  <si>
-    <t>25-02-2018 9:04 am</t>
-  </si>
-  <si>
-    <t>25-02-2018 9:55 pm</t>
-  </si>
-  <si>
-    <t>26-02-2018 5:04 am</t>
-  </si>
-  <si>
-    <t>26-02-2018 9:54 pm</t>
-  </si>
-  <si>
-    <t>27-02-2018 4:51 am</t>
-  </si>
-  <si>
-    <t>27-02-2018 10:06 pm</t>
-  </si>
-  <si>
-    <t>28-02-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>28-02-2018 10:06 pm</t>
-  </si>
-  <si>
-    <t>01-03-2018 5:04 am</t>
-  </si>
-  <si>
-    <t>01-03-2018 10:04 pm</t>
-  </si>
-  <si>
-    <t>02-03-2018 5:02 am</t>
-  </si>
-  <si>
-    <t>02-03-2018 11:45 pm</t>
-  </si>
-  <si>
-    <t>03-03-2018 6:05 am</t>
-  </si>
-  <si>
-    <t>03-03-2018 9:11 pm</t>
-  </si>
-  <si>
-    <t>04-03-2018 5:29 am</t>
-  </si>
-  <si>
-    <t>04-03-2018 10:25 pm</t>
-  </si>
-  <si>
-    <t>05-03-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>05-03-2018 9:43 pm</t>
-  </si>
-  <si>
-    <t>06-03-2018 5:00 am</t>
-  </si>
-  <si>
-    <t>06-03-2018 9:54 pm</t>
-  </si>
-  <si>
-    <t>07-03-2018 4:59 am</t>
-  </si>
-  <si>
-    <t>07-03-2018 9:59 pm</t>
-  </si>
-  <si>
-    <t>08-03-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>08-03-2018 9:48 pm</t>
-  </si>
-  <si>
-    <t>09-03-2018 4:59 am</t>
-  </si>
-  <si>
-    <t>09-03-2018 10:46 pm</t>
-  </si>
-  <si>
-    <t>10-03-2018 7:57 am</t>
-  </si>
-  <si>
-    <t>10-03-2018 9:47 pm</t>
-  </si>
-  <si>
-    <t>11-03-2018 6:20 am</t>
-  </si>
-  <si>
-    <t>11-03-2018 9:11 pm</t>
-  </si>
-  <si>
-    <t>12-03-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>12-03-2018 9:40 pm</t>
-  </si>
-  <si>
-    <t>13-03-2018 5:01 am</t>
-  </si>
-  <si>
-    <t>13-03-2018 10:07 pm</t>
-  </si>
-  <si>
-    <t>14-03-2018 5:05 am</t>
-  </si>
-  <si>
-    <t>14-03-2018 9:10 pm</t>
-  </si>
-  <si>
-    <t>15-03-2018 4:33 am</t>
-  </si>
-  <si>
-    <t>15-03-2018 9:20 pm</t>
-  </si>
-  <si>
-    <t>16-03-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>16-03-2018 9:34 pm</t>
-  </si>
-  <si>
-    <t>17-03-2018 5:57 am</t>
-  </si>
-  <si>
-    <t>17-03-2018 10:02 pm</t>
-  </si>
-  <si>
-    <t>18-03-2018 5:39 am</t>
-  </si>
-  <si>
-    <t>18-03-2018 9:35 pm</t>
-  </si>
-  <si>
-    <t>19-03-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>19-03-2018 10:11 pm</t>
-  </si>
-  <si>
-    <t>20-03-2018 4:26 am</t>
-  </si>
-  <si>
-    <t>20-03-2018 9:45 pm</t>
-  </si>
-  <si>
-    <t>21-03-2018 5:03 am</t>
-  </si>
-  <si>
-    <t>21-03-2018 10:08 pm</t>
-  </si>
-  <si>
-    <t>22-03-2018 4:36 am</t>
-  </si>
-  <si>
-    <t>22-03-2018 10:44 pm</t>
-  </si>
-  <si>
-    <t>23-03-2018 4:54 am</t>
-  </si>
-  <si>
-    <t>24-03-2018 9:16 pm</t>
-  </si>
-  <si>
-    <t>25-03-2018 6:20 am</t>
-  </si>
-  <si>
-    <t>25-03-2018 10:59 pm</t>
-  </si>
-  <si>
-    <t>26-03-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>27-03-2018 10:18 pm</t>
-  </si>
-  <si>
-    <t>28-03-2018 4:44 am</t>
-  </si>
-  <si>
-    <t>28-03-2018 10:30 pm</t>
-  </si>
-  <si>
-    <t>29-03-2018 4:47 am</t>
-  </si>
-  <si>
-    <t>29-03-2018 10:49 pm</t>
-  </si>
-  <si>
-    <t>30-03-2018 5:05 am</t>
-  </si>
-  <si>
-    <t>30-03-2018 9:56 pm</t>
-  </si>
-  <si>
-    <t>31-03-2018 5:23 am</t>
-  </si>
-  <si>
-    <t>31-03-2018 10:21 pm</t>
-  </si>
-  <si>
-    <t>01-04-2018 5:03 am</t>
-  </si>
-  <si>
-    <t>01-04-2018 10:00 pm</t>
-  </si>
-  <si>
-    <t>02-04-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>02-04-2018 9:51 pm</t>
-  </si>
-  <si>
-    <t>03-04-2018 4:13 am</t>
-  </si>
-  <si>
-    <t>04-04-2018 11:01 pm</t>
-  </si>
-  <si>
-    <t>05-04-2018 3:13 am</t>
-  </si>
-  <si>
-    <t>05-04-2018 10:12 pm</t>
-  </si>
-  <si>
-    <t>06-04-2018 4:39 am</t>
-  </si>
-  <si>
-    <t>06-04-2018 9:49 pm</t>
-  </si>
-  <si>
-    <t>07-04-2018 5:14 am</t>
-  </si>
-  <si>
-    <t>08-04-2018 12:28 am</t>
-  </si>
-  <si>
-    <t>08-04-2018 6:27 am</t>
-  </si>
-  <si>
-    <t>08-04-2018 9:43 pm</t>
-  </si>
-  <si>
-    <t>09-04-2018 5:03 am</t>
-  </si>
-  <si>
-    <t>09-04-2018 10:32 pm</t>
-  </si>
-  <si>
-    <t>10-04-2018 4:45 am</t>
-  </si>
-  <si>
-    <t>10-04-2018 10:46 pm</t>
-  </si>
-  <si>
-    <t>11-04-2018 5:03 am</t>
-  </si>
-  <si>
-    <t>11-04-2018 10:25 pm</t>
-  </si>
-  <si>
-    <t>12-04-2018 5:30 am</t>
-  </si>
-  <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>12-04-2018 10:41 pm</t>
-  </si>
-  <si>
-    <t>13-04-2018 5:10 am</t>
-  </si>
-  <si>
-    <t>13-04-2018 10:11 pm</t>
-  </si>
-  <si>
-    <t>14-04-2018 3:48 am</t>
-  </si>
-  <si>
-    <t>14-04-2018 11:07 pm</t>
-  </si>
-  <si>
-    <t>15-04-2018 5:22 am</t>
-  </si>
-  <si>
-    <t>15-04-2018 10:20 pm</t>
-  </si>
-  <si>
-    <t>16-04-2018 4:42 am</t>
-  </si>
-  <si>
-    <t>16-04-2018 10:48 pm</t>
-  </si>
-  <si>
-    <t>17-04-2018 4:57 am</t>
-  </si>
-  <si>
-    <t>17-04-2018 10:39 pm</t>
-  </si>
-  <si>
-    <t>18-04-2018 4:58 am</t>
-  </si>
-  <si>
-    <t>18-04-2018 9:45 pm</t>
-  </si>
-  <si>
-    <t>19-04-2018 4:55 am</t>
-  </si>
-  <si>
-    <t>19-04-2018 9:41 pm</t>
-  </si>
-  <si>
-    <t>20-04-2018 4:48 am</t>
-  </si>
-  <si>
-    <t>20-04-2018 10:00 pm</t>
-  </si>
-  <si>
-    <t>21-04-2018 6:29 am</t>
-  </si>
-  <si>
-    <t>21-04-2018 9:12 pm</t>
-  </si>
-  <si>
-    <t>22-04-2018 5:01 am</t>
-  </si>
-  <si>
-    <t>22-04-2018 9:53 pm</t>
-  </si>
-  <si>
-    <t>23-04-2018 5:06 am</t>
-  </si>
-  <si>
-    <t>23-04-2018 11:58 pm</t>
-  </si>
-  <si>
-    <t>24-04-2018 5:00 am</t>
-  </si>
-  <si>
-    <t>24-04-2018 9:35 pm</t>
-  </si>
-  <si>
-    <t>25-04-2018 6:52 am</t>
-  </si>
-  <si>
-    <t>25-04-2018 9:58 pm</t>
-  </si>
-  <si>
-    <t>26-04-2018 5:02 am</t>
-  </si>
-  <si>
-    <t>26-04-2018 10:13 pm</t>
-  </si>
-  <si>
-    <t>27-04-2018 5:05 am</t>
-  </si>
-  <si>
-    <t>27-04-2018 11:14 pm</t>
-  </si>
-  <si>
-    <t>28-04-2018 5:25 am</t>
-  </si>
-  <si>
-    <t>28-04-2018 10:14 pm</t>
-  </si>
-  <si>
-    <t>29-04-2018 6:05 am</t>
-  </si>
-  <si>
-    <t>29-04-2018 9:42 pm</t>
-  </si>
-  <si>
-    <t>30-04-2018 4:39 am</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1063,7 +568,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1071,6 +576,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1430,14 +937,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P182" sqref="P182:P211"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" style="7" customWidth="1"/>
     <col min="3" max="4" width="13.7265625" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.54296875" style="3" bestFit="1" customWidth="1"/>
@@ -1453,10 +960,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -1503,10 +1010,10 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="7">
         <v>42978.90625</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="7">
         <v>42979.160416666666</v>
       </c>
       <c r="C2" s="3">
@@ -1560,10 +1067,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3" s="7">
         <v>42979.934027777781</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="7">
         <v>42980.24722222222</v>
       </c>
       <c r="C3" s="3">
@@ -1617,10 +1124,10 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4" s="7">
         <v>42980.885416666664</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="7">
         <v>42981.229166666664</v>
       </c>
       <c r="C4" s="3">
@@ -1674,10 +1181,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="A5" s="7">
         <v>42981.923611111109</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="7">
         <v>42982.206944444442</v>
       </c>
       <c r="C5" s="3">
@@ -1731,10 +1238,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="A6" s="7">
         <v>42983.918749999997</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="7">
         <v>42984.209027777775</v>
       </c>
       <c r="C6" s="3">
@@ -1788,10 +1295,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="A7" s="7">
         <v>42984.924305555556</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="7">
         <v>42985.206250000003</v>
       </c>
       <c r="C7" s="3">
@@ -1845,10 +1352,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="A8" s="7">
         <v>42985.90347222222</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="7">
         <v>42986.214583333334</v>
       </c>
       <c r="C8" s="3">
@@ -1902,10 +1409,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="A9" s="7">
         <v>42986.927083333336</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="7">
         <v>42987.25277777778</v>
       </c>
       <c r="C9" s="3">
@@ -1959,10 +1466,10 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+      <c r="A10" s="7">
         <v>42987.913194444445</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="7">
         <v>42988.243055555555</v>
       </c>
       <c r="C10" s="3">
@@ -2016,10 +1523,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="A11" s="7">
         <v>42988.904861111114</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="7">
         <v>42989.213194444441</v>
       </c>
       <c r="C11" s="3">
@@ -2073,10 +1580,10 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+      <c r="A12" s="7">
         <v>42989.913194444445</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="7">
         <v>42990.189583333333</v>
       </c>
       <c r="C12" s="3">
@@ -2130,10 +1637,10 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+      <c r="A13" s="7">
         <v>42990.908333333333</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="7">
         <v>42991.210416666669</v>
       </c>
       <c r="C13" s="3">
@@ -2187,10 +1694,10 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="A14" s="7">
         <v>42991.886805555558</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="7">
         <v>42992.209027777775</v>
       </c>
       <c r="C14" s="3">
@@ -2244,10 +1751,10 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="A15" s="7">
         <v>42992.911111111112</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="7">
         <v>42993.225694444445</v>
       </c>
       <c r="C15" s="3">
@@ -2301,10 +1808,10 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
+      <c r="A16" s="7">
         <v>42993.916666666664</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="7">
         <v>42994.245138888888</v>
       </c>
       <c r="C16" s="3">
@@ -2358,10 +1865,10 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
+      <c r="A17" s="7">
         <v>42995.93472222222</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="7">
         <v>42996.213194444441</v>
       </c>
       <c r="C17" s="3">
@@ -2415,10 +1922,10 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+      <c r="A18" s="7">
         <v>42996.907638888886</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="7">
         <v>42997.224999999999</v>
       </c>
       <c r="C18" s="3">
@@ -2472,10 +1979,10 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+      <c r="A19" s="7">
         <v>42997.923611111109</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="7">
         <v>42998.178472222222</v>
       </c>
       <c r="C19" s="3">
@@ -2529,10 +2036,10 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
+      <c r="A20" s="7">
         <v>42998.89166666667</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="7">
         <v>42999.216666666667</v>
       </c>
       <c r="C20" s="3">
@@ -2586,10 +2093,10 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+      <c r="A21" s="7">
         <v>42999.925000000003</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="7">
         <v>43000.214583333334</v>
       </c>
       <c r="C21" s="3">
@@ -2643,10 +2150,10 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
+      <c r="A22" s="7">
         <v>43001.917361111111</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="7">
         <v>43002.219444444447</v>
       </c>
       <c r="C22" s="3">
@@ -2700,10 +2207,10 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
+      <c r="A23" s="7">
         <v>43002.897222222222</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="7">
         <v>43003.213194444441</v>
       </c>
       <c r="C23" s="3">
@@ -2757,10 +2264,10 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
+      <c r="A24" s="7">
         <v>43003.912499999999</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="7">
         <v>43004.208333333336</v>
       </c>
       <c r="C24" s="3">
@@ -2814,10 +2321,10 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
+      <c r="A25" s="7">
         <v>43007.95</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="7">
         <v>43008.181944444441</v>
       </c>
       <c r="C25" s="3">
@@ -2871,10 +2378,10 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
+      <c r="A26" s="7">
         <v>43008.804166666669</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="7">
         <v>43009.151388888888</v>
       </c>
       <c r="C26" s="3">
@@ -2928,10 +2435,10 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+      <c r="A27" s="7">
         <v>43009.946527777778</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="7">
         <v>43010.095138888886</v>
       </c>
       <c r="C27" s="3">
@@ -2985,10 +2492,10 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
+      <c r="A28" s="7">
         <v>43010.873611111114</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="7">
         <v>43011.174305555556</v>
       </c>
       <c r="C28" s="3">
@@ -3042,10 +2549,10 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
+      <c r="A29" s="7">
         <v>43011.977083333331</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="7">
         <v>43012.207638888889</v>
       </c>
       <c r="C29" s="3">
@@ -3099,10 +2606,10 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
+      <c r="A30" s="7">
         <v>43012.964583333334</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="7">
         <v>43013.207638888889</v>
       </c>
       <c r="C30" s="3">
@@ -3156,10 +2663,10 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
+      <c r="A31" s="7">
         <v>43013.972916666666</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="7">
         <v>43014.206944444442</v>
       </c>
       <c r="C31" s="3">
@@ -3213,10 +2720,10 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
+      <c r="A32" s="7">
         <v>43014.945138888892</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="7">
         <v>43015.256249999999</v>
       </c>
       <c r="C32" s="3">
@@ -3270,10 +2777,10 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
+      <c r="A33" s="7">
         <v>43016.902083333334</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="7">
         <v>43017.210416666669</v>
       </c>
       <c r="C33" s="3">
@@ -3327,10 +2834,10 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
+      <c r="A34" s="7">
         <v>43018.925694444442</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="7">
         <v>43019.172222222223</v>
       </c>
       <c r="C34" s="3">
@@ -3384,10 +2891,10 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
+      <c r="A35" s="7">
         <v>43020.895833333336</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="7">
         <v>43021.156944444447</v>
       </c>
       <c r="C35" s="3">
@@ -3441,10 +2948,10 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
+      <c r="A36" s="7">
         <v>43021.958333333336</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="7">
         <v>43022.189583333333</v>
       </c>
       <c r="C36" s="3">
@@ -3498,10 +3005,10 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
+      <c r="A37" s="7">
         <v>43024.885416666664</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="7">
         <v>43025.206944444442</v>
       </c>
       <c r="C37" s="3">
@@ -3555,10 +3062,10 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
+      <c r="A38" s="7">
         <v>43028.956250000003</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="7">
         <v>43029.200694444444</v>
       </c>
       <c r="C38" s="3">
@@ -3612,10 +3119,10 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
+      <c r="A39" s="7">
         <v>43029.945833333331</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="7">
         <v>43030.237500000003</v>
       </c>
       <c r="C39" s="3">
@@ -3669,10 +3176,10 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
+      <c r="A40" s="7">
         <v>43030.916666666664</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="7">
         <v>43031.213194444441</v>
       </c>
       <c r="C40" s="3">
@@ -3726,10 +3233,10 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
+      <c r="A41" s="7">
         <v>43031.956944444442</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="7">
         <v>43032.193055555559</v>
       </c>
       <c r="C41" s="3">
@@ -3783,10 +3290,10 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
+      <c r="A42" s="7">
         <v>43032.950694444444</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="7">
         <v>43033.215277777781</v>
       </c>
       <c r="C42" s="3">
@@ -3840,10 +3347,10 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
+      <c r="A43" s="7">
         <v>43033.934027777781</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="7">
         <v>43034.247916666667</v>
       </c>
       <c r="C43" s="3">
@@ -3897,10 +3404,10 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
+      <c r="A44" s="7">
         <v>43035.000694444447</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="7">
         <v>43035.299305555556</v>
       </c>
       <c r="C44" s="3">
@@ -3954,10 +3461,10 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
+      <c r="A45" s="7">
         <v>43035.934027777781</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="7">
         <v>43036.131944444445</v>
       </c>
       <c r="C45" s="3">
@@ -4011,10 +3518,10 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
+      <c r="A46" s="7">
         <v>43036.951388888891</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="7">
         <v>43037.21597222222</v>
       </c>
       <c r="C46" s="3">
@@ -4068,10 +3575,10 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
+      <c r="A47" s="7">
         <v>43037.926388888889</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="7">
         <v>43038.218055555553</v>
       </c>
       <c r="C47" s="3">
@@ -4125,10 +3632,10 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
+      <c r="A48" s="7">
         <v>43038.94027777778</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="7">
         <v>43039.207638888889</v>
       </c>
       <c r="C48" s="3">
@@ -4182,10 +3689,10 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
+      <c r="A49" s="7">
         <v>43039.945138888892</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="7">
         <v>43040.272916666669</v>
       </c>
       <c r="C49" s="3">
@@ -4239,10 +3746,10 @@
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
+      <c r="A50" s="7">
         <v>43041.017361111109</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="7">
         <v>43041.165972222225</v>
       </c>
       <c r="C50" s="3">
@@ -4296,10 +3803,10 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
+      <c r="A51" s="7">
         <v>43041.948611111111</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="7">
         <v>43042.263194444444</v>
       </c>
       <c r="C51" s="3">
@@ -4353,10 +3860,10 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A52" s="1">
+      <c r="A52" s="7">
         <v>43043.929166666669</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="7">
         <v>43044.247916666667</v>
       </c>
       <c r="C52" s="3">
@@ -4410,10 +3917,10 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A53" s="1">
+      <c r="A53" s="7">
         <v>43044.911111111112</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="7">
         <v>43045.118055555555</v>
       </c>
       <c r="C53" s="3">
@@ -4467,10 +3974,10 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A54" s="1">
+      <c r="A54" s="7">
         <v>43045.93472222222</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="7">
         <v>43046.291666666664</v>
       </c>
       <c r="C54" s="3">
@@ -4524,10 +4031,10 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A55" s="1">
+      <c r="A55" s="7">
         <v>43046.921527777777</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="7">
         <v>43047.211805555555</v>
       </c>
       <c r="C55" s="3">
@@ -4581,10 +4088,10 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A56" s="1">
+      <c r="A56" s="7">
         <v>43047.896527777775</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="7">
         <v>43048.164583333331</v>
       </c>
       <c r="C56" s="3">
@@ -4638,10 +4145,10 @@
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A57" s="1">
+      <c r="A57" s="7">
         <v>43048.927083333336</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="7">
         <v>43049.208333333336</v>
       </c>
       <c r="C57" s="3">
@@ -4695,10 +4202,10 @@
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A58" s="1">
+      <c r="A58" s="7">
         <v>43049.932638888888</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="7">
         <v>43050.260416666664</v>
       </c>
       <c r="C58" s="3">
@@ -4752,10 +4259,10 @@
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A59" s="1">
+      <c r="A59" s="7">
         <v>43050.943055555559</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="7">
         <v>43051.283333333333</v>
       </c>
       <c r="C59" s="3">
@@ -4809,10 +4316,10 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A60" s="1">
+      <c r="A60" s="7">
         <v>43051.911805555559</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="7">
         <v>43052.207638888889</v>
       </c>
       <c r="C60" s="3">
@@ -4866,10 +4373,10 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A61" s="1">
+      <c r="A61" s="7">
         <v>43052.925694444442</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="7">
         <v>43053.206944444442</v>
       </c>
       <c r="C61" s="3">
@@ -4923,10 +4430,10 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A62" s="1">
+      <c r="A62" s="7">
         <v>43053.914583333331</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="7">
         <v>43054.186111111114</v>
       </c>
       <c r="C62" s="3">
@@ -4980,10 +4487,10 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A63" s="1">
+      <c r="A63" s="7">
         <v>43055.901388888888</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="7">
         <v>43056.206944444442</v>
       </c>
       <c r="C63" s="3">
@@ -5037,10 +4544,10 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A64" s="1">
+      <c r="A64" s="7">
         <v>43056.92291666667</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="7">
         <v>43057.222916666666</v>
       </c>
       <c r="C64" s="3">
@@ -5094,10 +4601,10 @@
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A65" s="1">
+      <c r="A65" s="7">
         <v>43057.918749999997</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="7">
         <v>43058.20208333333</v>
       </c>
       <c r="C65" s="3">
@@ -5151,10 +4658,10 @@
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A66" s="1">
+      <c r="A66" s="7">
         <v>43058.90625</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="7">
         <v>43059.207638888889</v>
       </c>
       <c r="C66" s="3">
@@ -5208,10 +4715,10 @@
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A67" s="1">
+      <c r="A67" s="7">
         <v>43059.93472222222</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="7">
         <v>43060.20416666667</v>
       </c>
       <c r="C67" s="3">
@@ -5265,10 +4772,10 @@
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A68" s="1">
+      <c r="A68" s="7">
         <v>43060.912499999999</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="7">
         <v>43061.207638888889</v>
       </c>
       <c r="C68" s="3">
@@ -5322,10 +4829,10 @@
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A69" s="1">
+      <c r="A69" s="7">
         <v>43061.926388888889</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="7">
         <v>43062.212500000001</v>
       </c>
       <c r="C69" s="3">
@@ -5379,10 +4886,10 @@
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A70" s="1">
+      <c r="A70" s="7">
         <v>43062.915277777778</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="7">
         <v>43063.208333333336</v>
       </c>
       <c r="C70" s="3">
@@ -5436,10 +4943,10 @@
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A71" s="1">
+      <c r="A71" s="7">
         <v>43063.944444444445</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="7">
         <v>43064.214583333334</v>
       </c>
       <c r="C71" s="3">
@@ -5493,10 +5000,10 @@
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A72" s="1">
+      <c r="A72" s="7">
         <v>43065.009027777778</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="7">
         <v>43065.214583333334</v>
       </c>
       <c r="C72" s="3">
@@ -5550,10 +5057,10 @@
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A73" s="1">
+      <c r="A73" s="7">
         <v>43065.875694444447</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="7">
         <v>43066.229166666664</v>
       </c>
       <c r="C73" s="3">
@@ -5607,10 +5114,10 @@
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A74" s="1">
+      <c r="A74" s="7">
         <v>43066.915277777778</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="7">
         <v>43067.196527777778</v>
       </c>
       <c r="C74" s="3">
@@ -5664,10 +5171,10 @@
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A75" s="1">
+      <c r="A75" s="7">
         <v>43067.929166666669</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="7">
         <v>43068.213194444441</v>
       </c>
       <c r="C75" s="3">
@@ -5721,10 +5228,10 @@
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A76" s="1">
+      <c r="A76" s="7">
         <v>43068.92083333333</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="7">
         <v>43069.24722222222</v>
       </c>
       <c r="C76" s="3">
@@ -5778,10 +5285,10 @@
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A77" s="1">
+      <c r="A77" s="7">
         <v>43070.916666666664</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="7">
         <v>43071.262499999997</v>
       </c>
       <c r="C77" s="3">
@@ -5835,10 +5342,10 @@
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A78" s="1">
+      <c r="A78" s="7">
         <v>43072.926388888889</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="7">
         <v>43073.143055555556</v>
       </c>
       <c r="C78" s="3">
@@ -5892,10 +5399,10 @@
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A79" s="1">
+      <c r="A79" s="7">
         <v>43073.948611111111</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="7">
         <v>43074.214583333334</v>
       </c>
       <c r="C79" s="3">
@@ -5949,10 +5456,10 @@
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A80" s="1">
+      <c r="A80" s="7">
         <v>43074.929861111108</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="7">
         <v>43075.206250000003</v>
       </c>
       <c r="C80" s="3">
@@ -6006,10 +5513,10 @@
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A81" s="1">
+      <c r="A81" s="7">
         <v>43075.898611111108</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="7">
         <v>43076.206944444442</v>
       </c>
       <c r="C81" s="3">
@@ -6063,10 +5570,10 @@
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A82" s="1">
+      <c r="A82" s="7">
         <v>43076.911805555559</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="7">
         <v>43077.206944444442</v>
       </c>
       <c r="C82" s="3">
@@ -6120,10 +5627,10 @@
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A83" s="1">
+      <c r="A83" s="7">
         <v>43077.941666666666</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="7">
         <v>43078.211805555555</v>
       </c>
       <c r="C83" s="3">
@@ -6177,10 +5684,10 @@
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A84" s="1">
+      <c r="A84" s="7">
         <v>43079.943749999999</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="7">
         <v>43080.10833333333</v>
       </c>
       <c r="C84" s="3">
@@ -6234,10 +5741,10 @@
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A85" s="1">
+      <c r="A85" s="7">
         <v>43080.9375</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="7">
         <v>43081.207638888889</v>
       </c>
       <c r="C85" s="3">
@@ -6291,10 +5798,10 @@
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A86" s="1">
+      <c r="A86" s="7">
         <v>43087.9375</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="7">
         <v>43088.209722222222</v>
       </c>
       <c r="C86" s="3">
@@ -6348,10 +5855,10 @@
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A87" s="1">
+      <c r="A87" s="7">
         <v>43088.890972222223</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="7">
         <v>43089.184027777781</v>
       </c>
       <c r="C87" s="3">
@@ -6405,10 +5912,10 @@
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A88" s="1">
+      <c r="A88" s="7">
         <v>43089.907638888886</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="7">
         <v>43090.209027777775</v>
       </c>
       <c r="C88" s="3">
@@ -6462,10 +5969,10 @@
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A89" s="1">
+      <c r="A89" s="7">
         <v>43090.913888888892</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="7">
         <v>43091.214583333334</v>
       </c>
       <c r="C89" s="3">
@@ -6519,10 +6026,10 @@
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A90" s="1">
+      <c r="A90" s="7">
         <v>43091.904861111114</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="7">
         <v>43092.178472222222</v>
       </c>
       <c r="C90" s="3">
@@ -6576,10 +6083,10 @@
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A91" s="1">
+      <c r="A91" s="7">
         <v>43092.886805555558</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="7">
         <v>43093.189583333333</v>
       </c>
       <c r="C91" s="3">
@@ -6633,10 +6140,10 @@
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A92" s="1">
+      <c r="A92" s="7">
         <v>43093.930555555555</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="7">
         <v>43094.197916666664</v>
       </c>
       <c r="C92" s="3">
@@ -6690,10 +6197,10 @@
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A93" s="1">
+      <c r="A93" s="7">
         <v>43094.943055555559</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="7">
         <v>43095.203472222223</v>
       </c>
       <c r="C93" s="3">
@@ -6747,10 +6254,10 @@
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A94" s="1">
+      <c r="A94" s="7">
         <v>43095.911805555559</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="7">
         <v>43096.2</v>
       </c>
       <c r="C94" s="3">
@@ -6804,10 +6311,10 @@
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A95" s="1">
+      <c r="A95" s="7">
         <v>43096.897222222222</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="7">
         <v>43097.206944444442</v>
       </c>
       <c r="C95" s="3">
@@ -6861,10 +6368,10 @@
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A96" s="1">
+      <c r="A96" s="7">
         <v>43097.911805555559</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="7">
         <v>43098.211805555555</v>
       </c>
       <c r="C96" s="3">
@@ -6918,10 +6425,10 @@
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A97" s="1">
+      <c r="A97" s="7">
         <v>43098.905555555553</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="7">
         <v>43099.195138888892</v>
       </c>
       <c r="C97" s="3">
@@ -6975,10 +6482,10 @@
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A98" s="1">
+      <c r="A98" s="7">
         <v>43069.927777777775</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="7">
         <v>43070.243750000001</v>
       </c>
       <c r="C98" s="3">
@@ -7032,10 +6539,10 @@
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A99" s="1">
+      <c r="A99" s="7">
         <v>43099.890972222223</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="7">
         <v>43100.228472222225</v>
       </c>
       <c r="C99" s="3">
@@ -7089,10 +6596,10 @@
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A100" s="1">
+      <c r="A100" s="7">
         <v>43100.888888888891</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="7">
         <v>43101.198611111111</v>
       </c>
       <c r="C100" s="3">
@@ -7146,10 +6653,10 @@
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A101" s="1">
+      <c r="A101" s="7">
         <v>43101.849305555559</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101" s="7">
         <v>43102.069444444445</v>
       </c>
       <c r="C101" s="3">
@@ -7203,10 +6710,10 @@
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A102" s="1">
+      <c r="A102" s="7">
         <v>43102.88958333333</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="7">
         <v>43103.246527777781</v>
       </c>
       <c r="C102" s="3">
@@ -7260,10 +6767,10 @@
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A103" s="1">
+      <c r="A103" s="7">
         <v>43103.861805555556</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="7">
         <v>43104.232638888891</v>
       </c>
       <c r="C103" s="3">
@@ -7317,10 +6824,10 @@
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A104" s="1">
+      <c r="A104" s="7">
         <v>43104.89166666667</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="7">
         <v>43105.102777777778</v>
       </c>
       <c r="C104" s="3">
@@ -7374,10 +6881,10 @@
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A105" s="1">
+      <c r="A105" s="7">
         <v>43105.159722222219</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105" s="7">
         <v>43105.290972222225</v>
       </c>
       <c r="C105" s="3">
@@ -7431,10 +6938,10 @@
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A106" s="1">
+      <c r="A106" s="7">
         <v>43105.990972222222</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="7">
         <v>43106.248611111114</v>
       </c>
       <c r="C106" s="3">
@@ -7488,10 +6995,10 @@
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A107" s="1">
+      <c r="A107" s="7">
         <v>43106.89166666667</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="7">
         <v>43107.254166666666</v>
       </c>
       <c r="C107" s="3">
@@ -7545,10 +7052,10 @@
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A108" s="1">
+      <c r="A108" s="7">
         <v>43107.927777777775</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="7">
         <v>43108.17083333333</v>
       </c>
       <c r="C108" s="3">
@@ -7602,10 +7109,10 @@
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A109" s="1">
+      <c r="A109" s="7">
         <v>43108.881249999999</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="7">
         <v>43109.209027777775</v>
       </c>
       <c r="C109" s="3">
@@ -7659,10 +7166,10 @@
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A110" s="1">
+      <c r="A110" s="7">
         <v>43109.900694444441</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="7">
         <v>43110.206944444442</v>
       </c>
       <c r="C110" s="3">
@@ -7716,10 +7223,10 @@
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A111" s="1">
+      <c r="A111" s="7">
         <v>43110.887499999997</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111" s="7">
         <v>43111.185416666667</v>
       </c>
       <c r="C111" s="3">
@@ -7773,10 +7280,10 @@
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A112" s="1">
+      <c r="A112" s="7">
         <v>43111.897222222222</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112" s="7">
         <v>43112.169444444444</v>
       </c>
       <c r="C112" s="3">
@@ -7830,10 +7337,10 @@
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A113" s="1">
+      <c r="A113" s="7">
         <v>43112.917361111111</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="7">
         <v>43113.275694444441</v>
       </c>
       <c r="C113" s="3">
@@ -7887,10 +7394,10 @@
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A114" s="1">
+      <c r="A114" s="7">
         <v>43113.910416666666</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="7">
         <v>43114.220833333333</v>
       </c>
       <c r="C114" s="3">
@@ -7944,10 +7451,10 @@
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A115" s="1">
+      <c r="A115" s="7">
         <v>43114.881944444445</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="7">
         <v>43115.207638888889</v>
       </c>
       <c r="C115" s="3">
@@ -8001,10 +7508,10 @@
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A116" s="1">
+      <c r="A116" s="7">
         <v>43115.918055555558</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="7">
         <v>43116.263194444444</v>
       </c>
       <c r="C116" s="3">
@@ -8058,10 +7565,10 @@
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A117" s="1">
+      <c r="A117" s="7">
         <v>43116.893750000003</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B117" s="7">
         <v>43117.207638888889</v>
       </c>
       <c r="C117" s="3">
@@ -8115,10 +7622,10 @@
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A118" s="1">
+      <c r="A118" s="7">
         <v>43117.890277777777</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B118" s="7">
         <v>43118.211805555555</v>
       </c>
       <c r="C118" s="3">
@@ -8172,10 +7679,10 @@
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A119" s="1">
+      <c r="A119" s="7">
         <v>43119.897222222222</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B119" s="7">
         <v>43120.26666666667</v>
       </c>
       <c r="C119" s="3">
@@ -8229,10 +7736,10 @@
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A120" s="1">
+      <c r="A120" s="7">
         <v>43120.92291666667</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B120" s="7">
         <v>43121.251388888886</v>
       </c>
       <c r="C120" s="3">
@@ -8286,10 +7793,10 @@
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A121" s="1">
+      <c r="A121" s="7">
         <v>43121.89166666667</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B121" s="7">
         <v>43122.210416666669</v>
       </c>
       <c r="C121" s="3">
@@ -8343,10 +7850,10 @@
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A122" s="1">
+      <c r="A122" s="7">
         <v>43122.900694444441</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="7">
         <v>43123.222916666666</v>
       </c>
       <c r="C122" s="3">
@@ -8400,10 +7907,10 @@
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A123" s="1">
+      <c r="A123" s="7">
         <v>43123.909722222219</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="7">
         <v>43124.254861111112</v>
       </c>
       <c r="C123" s="3">
@@ -8457,10 +7964,10 @@
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A124" s="1">
+      <c r="A124" s="7">
         <v>43124.738194444442</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="7">
         <v>43125.15</v>
       </c>
       <c r="C124" s="3">
@@ -8514,10 +8021,10 @@
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A125" s="1">
+      <c r="A125" s="7">
         <v>43125.880555555559</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B125" s="7">
         <v>43126.218055555553</v>
       </c>
       <c r="C125" s="3">
@@ -8571,10 +8078,10 @@
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A126" s="1">
+      <c r="A126" s="7">
         <v>43126.9375</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B126" s="7">
         <v>43127.179861111108</v>
       </c>
       <c r="C126" s="3">
@@ -8628,10 +8135,10 @@
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A127" s="1">
+      <c r="A127" s="7">
         <v>43127.894444444442</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B127" s="7">
         <v>43128.19027777778</v>
       </c>
       <c r="C127" s="3">
@@ -8685,10 +8192,10 @@
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A128" s="1">
+      <c r="A128" s="7">
         <v>43130.906944444447</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B128" s="7">
         <v>43131.154166666667</v>
       </c>
       <c r="C128" s="3">
@@ -8742,11 +8249,11 @@
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A129" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>17</v>
+      <c r="A129" s="1">
+        <v>43132.911805555559</v>
+      </c>
+      <c r="B129" s="1">
+        <v>43133.195833333331</v>
       </c>
       <c r="C129" s="4">
         <v>353</v>
@@ -8799,11 +8306,11 @@
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A130" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>19</v>
+      <c r="A130" s="7">
+        <v>43133.915972222225</v>
+      </c>
+      <c r="B130" s="7">
+        <v>43134.197222222225</v>
       </c>
       <c r="C130" s="4">
         <v>358</v>
@@ -8856,11 +8363,11 @@
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A131" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>21</v>
+      <c r="A131" s="7">
+        <v>43135.926388888889</v>
+      </c>
+      <c r="B131" s="7">
+        <v>43136.167361111111</v>
       </c>
       <c r="C131" s="4">
         <v>309</v>
@@ -8913,11 +8420,11 @@
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A132" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>23</v>
+      <c r="A132" s="7">
+        <v>43135.020833333336</v>
+      </c>
+      <c r="B132" s="7">
+        <v>43135.252083333333</v>
       </c>
       <c r="C132" s="4">
         <v>299</v>
@@ -8970,11 +8477,11 @@
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A133" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>25</v>
+      <c r="A133" s="7">
+        <v>43136.893750000003</v>
+      </c>
+      <c r="B133" s="7">
+        <v>43137.215277777781</v>
       </c>
       <c r="C133" s="4">
         <v>413</v>
@@ -9027,11 +8534,11 @@
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A134" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>27</v>
+      <c r="A134" s="7">
+        <v>43137.883333333331</v>
+      </c>
+      <c r="B134" s="7">
+        <v>43138.086111111108</v>
       </c>
       <c r="C134" s="4">
         <v>260</v>
@@ -9084,11 +8591,11 @@
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A135" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>29</v>
+      <c r="A135" s="7">
+        <v>43138.880555555559</v>
+      </c>
+      <c r="B135" s="7">
+        <v>43139.114583333336</v>
       </c>
       <c r="C135" s="4">
         <v>309</v>
@@ -9141,11 +8648,11 @@
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A136" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>31</v>
+      <c r="A136" s="7">
+        <v>43139.865972222222</v>
+      </c>
+      <c r="B136" s="7">
+        <v>43140.177777777775</v>
       </c>
       <c r="C136" s="4">
         <v>391</v>
@@ -9198,11 +8705,11 @@
       </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A137" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>33</v>
+      <c r="A137" s="7">
+        <v>43140.908333333333</v>
+      </c>
+      <c r="B137" s="7">
+        <v>43141.241666666669</v>
       </c>
       <c r="C137" s="4">
         <v>431</v>
@@ -9255,11 +8762,11 @@
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A138" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>35</v>
+      <c r="A138" s="7">
+        <v>43141.850694444445</v>
+      </c>
+      <c r="B138" s="7">
+        <v>43142.185416666667</v>
       </c>
       <c r="C138" s="4">
         <v>422</v>
@@ -9312,11 +8819,11 @@
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>37</v>
+      <c r="A139" s="7">
+        <v>43142.893750000003</v>
+      </c>
+      <c r="B139" s="7">
+        <v>43143.162499999999</v>
       </c>
       <c r="C139" s="4">
         <v>356</v>
@@ -9369,11 +8876,11 @@
       </c>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A140" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>39</v>
+      <c r="A140" s="7">
+        <v>43145.884027777778</v>
+      </c>
+      <c r="B140" s="7">
+        <v>43146.206944444442</v>
       </c>
       <c r="C140" s="4">
         <v>426</v>
@@ -9426,11 +8933,11 @@
       </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A141" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>41</v>
+      <c r="A141" s="7">
+        <v>43146.909722222219</v>
+      </c>
+      <c r="B141" s="7">
+        <v>43147.171527777777</v>
       </c>
       <c r="C141" s="4">
         <v>337</v>
@@ -9483,11 +8990,11 @@
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A142" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>43</v>
+      <c r="A142" s="7">
+        <v>43147.929166666669</v>
+      </c>
+      <c r="B142" s="7">
+        <v>43148.217361111114</v>
       </c>
       <c r="C142" s="4">
         <v>379</v>
@@ -9540,11 +9047,11 @@
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A143" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>45</v>
+      <c r="A143" s="7">
+        <v>43148.925000000003</v>
+      </c>
+      <c r="B143" s="7">
+        <v>43149.213888888888</v>
       </c>
       <c r="C143" s="4">
         <v>375</v>
@@ -9597,11 +9104,11 @@
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A144" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>47</v>
+      <c r="A144" s="7">
+        <v>43149.938194444447</v>
+      </c>
+      <c r="B144" s="7">
+        <v>43150.206944444442</v>
       </c>
       <c r="C144" s="4">
         <v>339</v>
@@ -9654,11 +9161,11 @@
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>49</v>
+      <c r="A145" s="7">
+        <v>43150.910416666666</v>
+      </c>
+      <c r="B145" s="7">
+        <v>43151.186111111114</v>
       </c>
       <c r="C145" s="4">
         <v>352</v>
@@ -9711,11 +9218,11 @@
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A146" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>51</v>
+      <c r="A146" s="7">
+        <v>43151.958333333336</v>
+      </c>
+      <c r="B146" s="7">
+        <v>43152.211805555555</v>
       </c>
       <c r="C146" s="4">
         <v>315</v>
@@ -9768,11 +9275,11 @@
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A147" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>53</v>
+      <c r="A147" s="7">
+        <v>43152.947222222225</v>
+      </c>
+      <c r="B147" s="7">
+        <v>43153.206944444442</v>
       </c>
       <c r="C147" s="4">
         <v>323</v>
@@ -9825,11 +9332,11 @@
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A148" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>55</v>
+      <c r="A148" s="7">
+        <v>43153.893750000003</v>
+      </c>
+      <c r="B148" s="7">
+        <v>43154.205555555556</v>
       </c>
       <c r="C148" s="4">
         <v>405</v>
@@ -9882,11 +9389,11 @@
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A149" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>57</v>
+      <c r="A149" s="7">
+        <v>43154.911805555559</v>
+      </c>
+      <c r="B149" s="7">
+        <v>43155.251388888886</v>
       </c>
       <c r="C149" s="4">
         <v>437</v>
@@ -9939,11 +9446,11 @@
       </c>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A150" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>59</v>
+      <c r="A150" s="7">
+        <v>43156.137499999997</v>
+      </c>
+      <c r="B150" s="7">
+        <v>43156.37777777778</v>
       </c>
       <c r="C150" s="4">
         <v>291</v>
@@ -9996,11 +9503,11 @@
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A151" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>61</v>
+      <c r="A151" s="7">
+        <v>43156.913194444445</v>
+      </c>
+      <c r="B151" s="7">
+        <v>43157.211111111108</v>
       </c>
       <c r="C151" s="4">
         <v>371</v>
@@ -10053,11 +9560,11 @@
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A152" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>63</v>
+      <c r="A152" s="7">
+        <v>43157.912499999999</v>
+      </c>
+      <c r="B152" s="7">
+        <v>43158.20208333333</v>
       </c>
       <c r="C152" s="4">
         <v>371</v>
@@ -10110,11 +9617,11 @@
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A153" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>65</v>
+      <c r="A153" s="7">
+        <v>43158.92083333333</v>
+      </c>
+      <c r="B153" s="7">
+        <v>43159.206944444442</v>
       </c>
       <c r="C153" s="4">
         <v>363</v>
@@ -10167,11 +9674,11 @@
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
-        <v>66</v>
-      </c>
-      <c r="B154" t="s">
-        <v>67</v>
+      <c r="A154" s="7">
+        <v>43159.92083333333</v>
+      </c>
+      <c r="B154" s="7">
+        <v>43160.211111111108</v>
       </c>
       <c r="C154" s="4">
         <v>372</v>
@@ -10224,11 +9731,11 @@
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
-        <v>68</v>
-      </c>
-      <c r="B155" t="s">
-        <v>69</v>
+      <c r="A155" s="7">
+        <v>43160.919444444444</v>
+      </c>
+      <c r="B155" s="7">
+        <v>43161.209722222222</v>
       </c>
       <c r="C155" s="4">
         <v>368</v>
@@ -10281,11 +9788,11 @@
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
-        <v>70</v>
-      </c>
-      <c r="B156" t="s">
-        <v>71</v>
+      <c r="A156" s="7">
+        <v>43161.989583333336</v>
+      </c>
+      <c r="B156" s="7">
+        <v>43162.253472222219</v>
       </c>
       <c r="C156" s="4">
         <v>326</v>
@@ -10338,11 +9845,11 @@
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
-        <v>72</v>
-      </c>
-      <c r="B157" t="s">
-        <v>73</v>
+      <c r="A157" s="7">
+        <v>43162.882638888892</v>
+      </c>
+      <c r="B157" s="7">
+        <v>43163.228472222225</v>
       </c>
       <c r="C157" s="4">
         <v>440</v>
@@ -10395,11 +9902,11 @@
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
-        <v>74</v>
-      </c>
-      <c r="B158" t="s">
-        <v>75</v>
+      <c r="A158" s="7">
+        <v>43163.934027777781</v>
+      </c>
+      <c r="B158" s="7">
+        <v>43164.206944444442</v>
       </c>
       <c r="C158" s="4">
         <v>355</v>
@@ -10452,11 +9959,11 @@
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A159" t="s">
-        <v>76</v>
-      </c>
-      <c r="B159" t="s">
-        <v>77</v>
+      <c r="A159" s="7">
+        <v>43164.904861111114</v>
+      </c>
+      <c r="B159" s="7">
+        <v>43165.208333333336</v>
       </c>
       <c r="C159" s="4">
         <v>373</v>
@@ -10509,11 +10016,11 @@
       </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
-        <v>78</v>
-      </c>
-      <c r="B160" t="s">
-        <v>79</v>
+      <c r="A160" s="7">
+        <v>43165.912499999999</v>
+      </c>
+      <c r="B160" s="7">
+        <v>43166.207638888889</v>
       </c>
       <c r="C160" s="4">
         <v>375</v>
@@ -10566,11 +10073,11 @@
       </c>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
-        <v>80</v>
-      </c>
-      <c r="B161" t="s">
-        <v>81</v>
+      <c r="A161" s="7">
+        <v>43166.915972222225</v>
+      </c>
+      <c r="B161" s="7">
+        <v>43167.206944444442</v>
       </c>
       <c r="C161" s="4">
         <v>363</v>
@@ -10623,11 +10130,11 @@
       </c>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
-        <v>82</v>
-      </c>
-      <c r="B162" t="s">
-        <v>83</v>
+      <c r="A162" s="7">
+        <v>43167.908333333333</v>
+      </c>
+      <c r="B162" s="7">
+        <v>43168.207638888889</v>
       </c>
       <c r="C162" s="4">
         <v>396</v>
@@ -10680,11 +10187,11 @@
       </c>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
-        <v>84</v>
-      </c>
-      <c r="B163" t="s">
-        <v>85</v>
+      <c r="A163" s="7">
+        <v>43168.948611111111</v>
+      </c>
+      <c r="B163" s="7">
+        <v>43169.331250000003</v>
       </c>
       <c r="C163" s="4">
         <v>476</v>
@@ -10737,11 +10244,11 @@
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
-        <v>86</v>
-      </c>
-      <c r="B164" t="s">
-        <v>87</v>
+      <c r="A164" s="7">
+        <v>43169.907638888886</v>
+      </c>
+      <c r="B164" s="7">
+        <v>43170.263888888891</v>
       </c>
       <c r="C164" s="4">
         <v>420</v>
@@ -10794,11 +10301,11 @@
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
-        <v>88</v>
-      </c>
-      <c r="B165" t="s">
-        <v>89</v>
+      <c r="A165" s="7">
+        <v>43170.882638888892</v>
+      </c>
+      <c r="B165" s="7">
+        <v>43171.206944444442</v>
       </c>
       <c r="C165" s="4">
         <v>411</v>
@@ -10851,11 +10358,11 @@
       </c>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
-        <v>90</v>
-      </c>
-      <c r="B166" t="s">
-        <v>91</v>
+      <c r="A166" s="7">
+        <v>43171.902777777781</v>
+      </c>
+      <c r="B166" s="7">
+        <v>43172.209027777775</v>
       </c>
       <c r="C166" s="4">
         <v>382</v>
@@ -10908,11 +10415,11 @@
       </c>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
-        <v>92</v>
-      </c>
-      <c r="B167" t="s">
-        <v>93</v>
+      <c r="A167" s="7">
+        <v>43172.921527777777</v>
+      </c>
+      <c r="B167" s="7">
+        <v>43173.211805555555</v>
       </c>
       <c r="C167" s="4">
         <v>365</v>
@@ -10965,11 +10472,11 @@
       </c>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
-        <v>94</v>
-      </c>
-      <c r="B168" t="s">
-        <v>95</v>
+      <c r="A168" s="7">
+        <v>43173.881944444445</v>
+      </c>
+      <c r="B168" s="7">
+        <v>43174.189583333333</v>
       </c>
       <c r="C168" s="4">
         <v>390</v>
@@ -11022,11 +10529,11 @@
       </c>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
-        <v>96</v>
-      </c>
-      <c r="B169" t="s">
-        <v>97</v>
+      <c r="A169" s="7">
+        <v>43174.888888888891</v>
+      </c>
+      <c r="B169" s="7">
+        <v>43175.206944444442</v>
       </c>
       <c r="C169" s="4">
         <v>420</v>
@@ -11079,11 +10586,11 @@
       </c>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
-        <v>98</v>
-      </c>
-      <c r="B170" t="s">
-        <v>99</v>
+      <c r="A170" s="7">
+        <v>43175.898611111108</v>
+      </c>
+      <c r="B170" s="7">
+        <v>43176.247916666667</v>
       </c>
       <c r="C170" s="4">
         <v>436</v>
@@ -11136,11 +10643,11 @@
       </c>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
-        <v>100</v>
-      </c>
-      <c r="B171" t="s">
-        <v>101</v>
+      <c r="A171" s="7">
+        <v>43176.918055555558</v>
+      </c>
+      <c r="B171" s="7">
+        <v>43177.23541666667</v>
       </c>
       <c r="C171" s="4">
         <v>384</v>
@@ -11193,11 +10700,11 @@
       </c>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
-        <v>102</v>
-      </c>
-      <c r="B172" t="s">
-        <v>103</v>
+      <c r="A172" s="7">
+        <v>43177.899305555555</v>
+      </c>
+      <c r="B172" s="7">
+        <v>43178.206944444442</v>
       </c>
       <c r="C172" s="4">
         <v>391</v>
@@ -11250,11 +10757,11 @@
       </c>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
-        <v>104</v>
-      </c>
-      <c r="B173" t="s">
-        <v>105</v>
+      <c r="A173" s="7">
+        <v>43178.924305555556</v>
+      </c>
+      <c r="B173" s="7">
+        <v>43179.18472222222</v>
       </c>
       <c r="C173" s="4">
         <v>325</v>
@@ -11307,11 +10814,11 @@
       </c>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
-        <v>106</v>
-      </c>
-      <c r="B174" t="s">
-        <v>107</v>
+      <c r="A174" s="7">
+        <v>43179.90625</v>
+      </c>
+      <c r="B174" s="7">
+        <v>43180.210416666669</v>
       </c>
       <c r="C174" s="4">
         <v>389</v>
@@ -11364,11 +10871,11 @@
       </c>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
-        <v>108</v>
-      </c>
-      <c r="B175" t="s">
-        <v>109</v>
+      <c r="A175" s="7">
+        <v>43180.922222222223</v>
+      </c>
+      <c r="B175" s="7">
+        <v>43181.191666666666</v>
       </c>
       <c r="C175" s="4">
         <v>349</v>
@@ -11421,11 +10928,11 @@
       </c>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A176" t="s">
-        <v>110</v>
-      </c>
-      <c r="B176" t="s">
-        <v>111</v>
+      <c r="A176" s="7">
+        <v>43181.947222222225</v>
+      </c>
+      <c r="B176" s="7">
+        <v>43182.20416666667</v>
       </c>
       <c r="C176" s="4">
         <v>334</v>
@@ -11478,11 +10985,11 @@
       </c>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
-        <v>112</v>
-      </c>
-      <c r="B177" t="s">
-        <v>113</v>
+      <c r="A177" s="7">
+        <v>43183.886111111111</v>
+      </c>
+      <c r="B177" s="7">
+        <v>43184.263888888891</v>
       </c>
       <c r="C177" s="4">
         <v>491</v>
@@ -11535,11 +11042,11 @@
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A178" t="s">
-        <v>114</v>
-      </c>
-      <c r="B178" t="s">
-        <v>115</v>
+      <c r="A178" s="7">
+        <v>43184.957638888889</v>
+      </c>
+      <c r="B178" s="7">
+        <v>43185.206944444442</v>
       </c>
       <c r="C178" s="4">
         <v>325</v>
@@ -11592,11 +11099,11 @@
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
-        <v>116</v>
-      </c>
-      <c r="B179" t="s">
-        <v>117</v>
+      <c r="A179" s="7">
+        <v>43186.929166666669</v>
+      </c>
+      <c r="B179" s="7">
+        <v>43187.197222222225</v>
       </c>
       <c r="C179" s="4">
         <v>354</v>
@@ -11649,11 +11156,11 @@
       </c>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
-        <v>118</v>
-      </c>
-      <c r="B180" t="s">
-        <v>119</v>
+      <c r="A180" s="7">
+        <v>43187.9375</v>
+      </c>
+      <c r="B180" s="7">
+        <v>43188.199305555558</v>
       </c>
       <c r="C180" s="4">
         <v>327</v>
@@ -11706,11 +11213,11 @@
       </c>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
-        <v>120</v>
-      </c>
-      <c r="B181" t="s">
-        <v>121</v>
+      <c r="A181" s="7">
+        <v>43188.950694444444</v>
+      </c>
+      <c r="B181" s="7">
+        <v>43189.211805555555</v>
       </c>
       <c r="C181" s="4">
         <v>329</v>
@@ -11763,11 +11270,11 @@
       </c>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
-        <v>122</v>
-      </c>
-      <c r="B182" t="s">
-        <v>123</v>
+      <c r="A182" s="7">
+        <v>43189.913888888892</v>
+      </c>
+      <c r="B182" s="7">
+        <v>43190.224305555559</v>
       </c>
       <c r="C182" s="4">
         <v>406</v>
@@ -11820,11 +11327,11 @@
       </c>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A183" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B183" s="5" t="s">
-        <v>125</v>
+      <c r="A183" s="8">
+        <v>43190.931250000001</v>
+      </c>
+      <c r="B183" s="8">
+        <v>43191.210416666669</v>
       </c>
       <c r="C183" s="6">
         <v>355</v>
@@ -11877,11 +11384,11 @@
       </c>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A184" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B184" s="5" t="s">
-        <v>127</v>
+      <c r="A184" s="8">
+        <v>43191.916666666664</v>
+      </c>
+      <c r="B184" s="8">
+        <v>43192.206944444442</v>
       </c>
       <c r="C184" s="6">
         <v>373</v>
@@ -11934,11 +11441,11 @@
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A185" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>129</v>
+      <c r="A185" s="8">
+        <v>43192.910416666666</v>
+      </c>
+      <c r="B185" s="8">
+        <v>43193.175694444442</v>
       </c>
       <c r="C185" s="6">
         <v>322</v>
@@ -11991,11 +11498,11 @@
       </c>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A186" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B186" s="5" t="s">
-        <v>131</v>
+      <c r="A186" s="8">
+        <v>43194.959027777775</v>
+      </c>
+      <c r="B186" s="8">
+        <v>43195.134027777778</v>
       </c>
       <c r="C186" s="6">
         <v>235</v>
@@ -12048,11 +11555,11 @@
       </c>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A187" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B187" s="5" t="s">
-        <v>133</v>
+      <c r="A187" s="8">
+        <v>43195.925000000003</v>
+      </c>
+      <c r="B187" s="8">
+        <v>43196.193749999999</v>
       </c>
       <c r="C187" s="6">
         <v>343</v>
@@ -12105,11 +11612,11 @@
       </c>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A188" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B188" s="5" t="s">
-        <v>135</v>
+      <c r="A188" s="8">
+        <v>43196.90902777778</v>
+      </c>
+      <c r="B188" s="8">
+        <v>43197.218055555553</v>
       </c>
       <c r="C188" s="6">
         <v>398</v>
@@ -12162,11 +11669,11 @@
       </c>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A189" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B189" s="5" t="s">
-        <v>137</v>
+      <c r="A189" s="8">
+        <v>43198.019444444442</v>
+      </c>
+      <c r="B189" s="8">
+        <v>43198.268750000003</v>
       </c>
       <c r="C189" s="6">
         <v>319</v>
@@ -12219,11 +11726,11 @@
       </c>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A190" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B190" s="5" t="s">
-        <v>139</v>
+      <c r="A190" s="8">
+        <v>43198.904861111114</v>
+      </c>
+      <c r="B190" s="8">
+        <v>43199.210416666669</v>
       </c>
       <c r="C190" s="6">
         <v>388</v>
@@ -12276,11 +11783,11 @@
       </c>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A191" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B191" s="5" t="s">
-        <v>141</v>
+      <c r="A191" s="8">
+        <v>43199.938888888886</v>
+      </c>
+      <c r="B191" s="8">
+        <v>43200.197916666664</v>
       </c>
       <c r="C191" s="6">
         <v>333</v>
@@ -12333,11 +11840,11 @@
       </c>
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A192" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B192" s="5" t="s">
-        <v>143</v>
+      <c r="A192" s="8">
+        <v>43200.948611111111</v>
+      </c>
+      <c r="B192" s="8">
+        <v>43201.210416666669</v>
       </c>
       <c r="C192" s="6">
         <v>320</v>
@@ -12390,11 +11897,11 @@
       </c>
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A193" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B193" s="5" t="s">
-        <v>145</v>
+      <c r="A193" s="8">
+        <v>43201.934027777781</v>
+      </c>
+      <c r="B193" s="8">
+        <v>43202.229166666664</v>
       </c>
       <c r="C193" s="6">
         <v>396</v>
@@ -12409,13 +11916,13 @@
         <v>425</v>
       </c>
       <c r="G193" s="5" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="H193" s="5" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="I193" s="5" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="J193" t="str">
         <f t="shared" ref="J193:J211" si="28">IF(C193&gt;=420,"Yes","No")</f>
@@ -12447,11 +11954,11 @@
       </c>
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A194" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B194" s="5" t="s">
-        <v>148</v>
+      <c r="A194" s="8">
+        <v>43202.945138888892</v>
+      </c>
+      <c r="B194" s="8">
+        <v>43203.215277777781</v>
       </c>
       <c r="C194" s="6">
         <v>340</v>
@@ -12504,11 +12011,11 @@
       </c>
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A195" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B195" s="5" t="s">
-        <v>150</v>
+      <c r="A195" s="8">
+        <v>43203.924305555556</v>
+      </c>
+      <c r="B195" s="8">
+        <v>43204.158333333333</v>
       </c>
       <c r="C195" s="6">
         <v>291</v>
@@ -12561,11 +12068,11 @@
       </c>
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A196" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B196" s="5" t="s">
-        <v>152</v>
+      <c r="A196" s="8">
+        <v>43204.963194444441</v>
+      </c>
+      <c r="B196" s="8">
+        <v>43205.223611111112</v>
       </c>
       <c r="C196" s="6">
         <v>342</v>
@@ -12618,11 +12125,11 @@
       </c>
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A197" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B197" s="5" t="s">
-        <v>154</v>
+      <c r="A197" s="8">
+        <v>43205.930555555555</v>
+      </c>
+      <c r="B197" s="8">
+        <v>43206.195833333331</v>
       </c>
       <c r="C197" s="6">
         <v>335</v>
@@ -12675,11 +12182,11 @@
       </c>
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A198" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B198" s="5" t="s">
-        <v>156</v>
+      <c r="A198" s="8">
+        <v>43206.95</v>
+      </c>
+      <c r="B198" s="8">
+        <v>43207.206250000003</v>
       </c>
       <c r="C198" s="6">
         <v>343</v>
@@ -12732,11 +12239,11 @@
       </c>
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A199" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B199" s="5" t="s">
-        <v>158</v>
+      <c r="A199" s="8">
+        <v>43207.943749999999</v>
+      </c>
+      <c r="B199" s="8">
+        <v>43208.206944444442</v>
       </c>
       <c r="C199" s="6">
         <v>340</v>
@@ -12789,11 +12296,11 @@
       </c>
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A200" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B200" s="5" t="s">
-        <v>160</v>
+      <c r="A200" s="8">
+        <v>43208.90625</v>
+      </c>
+      <c r="B200" s="8">
+        <v>43209.204861111109</v>
       </c>
       <c r="C200" s="6">
         <v>391</v>
@@ -12846,11 +12353,11 @@
       </c>
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A201" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B201" s="5" t="s">
-        <v>162</v>
+      <c r="A201" s="8">
+        <v>43209.90347222222</v>
+      </c>
+      <c r="B201" s="8">
+        <v>43210.2</v>
       </c>
       <c r="C201" s="6">
         <v>384</v>
@@ -12903,11 +12410,11 @@
       </c>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A202" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B202" s="5" t="s">
-        <v>164</v>
+      <c r="A202" s="8">
+        <v>43210.916666666664</v>
+      </c>
+      <c r="B202" s="8">
+        <v>43211.270138888889</v>
       </c>
       <c r="C202" s="6">
         <v>425</v>
@@ -12960,11 +12467,11 @@
       </c>
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A203" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B203" s="5" t="s">
-        <v>166</v>
+      <c r="A203" s="8">
+        <v>43211.883333333331</v>
+      </c>
+      <c r="B203" s="8">
+        <v>43212.209027777775</v>
       </c>
       <c r="C203" s="6">
         <v>425</v>
@@ -13017,11 +12524,11 @@
       </c>
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A204" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B204" s="5" t="s">
-        <v>168</v>
+      <c r="A204" s="8">
+        <v>43212.911805555559</v>
+      </c>
+      <c r="B204" s="8">
+        <v>43213.212500000001</v>
       </c>
       <c r="C204" s="6">
         <v>395</v>
@@ -13074,11 +12581,11 @@
       </c>
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A205" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B205" s="5" t="s">
-        <v>170</v>
+      <c r="A205" s="8">
+        <v>43213.998611111114</v>
+      </c>
+      <c r="B205" s="8">
+        <v>43214.208333333336</v>
       </c>
       <c r="C205" s="6">
         <v>276</v>
@@ -13131,11 +12638,11 @@
       </c>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A206" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B206" s="5" t="s">
-        <v>172</v>
+      <c r="A206" s="8">
+        <v>43214.899305555555</v>
+      </c>
+      <c r="B206" s="8">
+        <v>43215.286111111112</v>
       </c>
       <c r="C206" s="6">
         <v>443</v>
@@ -13188,11 +12695,11 @@
       </c>
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A207" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B207" s="5" t="s">
-        <v>174</v>
+      <c r="A207" s="8">
+        <v>43215.915277777778</v>
+      </c>
+      <c r="B207" s="8">
+        <v>43216.209722222222</v>
       </c>
       <c r="C207" s="6">
         <v>385</v>
@@ -13245,11 +12752,11 @@
       </c>
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A208" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B208" s="5" t="s">
-        <v>176</v>
+      <c r="A208" s="8">
+        <v>43216.925694444442</v>
+      </c>
+      <c r="B208" s="8">
+        <v>43217.211805555555</v>
       </c>
       <c r="C208" s="6">
         <v>357</v>
@@ -13302,11 +12809,11 @@
       </c>
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A209" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B209" s="5" t="s">
-        <v>178</v>
+      <c r="A209" s="8">
+        <v>43217.968055555553</v>
+      </c>
+      <c r="B209" s="8">
+        <v>43218.225694444445</v>
       </c>
       <c r="C209" s="6">
         <v>335</v>
@@ -13359,11 +12866,11 @@
       </c>
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A210" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B210" s="5" t="s">
-        <v>180</v>
+      <c r="A210" s="8">
+        <v>43218.926388888889</v>
+      </c>
+      <c r="B210" s="8">
+        <v>43219.253472222219</v>
       </c>
       <c r="C210" s="6">
         <v>423</v>
@@ -13416,11 +12923,11 @@
       </c>
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A211" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B211" s="5" t="s">
-        <v>182</v>
+      <c r="A211" s="8">
+        <v>43219.904166666667</v>
+      </c>
+      <c r="B211" s="8">
+        <v>43220.193749999999</v>
       </c>
       <c r="C211" s="6">
         <v>384</v>

</xml_diff>